<commit_message>
Updated Mission Note sheet to be more representative of what data we actually need
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A539EAB9-B394-5342-A0D7-D8A16DEE8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188F3F4D-8961-4C4E-8848-D186CC95E1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>Deployment Method</t>
   </si>
   <si>
-    <t>Lead Deployer</t>
-  </si>
-  <si>
     <t>Deployment Notes</t>
   </si>
   <si>
@@ -118,21 +115,12 @@
     <t>NO BOARD</t>
   </si>
   <si>
-    <t>Aide</t>
-  </si>
-  <si>
-    <t>Notetaker</t>
-  </si>
-  <si>
     <t>microSWIFTs checked by</t>
   </si>
   <si>
     <t>Data Offloaded and Archived by</t>
   </si>
   <si>
-    <t>Lead Retriever</t>
-  </si>
-  <si>
     <t>Emily Iseley</t>
   </si>
   <si>
@@ -140,6 +128,18 @@
   </si>
   <si>
     <t>This is an example. All data offloaded correctly</t>
+  </si>
+  <si>
+    <t>Deployer 1</t>
+  </si>
+  <si>
+    <t>Deployer2</t>
+  </si>
+  <si>
+    <t>Retriever 1</t>
+  </si>
+  <si>
+    <t>Retriever 2/ Notetaker</t>
   </si>
 </sst>
 </file>
@@ -626,8 +626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,13 +657,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -672,25 +672,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>
@@ -699,31 +699,31 @@
         <v>2</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
@@ -740,46 +740,46 @@
         <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="M2" s="5">
         <v>6</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="P2" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -1981,7 +1981,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2006,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2014,7 +2014,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2022,7 +2022,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2030,7 +2030,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2038,7 +2038,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2046,7 +2046,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +2060,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +2068,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2076,7 +2076,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +2090,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2098,7 +2098,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +2114,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +2122,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +2130,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +2138,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +2146,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +2154,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +2170,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2178,7 +2178,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2186,7 +2186,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2194,7 +2194,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2202,7 +2202,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2210,7 +2210,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2218,7 +2218,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2226,7 +2226,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2234,7 +2234,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2242,7 +2242,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2250,7 +2250,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2258,7 +2258,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2266,7 +2266,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2282,7 +2282,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2290,7 +2290,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2298,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2306,7 +2306,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2314,7 +2314,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2322,7 +2322,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,7 +2344,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2352,7 +2352,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2360,7 +2360,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2368,7 +2368,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2376,7 +2376,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2384,7 +2384,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,7 +2392,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2408,7 +2408,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2416,7 +2416,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2424,7 +2424,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2432,7 +2432,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2440,7 +2440,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2448,7 +2448,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2464,7 +2464,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2472,7 +2472,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2486,7 +2486,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2494,7 +2494,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusted the notes excel sheet to better match the hand written data sheet and then updated the missionReport function to represent this
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188F3F4D-8961-4C4E-8848-D186CC95E1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFBF6A-DF7E-0749-9AE2-9C7161561530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
   <si>
     <t>Mission Number</t>
   </si>
@@ -52,18 +52,6 @@
     <t>Data Offload Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Remaining microSWIFTs to offload </t>
-  </si>
-  <si>
-    <t>microSWIFTs Offloaded</t>
-  </si>
-  <si>
-    <t>Files Offloaded</t>
-  </si>
-  <si>
-    <t>Lab Bench</t>
-  </si>
-  <si>
     <t>EJ Rainville</t>
   </si>
   <si>
@@ -76,9 +64,6 @@
     <t>Forecasted  Peak Direction, Dp [degrees]</t>
   </si>
   <si>
-    <t>Surf Board</t>
-  </si>
-  <si>
     <t>11,21,25,31,32,41</t>
   </si>
   <si>
@@ -91,15 +76,6 @@
     <t>2021-09-21T22:30:00</t>
   </si>
   <si>
-    <t>Minimum Significant Wave Height</t>
-  </si>
-  <si>
-    <t>Maximum Significant Wave Height</t>
-  </si>
-  <si>
-    <t>Average Significant Wave Height</t>
-  </si>
-  <si>
     <t>SSH into each microSWIFT</t>
   </si>
   <si>
@@ -133,13 +109,19 @@
     <t>Deployer 1</t>
   </si>
   <si>
-    <t>Deployer2</t>
-  </si>
-  <si>
     <t>Retriever 1</t>
   </si>
   <si>
     <t>Retriever 2/ Notetaker</t>
+  </si>
+  <si>
+    <t>surf board</t>
+  </si>
+  <si>
+    <t>two-cross shore lines</t>
+  </si>
+  <si>
+    <t>Deployer 2</t>
   </si>
 </sst>
 </file>
@@ -169,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -220,11 +202,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,11 +245,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -269,20 +267,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -624,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,9 +621,7 @@
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.33203125" customWidth="1"/>
-    <col min="13" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="31.33203125" customWidth="1"/>
     <col min="17" max="17" width="27.5" bestFit="1" customWidth="1"/>
@@ -652,18 +634,18 @@
     <col min="24" max="24" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -672,25 +654,25 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>3</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>1</v>
@@ -702,31 +684,13 @@
         <v>6</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -740,55 +704,49 @@
         <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="5">
+        <v>6</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" s="5">
-        <v>6</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -807,14 +765,8 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -833,14 +785,8 @@
       <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -859,14 +805,8 @@
       <c r="P5" s="4"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -885,14 +825,8 @@
       <c r="P6" s="4"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -911,14 +845,8 @@
       <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="4"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -937,14 +865,8 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -963,14 +885,8 @@
       <c r="P9" s="4"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="4"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -989,14 +905,8 @@
       <c r="P10" s="4"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="4"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1015,14 +925,8 @@
       <c r="P11" s="4"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="4"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1041,14 +945,8 @@
       <c r="P12" s="4"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="4"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="1"/>
-      <c r="U12" s="1"/>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1067,14 +965,8 @@
       <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="4"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1093,14 +985,8 @@
       <c r="P14" s="4"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="4"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1119,14 +1005,8 @@
       <c r="P15" s="4"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="4"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1145,14 +1025,8 @@
       <c r="P16" s="4"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="4"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1171,14 +1045,8 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="4"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1197,14 +1065,8 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="4"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1223,14 +1085,8 @@
       <c r="P19" s="4"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="4"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1249,14 +1105,8 @@
       <c r="P20" s="4"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="4"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1275,14 +1125,8 @@
       <c r="P21" s="4"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="4"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1301,14 +1145,8 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="4"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1327,14 +1165,8 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="4"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1353,14 +1185,8 @@
       <c r="P24" s="4"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="4"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1379,14 +1205,8 @@
       <c r="P25" s="4"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="4"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1405,14 +1225,8 @@
       <c r="P26" s="4"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="4"/>
-      <c r="S26" s="1"/>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1"/>
-      <c r="X26" s="1"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1431,14 +1245,8 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="4"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-      <c r="W27" s="1"/>
-      <c r="X27" s="1"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1457,14 +1265,8 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="4"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="X28" s="1"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1483,14 +1285,8 @@
       <c r="P29" s="4"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="4"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1509,14 +1305,8 @@
       <c r="P30" s="4"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="4"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1535,14 +1325,8 @@
       <c r="P31" s="4"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="4"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1561,14 +1345,8 @@
       <c r="P32" s="4"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="4"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1587,14 +1365,8 @@
       <c r="P33" s="4"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="4"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1613,14 +1385,8 @@
       <c r="P34" s="4"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="4"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1639,14 +1405,8 @@
       <c r="P35" s="4"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="4"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1665,14 +1425,8 @@
       <c r="P36" s="4"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="4"/>
-      <c r="S36" s="1"/>
-      <c r="T36" s="1"/>
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-      <c r="W36" s="1"/>
-      <c r="X36" s="1"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1691,14 +1445,8 @@
       <c r="P37" s="4"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="4"/>
-      <c r="S37" s="1"/>
-      <c r="T37" s="1"/>
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1"/>
-      <c r="X37" s="1"/>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1717,14 +1465,8 @@
       <c r="P38" s="4"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="4"/>
-      <c r="S38" s="1"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="X38" s="1"/>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1743,14 +1485,8 @@
       <c r="P39" s="4"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="4"/>
-      <c r="S39" s="1"/>
-      <c r="T39" s="1"/>
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="1"/>
-      <c r="X39" s="1"/>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1769,14 +1505,8 @@
       <c r="P40" s="4"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="4"/>
-      <c r="S40" s="1"/>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-      <c r="W40" s="1"/>
-      <c r="X40" s="1"/>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1795,14 +1525,8 @@
       <c r="P41" s="4"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="4"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-      <c r="W41" s="1"/>
-      <c r="X41" s="1"/>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1821,14 +1545,8 @@
       <c r="P42" s="4"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="4"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-      <c r="W42" s="1"/>
-      <c r="X42" s="1"/>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1847,14 +1565,8 @@
       <c r="P43" s="4"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="4"/>
-      <c r="S43" s="1"/>
-      <c r="T43" s="1"/>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1873,14 +1585,8 @@
       <c r="P44" s="4"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="4"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1899,14 +1605,8 @@
       <c r="P45" s="4"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="4"/>
-      <c r="S45" s="1"/>
-      <c r="T45" s="1"/>
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-      <c r="W45" s="1"/>
-      <c r="X45" s="1"/>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1925,35 +1625,21 @@
       <c r="P46" s="4"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="4"/>
-      <c r="S46" s="1"/>
-      <c r="T46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-      <c r="W46" s="1"/>
-      <c r="X46" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A46 E2:O46">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E46">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="4" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R46">
-    <cfRule type="containsBlanks" dxfId="5" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(P2))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S2:X46">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="1">
-      <formula>LEN(TRIM(S2))&gt;0</formula>
-    </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="3">
-      <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:R46">
@@ -1981,7 +1667,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B1" s="8"/>
     </row>
@@ -1990,7 +1676,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1998,7 +1684,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2006,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2014,7 +1700,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2022,7 +1708,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2030,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2038,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2046,7 +1732,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -2060,7 +1746,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2068,7 +1754,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2076,7 +1762,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2090,7 +1776,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2098,7 +1784,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2106,7 +1792,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -2114,7 +1800,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2122,7 +1808,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2130,7 +1816,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2138,7 +1824,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2146,7 +1832,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2154,7 +1840,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2162,7 +1848,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2170,7 +1856,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2178,7 +1864,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2186,7 +1872,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2194,7 +1880,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2202,7 +1888,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2210,7 +1896,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2218,7 +1904,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2226,7 +1912,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2234,7 +1920,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2242,7 +1928,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2250,7 +1936,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2258,7 +1944,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2266,7 +1952,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2274,7 +1960,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -2282,7 +1968,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2290,7 +1976,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2298,7 +1984,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2306,7 +1992,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2314,7 +2000,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2322,7 +2008,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2330,7 +2016,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2344,7 +2030,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -2352,7 +2038,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -2360,7 +2046,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -2368,7 +2054,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -2376,7 +2062,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -2384,7 +2070,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -2392,7 +2078,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -2400,7 +2086,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -2408,7 +2094,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -2416,7 +2102,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -2424,7 +2110,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -2432,7 +2118,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -2440,7 +2126,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -2448,7 +2134,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,7 +2142,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -2464,7 +2150,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -2472,7 +2158,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -2486,7 +2172,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -2494,7 +2180,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested individual microSwIFT offload script
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCFBF6A-DF7E-0749-9AE2-9C7161561530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B4378B-3B8B-6C4D-99F1-7891B90E8167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -242,11 +242,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +671,7 @@
       <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -1666,10 +1666,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7">

</xml_diff>

<commit_message>
Updated the offload script and notes sheet to have a microSWIFTs retrieved ssection
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B4378B-3B8B-6C4D-99F1-7891B90E8167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570E5994-0E80-3646-9031-4D8E84329560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
   <si>
     <t>Mission Number</t>
   </si>
@@ -122,6 +122,51 @@
   </si>
   <si>
     <t>Deployer 2</t>
+  </si>
+  <si>
+    <t>0.5 - 1</t>
+  </si>
+  <si>
+    <t>E - SE</t>
+  </si>
+  <si>
+    <t>clusters</t>
+  </si>
+  <si>
+    <t>Jim Thomson</t>
+  </si>
+  <si>
+    <t>Alex de Klerk</t>
+  </si>
+  <si>
+    <t>Christine Baker + Sean McGill</t>
+  </si>
+  <si>
+    <t>Total Number of Shepard Buoys Deployed</t>
+  </si>
+  <si>
+    <t>3,4,5,7,8,9,37,38,39,43,44,45</t>
+  </si>
+  <si>
+    <t>microSWIFTs Retrieved</t>
+  </si>
+  <si>
+    <t>3,4,5,8,9</t>
+  </si>
+  <si>
+    <t>Shepherds Retrieved</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>2021-10-04T14:59:24</t>
+  </si>
+  <si>
+    <t>2021-10-04T18:30:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 thenext 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
   </si>
 </sst>
 </file>
@@ -608,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,20 +666,23 @@
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
     <col min="5" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="13" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="31.33203125" customWidth="1"/>
-    <col min="17" max="17" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="26.33203125" customWidth="1"/>
+    <col min="17" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="58.1640625" customWidth="1"/>
+    <col min="20" max="20" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -672,25 +720,34 @@
         <v>13</v>
       </c>
       <c r="M1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -727,46 +784,96 @@
       <c r="L2" s="5">
         <v>6</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="4"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="170" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="4">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4">
+        <v>4</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="4"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -780,13 +887,16 @@
       <c r="K4" s="1"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R4" s="1"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="4"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -800,13 +910,16 @@
       <c r="K5" s="1"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R5" s="1"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -820,13 +933,16 @@
       <c r="K6" s="1"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R6" s="1"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -840,13 +956,16 @@
       <c r="K7" s="1"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="1"/>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R7" s="1"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -860,13 +979,16 @@
       <c r="K8" s="1"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="4"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R8" s="1"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -880,13 +1002,16 @@
       <c r="K9" s="1"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
       <c r="P9" s="4"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="4"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R9" s="1"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -900,13 +1025,16 @@
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="4"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R10" s="1"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -920,13 +1048,16 @@
       <c r="K11" s="1"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R11" s="1"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -940,13 +1071,16 @@
       <c r="K12" s="1"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R12" s="1"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="4"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -960,13 +1094,16 @@
       <c r="K13" s="1"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R13" s="1"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="4"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -980,13 +1117,16 @@
       <c r="K14" s="1"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="4"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R14" s="1"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1000,13 +1140,16 @@
       <c r="K15" s="1"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R15" s="1"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1020,13 +1163,16 @@
       <c r="K16" s="1"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="4"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R16" s="1"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="4"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1040,13 +1186,16 @@
       <c r="K17" s="1"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="4"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R17" s="1"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="4"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1060,13 +1209,16 @@
       <c r="K18" s="1"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="4"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R18" s="1"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="4"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1080,13 +1232,16 @@
       <c r="K19" s="1"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="4"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R19" s="1"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="4"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1100,13 +1255,16 @@
       <c r="K20" s="1"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="4"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R20" s="1"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="4"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1120,13 +1278,16 @@
       <c r="K21" s="1"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
       <c r="P21" s="4"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="4"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R21" s="1"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="4"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1140,13 +1301,16 @@
       <c r="K22" s="1"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="4"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R22" s="1"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="4"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1160,13 +1324,16 @@
       <c r="K23" s="1"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="4"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R23" s="1"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="4"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1180,13 +1347,16 @@
       <c r="K24" s="1"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="4"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R24" s="1"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="4"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1200,13 +1370,16 @@
       <c r="K25" s="1"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
       <c r="P25" s="4"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="4"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R25" s="1"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="4"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1220,13 +1393,16 @@
       <c r="K26" s="1"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
       <c r="P26" s="4"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="4"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R26" s="1"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="4"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1240,13 +1416,16 @@
       <c r="K27" s="1"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
       <c r="P27" s="4"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="4"/>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R27" s="1"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="4"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1260,13 +1439,16 @@
       <c r="K28" s="1"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
       <c r="P28" s="4"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="4"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R28" s="1"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="4"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1280,13 +1462,16 @@
       <c r="K29" s="1"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="4"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R29" s="1"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="4"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1300,13 +1485,16 @@
       <c r="K30" s="1"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
       <c r="P30" s="4"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="4"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R30" s="1"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="4"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1320,13 +1508,16 @@
       <c r="K31" s="1"/>
       <c r="L31" s="4"/>
       <c r="M31" s="4"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="4"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R31" s="1"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="4"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1340,13 +1531,16 @@
       <c r="K32" s="1"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="4"/>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R32" s="1"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="4"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1360,13 +1554,16 @@
       <c r="K33" s="1"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="4"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R33" s="1"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="4"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1380,13 +1577,16 @@
       <c r="K34" s="1"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="4"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R34" s="1"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="4"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1400,13 +1600,16 @@
       <c r="K35" s="1"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
       <c r="P35" s="4"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="4"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R35" s="1"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="4"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1420,13 +1623,16 @@
       <c r="K36" s="1"/>
       <c r="L36" s="4"/>
       <c r="M36" s="4"/>
-      <c r="N36" s="1"/>
-      <c r="O36" s="1"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
       <c r="P36" s="4"/>
       <c r="Q36" s="1"/>
-      <c r="R36" s="4"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R36" s="1"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="4"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1440,13 +1646,16 @@
       <c r="K37" s="1"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
       <c r="P37" s="4"/>
       <c r="Q37" s="1"/>
-      <c r="R37" s="4"/>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R37" s="1"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="4"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1460,13 +1669,16 @@
       <c r="K38" s="1"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
       <c r="P38" s="4"/>
       <c r="Q38" s="1"/>
-      <c r="R38" s="4"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R38" s="1"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="4"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1480,13 +1692,16 @@
       <c r="K39" s="1"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="1"/>
-      <c r="O39" s="1"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="1"/>
-      <c r="R39" s="4"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R39" s="1"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="4"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1500,13 +1715,16 @@
       <c r="K40" s="1"/>
       <c r="L40" s="4"/>
       <c r="M40" s="4"/>
-      <c r="N40" s="1"/>
-      <c r="O40" s="1"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="4"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="4"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R40" s="1"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="4"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1520,13 +1738,16 @@
       <c r="K41" s="1"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="1"/>
-      <c r="R41" s="4"/>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R41" s="1"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="1"/>
+      <c r="U41" s="4"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1540,13 +1761,16 @@
       <c r="K42" s="1"/>
       <c r="L42" s="4"/>
       <c r="M42" s="4"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
       <c r="P42" s="4"/>
       <c r="Q42" s="1"/>
-      <c r="R42" s="4"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R42" s="1"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="4"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1560,13 +1784,16 @@
       <c r="K43" s="1"/>
       <c r="L43" s="4"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="1"/>
-      <c r="R43" s="4"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R43" s="1"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="4"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1580,13 +1807,16 @@
       <c r="K44" s="1"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="1"/>
-      <c r="R44" s="4"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R44" s="1"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="4"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1600,13 +1830,16 @@
       <c r="K45" s="1"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
       <c r="P45" s="4"/>
       <c r="Q45" s="1"/>
-      <c r="R45" s="4"/>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="R45" s="1"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="4"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1622,12 +1855,15 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
-      <c r="P46" s="4"/>
+      <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
-      <c r="R46" s="4"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="1"/>
+      <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A46 E2:O46">
+  <conditionalFormatting sqref="A2:A46 E2:R46">
     <cfRule type="containsBlanks" dxfId="5" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
@@ -1637,12 +1873,12 @@
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:R46">
+  <conditionalFormatting sqref="S2:U46">
     <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(P2))=0</formula>
+      <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:R46">
+  <conditionalFormatting sqref="A2:U46">
     <cfRule type="notContainsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated the mission notes
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570E5994-0E80-3646-9031-4D8E84329560}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A1F55-ED9B-0048-9D1C-33D29D615D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -151,9 +151,6 @@
     <t>microSWIFTs Retrieved</t>
   </si>
   <si>
-    <t>3,4,5,8,9</t>
-  </si>
-  <si>
     <t>Shepherds Retrieved</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 thenext 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
+  </si>
+  <si>
+    <t>3,4,5,38,39</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,7 +729,7 @@
         <v>40</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>1</v>
@@ -856,19 +856,19 @@
         <v>39</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="P3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="4"/>

</xml_diff>

<commit_message>
added offload notes from mission 1
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A1F55-ED9B-0048-9D1C-33D29D615D31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C6F8C2-3CA8-5F42-A46F-F67C52B96869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
   <si>
     <t>Mission Number</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>3,4,5,38,39</t>
+  </si>
+  <si>
+    <t>All data that we have has been offloaded and backed up.</t>
   </si>
 </sst>
 </file>
@@ -656,7 +659,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,8 +873,12 @@
       <c r="S3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="4"/>
+      <c r="T3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>

</xml_diff>

<commit_message>
updates notes to correct some grammar
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C6F8C2-3CA8-5F42-A46F-F67C52B96869}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625B27CA-6411-9D46-83C9-F4E958BF14CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,13 +163,13 @@
     <t>2021-10-04T18:30:00</t>
   </si>
   <si>
-    <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 thenext 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
-  </si>
-  <si>
     <t>3,4,5,38,39</t>
   </si>
   <si>
     <t>All data that we have has been offloaded and backed up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 the next 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
   </si>
 </sst>
 </file>
@@ -658,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,7 +859,7 @@
         <v>39</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>42</v>
@@ -871,13 +871,13 @@
         <v>44</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added mission 2 notes
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625B27CA-6411-9D46-83C9-F4E958BF14CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41423E59-7A65-CC43-9E52-36D90E636E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
   <si>
     <t>Mission Number</t>
   </si>
@@ -163,13 +163,45 @@
     <t>2021-10-04T18:30:00</t>
   </si>
   <si>
+    <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 thenext 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
+  </si>
+  <si>
     <t>3,4,5,38,39</t>
   </si>
   <si>
     <t>All data that we have has been offloaded and backed up.</t>
   </si>
   <si>
-    <t xml:space="preserve">At 14:46 the first 8 were deployed which consisted of two sets of four initially move offshore. Then at 14:59 the next 8 were deployed in two sets of four closer onshore. At 15:17 recovered the second deployment set on north side of pier. At 15:28 redeployed the second set further south and onshore. At 15:50 Recovered second set and redployed in the breaking zone at 16:00. At 16:20 the first set continued to track north and offshore, approximately 0.6 km offshore. Finally at 17:54 we paddled very far offshore and recovered five microSWIFTs and two shepherds from the second set. </t>
+    <t>clusters and people watching them to make sure they don't drift too far.</t>
+  </si>
+  <si>
+    <t>Sean McGill</t>
+  </si>
+  <si>
+    <t>Christine Baker</t>
+  </si>
+  <si>
+    <t>3,4,5,6,10,39</t>
+  </si>
+  <si>
+    <t>2021-10-05T14:30:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T16:00:00</t>
+  </si>
+  <si>
+    <t>8:53 - 003 isntgetting gps signal and 006 is not able to initaize the modem
+9:00 - 003 has gotten gps signal and 006 has initialized modem after a reboot
+10:30 - micros deployed with a strong northerly alongshore current
+10:38 - Chirstine reports feeling current reversals while swimming in bar trough
+10:45 - micros are reset close to the original location
+11:00 - All micros Retreived from first deployment but etner surf zone and exited during send window
+11:10 - All mcros headed back out in same array
+11:17 - All micros enter the whitewater
+11:25 - All micros are retrieved
+11:35 - All micros headed back out 
+11:40 - All micros in water
+11:55 - All micros retrieved</t>
   </si>
 </sst>
 </file>
@@ -267,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -295,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -658,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,13 +703,15 @@
     <col min="2" max="2" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="61.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="24.6640625" customWidth="1"/>
     <col min="11" max="12" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="35.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="26.33203125" customWidth="1"/>
     <col min="17" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="58.1640625" customWidth="1"/>
+    <col min="19" max="19" width="91.1640625" customWidth="1"/>
     <col min="20" max="20" width="27.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="30.5" bestFit="1" customWidth="1"/>
@@ -859,7 +896,7 @@
         <v>39</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>42</v>
@@ -871,35 +908,73 @@
         <v>44</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="4"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="204" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="4">
+        <v>6</v>
+      </c>
+      <c r="M4" s="4">
+        <v>2</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>54</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="4"/>
     </row>

</xml_diff>

<commit_message>
updated mission 2 notes for grammar
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41423E59-7A65-CC43-9E52-36D90E636E95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F5D0B-3DD3-1740-B008-7B7010C7FB82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
   <si>
     <t>Mission Number</t>
   </si>
@@ -172,9 +172,6 @@
     <t>All data that we have has been offloaded and backed up.</t>
   </si>
   <si>
-    <t>clusters and people watching them to make sure they don't drift too far.</t>
-  </si>
-  <si>
     <t>Sean McGill</t>
   </si>
   <si>
@@ -190,7 +187,10 @@
     <t>2021-10-05T16:00:00</t>
   </si>
   <si>
-    <t>8:53 - 003 isntgetting gps signal and 006 is not able to initaize the modem
+    <t>clusters and people watched them to make sure they don't drift too far</t>
+  </si>
+  <si>
+    <t>8:53 - 003 isn't getting gps signal and 006 is not able to initaize the modem
 9:00 - 003 has gotten gps signal and 006 has initialized modem after a reboot
 10:30 - micros deployed with a strong northerly alongshore current
 10:38 - Chirstine reports feeling current reversals while swimming in bar trough
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -934,16 +934,16 @@
         <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>8</v>
@@ -958,25 +958,29 @@
         <v>2</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="4"/>
+      <c r="T4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
updated notes with mission 3, 4, and 5
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F5D0B-3DD3-1740-B008-7B7010C7FB82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEB6B66-0A6D-154F-A7E4-1BC3C3F56C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="66">
   <si>
     <t>Mission Number</t>
   </si>
@@ -202,6 +202,41 @@
 11:35 - All micros headed back out 
 11:40 - All micros in water
 11:55 - All micros retrieved</t>
+  </si>
+  <si>
+    <t>small grid (3x3)</t>
+  </si>
+  <si>
+    <t>2021-10-05T17:10:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T17:38:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T18:06:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T18:25:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T18:35:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T18:48:00</t>
+  </si>
+  <si>
+    <t>All microSWIFTs were retrieved
+- We needed to play goalie at the pier since the micros were headed north quickly - this was effective for getting them all back
+- this mission was right at low tide</t>
+  </si>
+  <si>
+    <t>This mission was just after low tide and there was a light onshore breeze</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This mission was very short </t>
+  </si>
+  <si>
+    <t>3,4,5,40,41,42,39,38,57</t>
   </si>
 </sst>
 </file>
@@ -339,6 +374,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
@@ -350,20 +399,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -693,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -711,7 +746,7 @@
     <col min="14" max="14" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="26.33203125" customWidth="1"/>
     <col min="17" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="91.1640625" customWidth="1"/>
+    <col min="19" max="19" width="108.83203125" customWidth="1"/>
     <col min="20" max="20" width="27.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="30.5" bestFit="1" customWidth="1"/>
@@ -982,72 +1017,186 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="4"/>
+    <row r="5" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="4">
+        <v>9</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="T5" s="1"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="4"/>
+    <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9</v>
+      </c>
+      <c r="M6" s="4">
+        <v>2</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="T6" s="1"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="4"/>
+    <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="4">
+        <v>9</v>
+      </c>
+      <c r="M7" s="4">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="T7" s="1"/>
       <c r="U7" s="4"/>
     </row>
@@ -1950,22 +2099,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A46 E2:R46">
-    <cfRule type="containsBlanks" dxfId="5" priority="8">
+    <cfRule type="containsBlanks" dxfId="1" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:E46">
-    <cfRule type="containsBlanks" dxfId="4" priority="7">
+    <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:U46">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2510,10 +2659,10 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated notes and mission netcdf script
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634C2D79-72D8-7741-8075-2C1A8290359E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B272C916-0BAD-DD48-A022-E012A58F3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="68">
   <si>
     <t>Mission Number</t>
   </si>
@@ -207,13 +207,7 @@
     <t>2021-10-05T18:06:00</t>
   </si>
   <si>
-    <t>2021-10-05T18:25:00</t>
-  </si>
-  <si>
     <t>2021-10-05T18:35:00</t>
-  </si>
-  <si>
-    <t>2021-10-05T18:48:00</t>
   </si>
   <si>
     <t>All microSWIFTs were retrieved
@@ -245,7 +239,10 @@
     <t xml:space="preserve">NOTE: This was not a separate mission from mission 1. These were the microSWIFTs that were lost from the first mission and recovered by boat the following day on 10/5. </t>
   </si>
   <si>
-    <t>2021-10-05T17:50:00</t>
+    <t>2021-10-05T17:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-05T18:50:00</t>
   </si>
 </sst>
 </file>
@@ -369,11 +366,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -723,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,7 +923,7 @@
         <v>39</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="P3" s="5" t="s">
         <v>42</v>
@@ -938,7 +935,7 @@
         <v>44</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>8</v>
@@ -1002,7 +999,7 @@
       <c r="R4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="S4" s="9" t="s">
         <v>52</v>
       </c>
       <c r="T4" s="1" t="s">
@@ -1053,10 +1050,10 @@
         <v>2</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P5" s="4" t="s">
         <v>42</v>
@@ -1065,10 +1062,10 @@
         <v>54</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="4"/>
@@ -1114,10 +1111,10 @@
         <v>2</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P6" s="4" t="s">
         <v>42</v>
@@ -1129,7 +1126,7 @@
         <v>56</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="4"/>
@@ -1175,22 +1172,22 @@
         <v>2</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="4"/>
@@ -1236,10 +1233,10 @@
         <v>0</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P8" s="5">
         <v>0</v>
@@ -1248,10 +1245,10 @@
         <v>43</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="T8" s="1"/>
       <c r="U8" s="4"/>
@@ -2160,10 +2157,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7">

</xml_diff>

<commit_message>
added mission 7 to the notes sheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B272C916-0BAD-DD48-A022-E012A58F3C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AF875-BFE2-1C48-9E49-1E77A2E373D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
   <si>
     <t>Mission Number</t>
   </si>
@@ -243,6 +243,41 @@
   </si>
   <si>
     <t>2021-10-05T18:50:00</t>
+  </si>
+  <si>
+    <t>helicopter</t>
+  </si>
+  <si>
+    <t>alongshore line</t>
+  </si>
+  <si>
+    <t>4,5,37,38,39,40,41,57</t>
+  </si>
+  <si>
+    <t>2021-10-06T14:55:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All parachutes deploye correctly
+All times when plotting seem to be an hour ahead of our hnd written notes - for now adjsting that value in this document for start and end times and it s shifted forward and hour from what was written down. 
+Accidentally deplyed a microSWIFT on the north end just after the spotter buoy rather than a shepherd buoy. </t>
+  </si>
+  <si>
+    <t>2021-10-06T18:00:00</t>
+  </si>
+  <si>
+    <t>microSWIFT number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is it recording data? </t>
+  </si>
+  <si>
+    <t>Is it sending telemetry?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Do we have this microSWIFT? (Valiant Effort and lost)</t>
   </si>
 </sst>
 </file>
@@ -340,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -369,14 +404,77 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -405,6 +503,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -720,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,26 +1361,64 @@
       <c r="T8" s="1"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="4"/>
+    <row r="9" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D9" s="1">
+        <v>78</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="4">
+        <v>8</v>
+      </c>
+      <c r="M9" s="4">
+        <v>2</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="T9" s="1"/>
       <c r="U9" s="4"/>
     </row>
@@ -2129,12 +2275,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="containsBlanks" dxfId="3" priority="8">
+    <cfRule type="containsBlanks" dxfId="9" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2144,546 +2290,1162 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
-  <dimension ref="A1:B66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D68" sqref="C68:D68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="10"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>10</v>
       </c>
       <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>14</v>
       </c>
       <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C35" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C38" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C40" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C41" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C42" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C44" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C45" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>46</v>
       </c>
       <c r="B46" s="6"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C48" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C49" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C51" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C52" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C53" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C54" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C55" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C56" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C57" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C58" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C59" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C60" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C61" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C62" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C63" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>64</v>
       </c>
       <c r="B64" s="6"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C64" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C65" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="C66" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="0" priority="2">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:E66">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C66">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:E66">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated spreadsheet with working micros
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AF875-BFE2-1C48-9E49-1E77A2E373D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0292F5-EF9A-354B-9489-92A11D016F6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="81">
   <si>
     <t>Mission Number</t>
   </si>
@@ -278,6 +278,12 @@
   </si>
   <si>
     <t>Do we have this microSWIFT? (Valiant Effort and lost)</t>
+  </si>
+  <si>
+    <t>Git Branch</t>
+  </si>
+  <si>
+    <t>DUNEX</t>
   </si>
 </sst>
 </file>
@@ -293,7 +299,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -303,6 +309,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -375,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,11 +422,268 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="37">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2275,12 +2544,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="containsBlanks" dxfId="9" priority="8">
+    <cfRule type="containsBlanks" dxfId="35" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2290,1161 +2559,1369 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>2</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>9</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>10</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>14</v>
       </c>
       <c r="B14" s="6"/>
-      <c r="C14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>16</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>17</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>20</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>21</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>23</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>24</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>25</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>26</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>27</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>28</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C28" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>29</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>30</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>31</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>32</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
         <v>33</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>34</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
         <v>35</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C35" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>36</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
         <v>37</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C37" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>38</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C38" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
         <v>39</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C39" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C39" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>40</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="6">
         <v>41</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C41" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>42</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C42" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="6">
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C43" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C44" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="6">
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C45" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>46</v>
       </c>
       <c r="B46" s="6"/>
-      <c r="C46" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C46" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="6">
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C47" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C48" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="6">
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C49" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>50</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F50" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="6">
         <v>51</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C51" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>52</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C52" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="6">
         <v>53</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>54</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F54" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="6">
         <v>55</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F55" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>56</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="6">
         <v>57</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C57" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>58</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C58" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F58" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="6">
         <v>59</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C59" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F59" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>60</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C60" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E60" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F60" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="6">
         <v>61</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C61" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F61" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>62</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C62" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D62" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E62" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="6">
         <v>63</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C63" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E63" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F63" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>64</v>
       </c>
       <c r="B64" s="6"/>
-      <c r="C64" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C64" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="6">
         <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C65" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D65" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>66</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66" s="10" t="s">
+      <c r="C66" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D66" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" s="12" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="7" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="12">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="20" priority="13">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E66">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="x">
-      <formula>NOT(ISERROR(SEARCH("x",D2)))</formula>
+  <conditionalFormatting sqref="E2:F66">
+    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",E2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:E66">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+  <conditionalFormatting sqref="C2:C66 E2:F66">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="notEqual">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C66 E2:F66">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D66">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added missions 8-14 in the notes sheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0292F5-EF9A-354B-9489-92A11D016F6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E549D9C-AFBC-8C4F-90AC-9DD4A9271CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="111">
   <si>
     <t>Mission Number</t>
   </si>
@@ -284,6 +284,96 @@
   </si>
   <si>
     <t>DUNEX</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No git repo - lock time is wrong - </t>
+  </si>
+  <si>
+    <t>DUNEX-Develoment</t>
+  </si>
+  <si>
+    <t>jetski</t>
+  </si>
+  <si>
+    <t>thrown from pier</t>
+  </si>
+  <si>
+    <t>cross shore line outside of break</t>
+  </si>
+  <si>
+    <t>42,44,5,45,40,46,31,57,29</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>2021-10-07T14:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-07T14:20:00</t>
+  </si>
+  <si>
+    <t>33,4,27,41,38,37,39,25</t>
+  </si>
+  <si>
+    <t>2021-10-07T14:30:00</t>
+  </si>
+  <si>
+    <t>2021-10-07T14:50:00</t>
+  </si>
+  <si>
+    <t>42,44,5,45,40,46,31,57</t>
+  </si>
+  <si>
+    <t>2021-10-07T14:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-07T15:10:00</t>
+  </si>
+  <si>
+    <t>34,38,41,37,25,39,4,27,33</t>
+  </si>
+  <si>
+    <t>2021-10-07T16:00:00</t>
+  </si>
+  <si>
+    <t>4,5,25,31,33,34,37,38,39,40,41,42,44,45,46,57,27</t>
+  </si>
+  <si>
+    <t>3,4,5,6</t>
+  </si>
+  <si>
+    <t>2021-10-07T16:30:00</t>
+  </si>
+  <si>
+    <t>4,5,25,27,29,31,33,34,37,38,39,40,41,42,44,45,46,57</t>
+  </si>
+  <si>
+    <t>2021-10-07T17:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-07T17:25:00</t>
+  </si>
+  <si>
+    <t>No telemetry on 004</t>
+  </si>
+  <si>
+    <t>2021-10-07T18:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-07T18:35:00</t>
+  </si>
+  <si>
+    <t>lifeguard 1</t>
+  </si>
+  <si>
+    <t>lifeguard 2</t>
+  </si>
+  <si>
+    <t>No Additional Notes</t>
   </si>
 </sst>
 </file>
@@ -429,134 +519,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <color theme="1"/>
@@ -645,99 +608,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -748,40 +618,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1097,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1691,164 +1527,430 @@
       <c r="T9" s="1"/>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="4"/>
+    <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="4">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T10" s="1"/>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="4"/>
+    <row r="11" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="4">
+        <v>9</v>
+      </c>
+      <c r="M11" s="4">
+        <v>2</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T11" s="1"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="4"/>
+    <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" s="4">
+        <v>8</v>
+      </c>
+      <c r="M12" s="4">
+        <v>2</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T12" s="1"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="4"/>
+    <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9</v>
+      </c>
+      <c r="M13" s="4">
+        <v>2</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T13" s="1"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="4"/>
+    <row r="14" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>44</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" s="4">
+        <v>17</v>
+      </c>
+      <c r="M14" s="4">
+        <v>4</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T14" s="1"/>
       <c r="U14" s="4"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="4"/>
+    <row r="15" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" s="4">
+        <v>18</v>
+      </c>
+      <c r="M15" s="4">
+        <v>4</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="T15" s="1"/>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="4"/>
+    <row r="16" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" s="4">
+        <v>18</v>
+      </c>
+      <c r="M16" s="4">
+        <v>4</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T16" s="1"/>
       <c r="U16" s="4"/>
     </row>
@@ -2544,12 +2646,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="containsBlanks" dxfId="35" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:U46">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2559,10 +2661,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2647,10 +2749,10 @@
         <v>80</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -2667,10 +2769,10 @@
         <v>80</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2889,7 +2991,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>17</v>
       </c>
@@ -2909,7 +3011,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>18</v>
       </c>
@@ -2929,7 +3031,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>19</v>
       </c>
@@ -2949,7 +3051,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>20</v>
       </c>
@@ -2969,7 +3071,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>21</v>
       </c>
@@ -2989,7 +3091,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>22</v>
       </c>
@@ -3009,7 +3111,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>23</v>
       </c>
@@ -3029,7 +3131,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>24</v>
       </c>
@@ -3049,7 +3151,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>25</v>
       </c>
@@ -3069,7 +3171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>26</v>
       </c>
@@ -3089,7 +3191,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>27</v>
       </c>
@@ -3109,7 +3211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>28</v>
       </c>
@@ -3129,7 +3231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
         <v>29</v>
       </c>
@@ -3146,10 +3248,10 @@
         <v>17</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>30</v>
       </c>
@@ -3169,7 +3271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
         <v>31</v>
       </c>
@@ -3177,19 +3279,19 @@
         <v>17</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>32</v>
       </c>
@@ -3197,16 +3299,19 @@
         <v>17</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>77</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="G32" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -3237,13 +3342,13 @@
         <v>17</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>77</v>
@@ -3303,10 +3408,10 @@
         <v>80</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3323,10 +3428,10 @@
         <v>80</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3343,10 +3448,10 @@
         <v>80</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -3363,10 +3468,10 @@
         <v>80</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -3383,10 +3488,10 @@
         <v>80</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -3397,16 +3502,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -3437,16 +3542,16 @@
         <v>17</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F44" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -3457,13 +3562,13 @@
         <v>17</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F45" s="12" t="s">
         <v>77</v>
@@ -3473,15 +3578,17 @@
       <c r="A46" s="6">
         <v>46</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C46" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>77</v>
@@ -3701,10 +3808,10 @@
         <v>80</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F57" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -3887,41 +3994,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="21" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="12">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="20" priority="13">
+    <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F66">
-    <cfRule type="containsText" dxfId="19" priority="10" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66">
-    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D66">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated notes spreadsheet with more missions
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537F8425-8058-3149-9232-518E5038FF23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59887893-791F-CE4F-A1CE-81317E3D46E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="125">
   <si>
     <t>Mission Number</t>
   </si>
@@ -375,12 +375,54 @@
   <si>
     <t>No Additional Notes</t>
   </si>
+  <si>
+    <t>4,5,7,14,15,16,17,18,19,20,21,22,23,24,25,29,31,33,34,37,38,39,40,41,42,43,44,45,46,56,57,11,13,12</t>
+  </si>
+  <si>
+    <t>4,5,7,14,16,17,18,19,20,21,22,23,24,29,31,33,34,37,38,39,40,41,42,43,44,45,46,56,57,11,13,12</t>
+  </si>
+  <si>
+    <t>2021-10-08T13:17:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T13:46:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T14:05:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T14:46:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T15:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T16:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">microSWIFTs 21 and 40 are not able to be ssh'ed into so they still need to be offloaded for this mission. </t>
+  </si>
+  <si>
+    <t>2021-10-08T17:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T18:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T18:18:00</t>
+  </si>
+  <si>
+    <t>2021-10-08T19:00:00</t>
+  </si>
+  <si>
+    <t>needs help</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,8 +430,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +455,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -477,7 +532,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -513,6 +568,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -933,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P4" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1970,8 +2028,10 @@
       </c>
       <c r="U16" s="4"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
+    <row r="17" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1984,17 +2044,29 @@
       <c r="K17" s="1"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="N17" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="P17" s="4"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+      <c r="Q17" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="S17" s="4"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
+      <c r="U17" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2007,17 +2079,27 @@
       <c r="K18" s="1"/>
       <c r="L18" s="4"/>
       <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
+      <c r="N18" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="P18" s="4"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+      <c r="Q18" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="S18" s="4"/>
       <c r="T18" s="1"/>
       <c r="U18" s="4"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -2030,17 +2112,27 @@
       <c r="K19" s="1"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="N19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="P19" s="4"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+      <c r="Q19" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="R19" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="S19" s="4"/>
       <c r="T19" s="1"/>
       <c r="U19" s="4"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -2053,17 +2145,27 @@
       <c r="K20" s="1"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
+      <c r="N20" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="P20" s="4"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="Q20" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="R20" s="13" t="s">
+        <v>121</v>
+      </c>
       <c r="S20" s="4"/>
       <c r="T20" s="1"/>
       <c r="U20" s="4"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -2076,11 +2178,19 @@
       <c r="K21" s="1"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
+      <c r="N21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="P21" s="4"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+      <c r="Q21" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>123</v>
+      </c>
       <c r="S21" s="4"/>
       <c r="T21" s="1"/>
       <c r="U21" s="4"/>
@@ -2661,12 +2771,12 @@
       <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:U46">
+  <conditionalFormatting sqref="A2:U18 A22:U46 A19:P21 S19:U21">
     <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:U46">
+  <conditionalFormatting sqref="A2:U18 A22:U46 A19:P21 S19:U21">
     <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
@@ -2679,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2767,9 +2877,7 @@
       <c r="E4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="F4" s="12"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
@@ -2819,17 +2927,15 @@
         <v>17</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>77</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
@@ -2897,16 +3003,16 @@
         <v>17</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2917,16 +3023,16 @@
         <v>17</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2953,7 +3059,9 @@
       <c r="A14" s="6">
         <v>14</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C14" s="12" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
All missions have been updated in the notes spreadsheet from week 1
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59887893-791F-CE4F-A1CE-81317E3D46E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F792FF5-CC88-DF4E-8EEC-6190FDA90652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="130">
   <si>
     <t>Mission Number</t>
   </si>
@@ -416,6 +416,23 @@
   </si>
   <si>
     <t>needs help</t>
+  </si>
+  <si>
+    <t>1,3,4,5,6</t>
+  </si>
+  <si>
+    <t>microSWIFT 015 has some water in it
+Shepherd 4 needs foam on the bolts so it doesn’t get damaged
+025 has some water in it</t>
+  </si>
+  <si>
+    <t>two along shore lines with 50 ft spacing and one cross shore line</t>
+  </si>
+  <si>
+    <t>lifeguards</t>
+  </si>
+  <si>
+    <t>Christine and Sean</t>
   </si>
 </sst>
 </file>
@@ -991,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,8 +1355,12 @@
       <c r="S5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="4"/>
+      <c r="T5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="6" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1399,8 +1420,12 @@
       <c r="S6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="4"/>
+      <c r="T6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="7" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1460,8 +1485,12 @@
       <c r="S7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="4"/>
+      <c r="T7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="8" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1521,8 +1550,12 @@
       <c r="S8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="1"/>
-      <c r="U8" s="4"/>
+      <c r="T8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1582,8 +1615,12 @@
       <c r="S9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="T9" s="1"/>
-      <c r="U9" s="4"/>
+      <c r="T9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1711,7 +1748,9 @@
       <c r="T11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U11" s="4"/>
+      <c r="U11" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="12" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1774,7 +1813,9 @@
       <c r="T12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U12" s="4"/>
+      <c r="U12" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="13" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1837,7 +1878,9 @@
       <c r="T13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U13" s="4"/>
+      <c r="U13" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="14" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1900,7 +1943,9 @@
       <c r="T14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U14" s="4"/>
+      <c r="U14" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="15" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1963,7 +2008,9 @@
       <c r="T15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U15" s="4"/>
+      <c r="U15" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:21" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -2026,39 +2073,71 @@
       <c r="T16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="U16" s="4"/>
+      <c r="U16" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="17" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+      <c r="B17" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>60</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="4">
+        <v>34</v>
+      </c>
+      <c r="M17" s="4">
+        <v>5</v>
+      </c>
       <c r="N17" s="4" t="s">
         <v>111</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P17" s="4"/>
+      <c r="P17" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="Q17" s="1" t="s">
         <v>113</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="S17" s="4"/>
-      <c r="T17" s="1"/>
+      <c r="S17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="U17" s="4" t="s">
         <v>119</v>
       </c>
@@ -2067,133 +2146,261 @@
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
+      <c r="B18" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L18" s="4">
+        <v>32</v>
+      </c>
+      <c r="M18" s="4">
+        <v>5</v>
+      </c>
       <c r="N18" s="4" t="s">
         <v>112</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P18" s="4"/>
+      <c r="P18" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="Q18" s="1" t="s">
         <v>115</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="S18" s="4"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="4"/>
+      <c r="S18" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U18" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="19" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
+      <c r="B19" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>60</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L19" s="4">
+        <v>32</v>
+      </c>
+      <c r="M19" s="4">
+        <v>5</v>
+      </c>
       <c r="N19" s="4" t="s">
         <v>112</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P19" s="4"/>
+      <c r="P19" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="Q19" s="13" t="s">
         <v>117</v>
       </c>
       <c r="R19" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="S19" s="4"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="4"/>
+      <c r="S19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="20" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
+      <c r="B20" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
+        <v>60</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="4">
+        <v>32</v>
+      </c>
+      <c r="M20" s="4">
+        <v>5</v>
+      </c>
       <c r="N20" s="4" t="s">
         <v>112</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P20" s="4"/>
+      <c r="P20" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="Q20" s="13" t="s">
         <v>120</v>
       </c>
       <c r="R20" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="S20" s="4"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="4"/>
+      <c r="S20" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
+      <c r="B21" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>60</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L21" s="4">
+        <v>32</v>
+      </c>
+      <c r="M21" s="4">
+        <v>5</v>
+      </c>
       <c r="N21" s="4" t="s">
         <v>112</v>
       </c>
       <c r="O21" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P21" s="4"/>
+      <c r="P21" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="Q21" s="13" t="s">
         <v>122</v>
       </c>
       <c r="R21" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="S21" s="4"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="4"/>
+      <c r="S21" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -2771,12 +2978,12 @@
       <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:U18 A22:U46 A19:P21 S19:U21">
+  <conditionalFormatting sqref="A19:P21 A22:U46 A2:U18 S19:U21">
     <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:U18 A22:U46 A19:P21 S19:U21">
+  <conditionalFormatting sqref="A19:P21 A22:U46 A2:U18 S19:U21">
     <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
@@ -2789,8 +2996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3043,16 +3250,16 @@
         <v>17</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3063,16 +3270,16 @@
         <v>17</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added missions 20-23 to the notes sheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F792FF5-CC88-DF4E-8EEC-6190FDA90652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874F0911-B718-F24F-8DB6-CCA4A7DC12FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="143">
   <si>
     <t>Mission Number</t>
   </si>
@@ -433,6 +433,45 @@
   </si>
   <si>
     <t>Christine and Sean</t>
+  </si>
+  <si>
+    <t>54,2,3,4,6,7,8,9,56,11,12,13,14,57,16,17,18,19,20,21,22,23,24,58,26,27,28,29,59,31,32,33,34,35,36,37,38,40,41,42,43,44,45,46,47,48,49,39,50</t>
+  </si>
+  <si>
+    <t>54,2,3,4,5,6,7,8,9,56,11,12,13,14,57,16,17,18,19,20,21,22,23,24,58,26,27,28,29,59,31,32,33,34,35,36,37,38,40,41,42,43,44,45,46,47,48,49,39,50</t>
+  </si>
+  <si>
+    <t>2,3,4,6,7,8,9,56,11,12,13,14,57,16,17,18,20,21,22,23,24,58,26,27,28,29,59,31,32,33,34,35,36,37,38,40,41,42,43,44,45,46,48,49,39,50</t>
+  </si>
+  <si>
+    <t>2021-10-10T13:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T13:27:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T14:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T14:36:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T15:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T15:27:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T16:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-10T16:35:00</t>
+  </si>
+  <si>
+    <t>launcher and pier</t>
+  </si>
+  <si>
+    <t>clusters from the end of pier and a cross shore line from pier</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2402,94 +2441,238 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+    <row r="22" spans="1:21" ht="85" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="C22" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D22" s="1">
+        <v>105</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="4">
+        <v>51</v>
+      </c>
+      <c r="M22" s="4">
+        <v>5</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="S22" s="4"/>
       <c r="T22" s="1"/>
       <c r="U22" s="4"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
+    <row r="23" spans="1:21" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="C23" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D23" s="1">
+        <v>105</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="4">
+        <v>51</v>
+      </c>
+      <c r="M23" s="4">
+        <v>5</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="S23" s="4"/>
       <c r="T23" s="1"/>
       <c r="U23" s="4"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
+    <row r="24" spans="1:21" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="C24" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D24" s="1">
+        <v>105</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L24" s="4">
+        <v>47</v>
+      </c>
+      <c r="M24" s="4">
+        <v>5</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P24" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="S24" s="4"/>
       <c r="T24" s="1"/>
       <c r="U24" s="4"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
+    <row r="25" spans="1:21" ht="85" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="C25" s="1">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="D25" s="1">
+        <v>105</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L25" s="4">
+        <v>47</v>
+      </c>
+      <c r="M25" s="4">
+        <v>5</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="S25" s="4"/>
       <c r="T25" s="1"/>
       <c r="U25" s="4"/>
@@ -2978,12 +3161,12 @@
       <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A22:U46 A2:U18 S19:U21">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U46">
     <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A22:U46 A2:U18 S19:U21">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U46">
     <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
All mission notes updated in spreadsheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924570C6-70D6-2A4C-B0ED-391F42C79302}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF06213-D1BD-524B-8A2F-21D4B728B014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="160">
   <si>
     <t>Mission Number</t>
   </si>
@@ -475,6 +475,57 @@
   </si>
   <si>
     <t>005,019,054 and 47 got water in them and we have not been able to recover data from them yet</t>
+  </si>
+  <si>
+    <t>2,3,4,6,8,56,11,12,13,14,57,16,17,18,20,22,23,24,58,27,28,29,59,31,32,33,34,35,36,37,39,41,42,43,44,46,49,50,6</t>
+  </si>
+  <si>
+    <t>2021-10-11T13:05:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T14:10:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T16:05:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T17:25:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T13:47:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T14:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T17:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-11T18:10:00</t>
+  </si>
+  <si>
+    <t>pier</t>
+  </si>
+  <si>
+    <t>Melissa Moulton</t>
+  </si>
+  <si>
+    <t>Joe Talbert</t>
+  </si>
+  <si>
+    <t>two oblong clusters</t>
+  </si>
+  <si>
+    <t>041 Swing Arms off
+043 gps battery popped out
+029 one nut came off modem 
+017 had swing arms off</t>
+  </si>
+  <si>
+    <t>switched to oblong clusters to get good alongshore resolution on boundary and closer to shore drifters to compare</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N17" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" topLeftCell="G26" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2688,95 +2739,247 @@
       <c r="T25" s="1"/>
       <c r="U25" s="4"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
-      <c r="S26" s="4"/>
+    <row r="26" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>79</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L26" s="4">
+        <v>39</v>
+      </c>
+      <c r="M26" s="4">
+        <v>5</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T26" s="1"/>
       <c r="U26" s="4"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="4"/>
+    <row r="27" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C27" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D27" s="1">
+        <v>79</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L27" s="4">
+        <v>39</v>
+      </c>
+      <c r="M27" s="4">
+        <v>5</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="S27" s="4" t="s">
+        <v>157</v>
+      </c>
       <c r="T27" s="1"/>
       <c r="U27" s="4"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="4"/>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="4"/>
+    <row r="28" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28" s="4">
+        <v>38</v>
+      </c>
+      <c r="M28" s="4">
+        <v>5</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="T28" s="1"/>
       <c r="U28" s="4"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="4"/>
-      <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="4"/>
-      <c r="P29" s="4"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="4"/>
+    <row r="29" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C29" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>79</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29" s="4">
+        <v>37</v>
+      </c>
+      <c r="M29" s="4">
+        <v>5</v>
+      </c>
+      <c r="N29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q29" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="R29" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>158</v>
+      </c>
       <c r="T29" s="1"/>
       <c r="U29" s="4"/>
     </row>
@@ -3079,7 +3282,7 @@
       <c r="T42" s="1"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3091,7 +3294,9 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="4"/>
+      <c r="L43" s="4" t="s">
+        <v>159</v>
+      </c>
       <c r="M43" s="4"/>
       <c r="N43" s="4"/>
       <c r="O43" s="4"/>
@@ -3172,12 +3377,12 @@
       <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U46">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A30:U46 A29:P29 A22:U28 S29:U29">
     <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U46">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A30:U46 A29:P29 A22:U28 S29:U29">
     <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated notes sheet to have mission 28
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF06213-D1BD-524B-8A2F-21D4B728B014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B236848-3EC9-B84F-9F3F-D4334C7729BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="165">
   <si>
     <t>Mission Number</t>
   </si>
@@ -526,6 +526,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>jeski</t>
+  </si>
+  <si>
+    <t>two along shore lines with 50 ft spacing</t>
+  </si>
+  <si>
+    <t>2021-10-12T18:00:00</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,8,56,12,13,14,57,16,17,18,19,20,23,24,58,27,28,29</t>
+  </si>
+  <si>
+    <t>2021-10-12T13:10:00</t>
   </si>
 </sst>
 </file>
@@ -1101,8 +1116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G26" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" topLeftCell="M26" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2983,13 +2998,19 @@
       <c r="T29" s="1"/>
       <c r="U29" s="4"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
+    <row r="30" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="E30" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2997,11 +3018,21 @@
       <c r="K30" s="1"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4"/>
-      <c r="N30" s="4"/>
-      <c r="O30" s="4"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
+      <c r="N30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q30" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="R30" s="13" t="s">
+        <v>162</v>
+      </c>
       <c r="S30" s="4"/>
       <c r="T30" s="1"/>
       <c r="U30" s="4"/>
@@ -3377,12 +3408,12 @@
       <c r="U46" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A30:U46 A29:P29 A22:U28 S29:U29">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 A31:U46 S29:U30 A29:P30">
     <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A30:U46 A29:P29 A22:U28 S29:U29">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 A31:U46 S29:U30 A29:P30">
     <cfRule type="notContainsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated notes to mission 40
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B236848-3EC9-B84F-9F3F-D4334C7729BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E8FBAC-87F2-D64A-A22B-7AC693D573FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="218">
   <si>
     <t>Mission Number</t>
   </si>
@@ -541,6 +541,165 @@
   </si>
   <si>
     <t>2021-10-12T13:10:00</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,56,11,12,13,14</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2021-10-13T13:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-13T13:35:00</t>
+  </si>
+  <si>
+    <t>2,3,4,5,56,11,12,13,14,57,41,42,43,44,46,49,50,60,31</t>
+  </si>
+  <si>
+    <t>1,6,3,4</t>
+  </si>
+  <si>
+    <t>2021-10-13T14:04:00</t>
+  </si>
+  <si>
+    <t>2021-10-13T15:15:00</t>
+  </si>
+  <si>
+    <t>2,3,4,5,11,12,13,14,16,17,41,42,43,46,31,44,32,33,34,35</t>
+  </si>
+  <si>
+    <t>1,3,4,6</t>
+  </si>
+  <si>
+    <t>3,2,57,56,18,19,20,59,29,28,27,16,58,46,23,12,11,14,13,17,36,42,31,44,41,43,33,49,32</t>
+  </si>
+  <si>
+    <t>1,3,6,4,5</t>
+  </si>
+  <si>
+    <t>2021-10-13T16:15:00</t>
+  </si>
+  <si>
+    <t>2021-10-13T17:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-13T17:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-13T17:20:00</t>
+  </si>
+  <si>
+    <t>44,2,43,41,31,32,33,34,35,36</t>
+  </si>
+  <si>
+    <t>2021-10-14T12:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-14T12:45:00</t>
+  </si>
+  <si>
+    <t>3,4,11,12,13,14,57,16,18,17,56,9,60,23,37</t>
+  </si>
+  <si>
+    <t>2021-10-14T13:15:00</t>
+  </si>
+  <si>
+    <t>2021-10-14T12:56:00</t>
+  </si>
+  <si>
+    <t>2021-10-14T14:00:00</t>
+  </si>
+  <si>
+    <t>43,44,46,35,36,37,34,33,32,31,23,39,58</t>
+  </si>
+  <si>
+    <t>2021-10-14T15:00:00</t>
+  </si>
+  <si>
+    <t>11,12,2,3,4,13,14,57,16,17,18,19,9,56,27,60</t>
+  </si>
+  <si>
+    <t>2021-10-14T15:06:00</t>
+  </si>
+  <si>
+    <t>2021-10-14T16:00:00</t>
+  </si>
+  <si>
+    <t>42,4,12,56,19,2,11,16,27,13,3,17,9,18,14,43,44,31,23,32,33,34,35,46,58,60,36,37,39,29</t>
+  </si>
+  <si>
+    <t>2021-10-14T17:13:00</t>
+  </si>
+  <si>
+    <t>2021-10-14T18:00:00</t>
+  </si>
+  <si>
+    <t>along shore line on north side of pier</t>
+  </si>
+  <si>
+    <t>along shore lines on north side of pier</t>
+  </si>
+  <si>
+    <t>along shore lines on north side of pier but asked thme to place them closer alongshore distance than previous lines</t>
+  </si>
+  <si>
+    <t>alongshore lines on south side of pier</t>
+  </si>
+  <si>
+    <t>along shore line on south side of pier in surfzone</t>
+  </si>
+  <si>
+    <t>along shore lines on south side of pier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alognshore line in surfzone with offshore clusters </t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>1,7</t>
+  </si>
+  <si>
+    <t>7,1</t>
+  </si>
+  <si>
+    <t>1,7,6,3,5,4</t>
+  </si>
+  <si>
+    <t>Instructed to place closer alongshore spacing</t>
+  </si>
+  <si>
+    <t>2,9,56,11,12,14,57,16,23,19,59,33,42,46,60,31</t>
+  </si>
+  <si>
+    <t>7,6,5,3</t>
+  </si>
+  <si>
+    <t>2021-10-15T16:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-15T17:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-15T18:00:00</t>
+  </si>
+  <si>
+    <t>surfboard</t>
+  </si>
+  <si>
+    <t>two alongshore lines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve, Britt and Jinshi helped with this mission </t>
+  </si>
+  <si>
+    <t>Interesting circulation patterns - had to pick up many micros on the north side of the pier after they went into the trough on the south side</t>
   </si>
 </sst>
 </file>
@@ -702,7 +861,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1114,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M26" workbookViewId="0">
-      <selection activeCell="Q31" sqref="Q31"/>
+    <sheetView tabSelected="1" topLeftCell="N28" workbookViewId="0">
+      <selection activeCell="S40" sqref="S40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3002,22 +3189,42 @@
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C30" s="1">
+        <v>9</v>
+      </c>
+      <c r="D30" s="1">
+        <v>75</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>160</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="4"/>
+      <c r="G30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L30" s="4">
+        <v>22</v>
+      </c>
+      <c r="M30" s="4">
+        <v>5</v>
+      </c>
       <c r="N30" s="4" t="s">
         <v>163</v>
       </c>
@@ -3033,283 +3240,741 @@
       <c r="R30" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="S30" s="4"/>
+      <c r="S30" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T30" s="1"/>
       <c r="U30" s="4"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="4"/>
+    <row r="31" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C31" s="1">
+        <v>9</v>
+      </c>
+      <c r="D31" s="1">
+        <v>75</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L31" s="4">
+        <v>10</v>
+      </c>
+      <c r="M31" s="4">
+        <v>2</v>
+      </c>
+      <c r="N31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T31" s="1"/>
       <c r="U31" s="4"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="4"/>
+    <row r="32" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C32" s="1">
+        <v>9</v>
+      </c>
+      <c r="D32" s="1">
+        <v>75</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" s="4">
+        <v>19</v>
+      </c>
+      <c r="M32" s="4">
+        <v>4</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T32" s="1"/>
       <c r="U32" s="4"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="4"/>
+    <row r="33" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C33" s="1">
+        <v>9</v>
+      </c>
+      <c r="D33" s="1">
+        <v>75</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L33" s="4">
+        <v>20</v>
+      </c>
+      <c r="M33" s="4">
+        <v>4</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T33" s="1"/>
       <c r="U33" s="4"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
-      <c r="O34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="4"/>
+    <row r="34" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="C34" s="1">
+        <v>9</v>
+      </c>
+      <c r="D34" s="1">
+        <v>75</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L34" s="4">
+        <v>29</v>
+      </c>
+      <c r="M34" s="4">
+        <v>5</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>208</v>
+      </c>
       <c r="T34" s="1"/>
       <c r="U34" s="4"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="4"/>
+    <row r="35" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D35" s="1">
+        <v>93</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" s="4">
+        <v>10</v>
+      </c>
+      <c r="M35" s="4">
+        <v>2</v>
+      </c>
+      <c r="N35" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="R35" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T35" s="1"/>
       <c r="U35" s="4"/>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
-      <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="1"/>
-      <c r="R36" s="1"/>
-      <c r="S36" s="4"/>
+    <row r="36" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D36" s="1">
+        <v>93</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="4">
+        <v>10</v>
+      </c>
+      <c r="M36" s="4">
+        <v>2</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="S36" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T36" s="1"/>
       <c r="U36" s="4"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="4"/>
-      <c r="N37" s="4"/>
-      <c r="O37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
-      <c r="S37" s="4"/>
+    <row r="37" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D37" s="1">
+        <v>93</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L37" s="4">
+        <v>15</v>
+      </c>
+      <c r="M37" s="4">
+        <v>2</v>
+      </c>
+      <c r="N37" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="P37" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="S37" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T37" s="1"/>
       <c r="U37" s="4"/>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
-      <c r="N38" s="4"/>
-      <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="4"/>
+    <row r="38" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D38" s="1">
+        <v>93</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="4">
+        <v>13</v>
+      </c>
+      <c r="M38" s="4">
+        <v>2</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S38" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T38" s="1"/>
       <c r="U38" s="4"/>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="1"/>
-      <c r="R39" s="1"/>
-      <c r="S39" s="4"/>
+    <row r="39" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D39" s="1">
+        <v>93</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="4">
+        <v>16</v>
+      </c>
+      <c r="M39" s="4">
+        <v>2</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="P39" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="S39" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T39" s="1"/>
       <c r="U39" s="4"/>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="4"/>
-      <c r="M40" s="4"/>
-      <c r="N40" s="4"/>
-      <c r="O40" s="4"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
-      <c r="S40" s="4"/>
+    <row r="40" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="D40" s="1">
+        <v>93</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L40" s="4">
+        <v>30</v>
+      </c>
+      <c r="M40" s="4">
+        <v>6</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P40" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="S40" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="T40" s="1"/>
       <c r="U40" s="4"/>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="4"/>
+    <row r="41" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="C41" s="1">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L41" s="4">
+        <v>16</v>
+      </c>
+      <c r="M41" s="4">
+        <v>4</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="P41" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="S41" s="4" t="s">
+        <v>217</v>
+      </c>
       <c r="T41" s="1"/>
       <c r="U41" s="4"/>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="4"/>
+    <row r="42" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="C42" s="1">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1">
+        <v>83</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L42" s="4">
+        <v>16</v>
+      </c>
+      <c r="M42" s="4">
+        <v>4</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="P42" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="R42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="S42" s="4" t="s">
+        <v>216</v>
+      </c>
       <c r="T42" s="1"/>
       <c r="U42" s="4"/>
     </row>
@@ -3407,15 +4072,702 @@
       <c r="T46" s="1"/>
       <c r="U46" s="4"/>
     </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="4"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="1"/>
+      <c r="U48" s="4"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="4"/>
+      <c r="T49" s="1"/>
+      <c r="U49" s="4"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="1"/>
+      <c r="U50" s="4"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="1"/>
+      <c r="U51" s="4"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" s="4"/>
+      <c r="T52" s="1"/>
+      <c r="U52" s="4"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="1"/>
+      <c r="U53" s="4"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="1"/>
+      <c r="U54" s="4"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="1"/>
+      <c r="U55" s="4"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="4"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="4"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="1"/>
+      <c r="U58" s="4"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="1"/>
+      <c r="U59" s="4"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="1"/>
+      <c r="U60" s="4"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="1"/>
+      <c r="U61" s="4"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="1"/>
+      <c r="U62" s="4"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="4"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="1"/>
+      <c r="U63" s="4"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="J64" s="1"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="1"/>
+      <c r="U64" s="4"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="4"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="1"/>
+      <c r="U65" s="4"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+      <c r="S66" s="4"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="4"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="4"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+      <c r="S68" s="4"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="4"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="4"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="4"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="4"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="4"/>
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="4"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="4"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="4"/>
+      <c r="M73" s="4"/>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4"/>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="1"/>
+      <c r="U73" s="4"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="J74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="1"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="1"/>
+      <c r="U74" s="4"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="J75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="4"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 A31:U46 S29:U30 A29:P30">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
+    <cfRule type="containsBlanks" dxfId="14" priority="12">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 A31:U46 S29:U30 A29:P30">
-    <cfRule type="notContainsBlanks" dxfId="9" priority="2">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
+    <cfRule type="notContainsBlanks" dxfId="13" priority="6">
       <formula>LEN(TRIM(A2))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N36">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(N36))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N36">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(N36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O36">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(O36))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O36">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4755,41 +6107,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="12">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="7" priority="13">
+    <cfRule type="containsBlanks" dxfId="11" priority="13">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F66">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D66">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added sheet for broken micros
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E8FBAC-87F2-D64A-A22B-7AC693D573FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6B5C3C-909A-BF47-AD24-27A1778809EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="226">
   <si>
     <t>Mission Number</t>
   </si>
@@ -700,6 +701,30 @@
   </si>
   <si>
     <t>Interesting circulation patterns - had to pick up many micros on the north side of the pier after they went into the trough on the south side</t>
+  </si>
+  <si>
+    <t>microSWIFTs to fix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problem </t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
+  <si>
+    <t>No IMU</t>
+  </si>
+  <si>
+    <t>No GPS data</t>
+  </si>
+  <si>
+    <t>Water Damage and no GPS battery</t>
+  </si>
+  <si>
+    <t>missing all data</t>
+  </si>
+  <si>
+    <t>water damage</t>
   </si>
 </sst>
 </file>
@@ -1303,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N28" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4775,6 +4800,169 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2291D0-3C09-0C45-8CBB-DD5A881036D5}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="10">
+        <v>22</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="10">
+        <v>40</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>39</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>9</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>26</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>38</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>41</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>54</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>24</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>18</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>45</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>48</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>21</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:G66"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added borken micros notes on sheet 3
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/Documents/UW/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B6324-67C6-2F49-892A-5D21F4798D3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDACC140-0697-4046-B5AC-C07D9FBC62C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="255">
   <si>
     <t>Mission Number</t>
   </si>
@@ -709,9 +709,6 @@
     <t xml:space="preserve">Problem </t>
   </si>
   <si>
-    <t>Fixed?</t>
-  </si>
-  <si>
     <t>No IMU</t>
   </si>
   <si>
@@ -725,6 +722,96 @@
   </si>
   <si>
     <t>water damage</t>
+  </si>
+  <si>
+    <t>Lots of problems - No IMU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O error on IMU </t>
+  </si>
+  <si>
+    <t>Is recroding IMU now with no problems - data all looks normal</t>
+  </si>
+  <si>
+    <t>Further Details</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Initializes IMU and powers on but never opens file to run - missing two devices so it needs some solders - missing gyro/accel and current sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not able to initialize GPS so it may need a new GPS battery </t>
+  </si>
+  <si>
+    <t>had lights off during last deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seems to be running just fine now </t>
+  </si>
+  <si>
+    <t>is currently getting all data</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>only seeing two devices - missing aceel/gyro and current sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no none problem </t>
+  </si>
+  <si>
+    <t>was missing all data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">needs recloning and needs service script started - no processes running </t>
+  </si>
+  <si>
+    <t>not able to ssh into</t>
+  </si>
+  <si>
+    <t>looks fine</t>
+  </si>
+  <si>
+    <t>not getting gps data</t>
+  </si>
+  <si>
+    <t>not offloading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could have been too low of battery to actually ssh into </t>
+  </si>
+  <si>
+    <t>broken SD card holder</t>
+  </si>
+  <si>
+    <t>needs to raspberry pi</t>
+  </si>
+  <si>
+    <t>getting nan values or no data for GPS data and not software update needed since it was trying to send in a record window - old settings?</t>
+  </si>
+  <si>
+    <t>seems fine now</t>
+  </si>
+  <si>
+    <t>need to replace Raspberry pi</t>
+  </si>
+  <si>
+    <t>no light on raspberry pi - needs new raspberry pi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">needs a git pull on DUNEX branch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rebooting at minute 50 </t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>missing current sensor on i2cdetect</t>
   </si>
 </sst>
 </file>
@@ -888,34 +975,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -999,6 +1058,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4776,22 +4863,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="3">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="10" priority="2">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6132,41 +6219,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="12">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="11" priority="13">
+    <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F66">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D66">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6176,19 +6263,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2291D0-3C09-0C45-8CBB-DD5A881036D5}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="122.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>218</v>
       </c>
@@ -6196,180 +6284,262 @@
         <v>219</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>22</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>40</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>5</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="10"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>8</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="D5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>39</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="C6" s="10"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="D6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>9</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>220</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>26</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>11</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>38</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>41</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>54</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>24</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="D14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>18</v>
       </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>45</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B16" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="C17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>21</v>
       </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D18" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="D19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>15</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>25</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>28</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>6</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="10"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added up to mission 50 to notes
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085B6324-67C6-2F49-892A-5D21F4798D3F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3578897D-12F9-824B-AE6E-0965F27D58C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33220" windowHeight="18580" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="252">
   <si>
     <t>Mission Number</t>
   </si>
@@ -725,6 +725,84 @@
   </si>
   <si>
     <t>water damage</t>
+  </si>
+  <si>
+    <t>49,46,50,44,43,42,37,36,35,34,33,32,31,58,23</t>
+  </si>
+  <si>
+    <t>2021-10-17T12:15:00</t>
+  </si>
+  <si>
+    <t>2021-10-17T13:00:00</t>
+  </si>
+  <si>
+    <t>46,42,36,2,3,4,35,33,29,17,58,23,10,19,32,27,44,31,49,13,57,14,50,43,56,59,16,34</t>
+  </si>
+  <si>
+    <t>2021-10-17T15:22:00</t>
+  </si>
+  <si>
+    <t>2021-10-17T16:30:00</t>
+  </si>
+  <si>
+    <t>42,43,44,46,49,50,31,32,34,35,36,37,23,58,56,2,3,4,16,17,10,27,59,19,60,29</t>
+  </si>
+  <si>
+    <t>2021-10-17T14:00:00</t>
+  </si>
+  <si>
+    <t>4,2,3,4,8,56,9,10,11,12,13,14,16,17,18,19,20,21,23,57</t>
+  </si>
+  <si>
+    <t>2021-10-18T13:09:00</t>
+  </si>
+  <si>
+    <t>2021-10-18T15:42:00</t>
+  </si>
+  <si>
+    <t>56,2,3,4,8,10,12,13,14,57,16,17,18,19,20,21,23,24,58,42</t>
+  </si>
+  <si>
+    <t>2021-10-18T17:15:00</t>
+  </si>
+  <si>
+    <t>2021-10-18T18:40:00</t>
+  </si>
+  <si>
+    <t>41,42,43,44,46,49,50,31,32,33,34,35</t>
+  </si>
+  <si>
+    <t>2021-10-19T12:03:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T12:13:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T12:45:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T12:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T13:18:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T13:28:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T13:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T13:50:00</t>
+  </si>
+  <si>
+    <t>31,33,34,35,36,37,21,23,24,58,27,13,14,2,4,57,16,17,9,56,20,29,8</t>
+  </si>
+  <si>
+    <t>2021-10-19T15:15:00</t>
+  </si>
+  <si>
+    <t>2021-10-19T15:36:00</t>
   </si>
 </sst>
 </file>
@@ -888,34 +966,6 @@
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="1"/>
       </font>
@@ -999,6 +1049,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1328,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="I40" workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4003,8 +4081,10 @@
       <c r="T42" s="1"/>
       <c r="U42" s="4"/>
     </row>
-    <row r="43" spans="1:21" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
+    <row r="43" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -4019,17 +4099,27 @@
         <v>159</v>
       </c>
       <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
+      <c r="N43" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>226</v>
+      </c>
       <c r="P43" s="4"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
+      <c r="Q43" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="R43" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="S43" s="4"/>
       <c r="T43" s="1"/>
       <c r="U43" s="4"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
+    <row r="44" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -4042,17 +4132,27 @@
       <c r="K44" s="1"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
+      <c r="N44" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="P44" s="4"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+      <c r="Q44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="S44" s="4"/>
       <c r="T44" s="1"/>
       <c r="U44" s="4"/>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
+    <row r="45" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -4065,17 +4165,27 @@
       <c r="K45" s="1"/>
       <c r="L45" s="4"/>
       <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
+      <c r="N45" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="P45" s="4"/>
-      <c r="Q45" s="1"/>
-      <c r="R45" s="1"/>
+      <c r="Q45" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="R45" s="1" t="s">
+        <v>231</v>
+      </c>
       <c r="S45" s="4"/>
       <c r="T45" s="1"/>
       <c r="U45" s="4"/>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+    <row r="46" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -4088,17 +4198,27 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
+      <c r="N46" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="P46" s="1"/>
-      <c r="Q46" s="1"/>
-      <c r="R46" s="1"/>
+      <c r="Q46" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="R46" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="S46" s="4"/>
       <c r="T46" s="1"/>
       <c r="U46" s="4"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+    <row r="47" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -4111,17 +4231,27 @@
       <c r="K47" s="1"/>
       <c r="L47" s="4"/>
       <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
+      <c r="N47" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>237</v>
+      </c>
       <c r="P47" s="4"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
+      <c r="Q47" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="R47" s="1" t="s">
+        <v>239</v>
+      </c>
       <c r="S47" s="4"/>
       <c r="T47" s="1"/>
       <c r="U47" s="4"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
+    <row r="48" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -4134,17 +4264,27 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
+      <c r="N48" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="P48" s="1"/>
-      <c r="Q48" s="1"/>
-      <c r="R48" s="1"/>
+      <c r="Q48" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="R48" s="1" t="s">
+        <v>242</v>
+      </c>
       <c r="S48" s="4"/>
       <c r="T48" s="1"/>
       <c r="U48" s="4"/>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
+    <row r="49" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -4157,17 +4297,27 @@
       <c r="K49" s="1"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
+      <c r="N49" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="P49" s="4"/>
-      <c r="Q49" s="1"/>
-      <c r="R49" s="1"/>
+      <c r="Q49" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="R49" s="1" t="s">
+        <v>244</v>
+      </c>
       <c r="S49" s="4"/>
       <c r="T49" s="1"/>
       <c r="U49" s="4"/>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
+    <row r="50" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -4180,17 +4330,27 @@
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
+      <c r="N50" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+      <c r="Q50" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="R50" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="S50" s="4"/>
       <c r="T50" s="1"/>
       <c r="U50" s="4"/>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
+    <row r="51" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -4203,17 +4363,27 @@
       <c r="K51" s="1"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
+      <c r="N51" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>240</v>
+      </c>
       <c r="P51" s="4"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="1"/>
+      <c r="Q51" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="R51" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="S51" s="4"/>
       <c r="T51" s="1"/>
       <c r="U51" s="4"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
+    <row r="52" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -4226,11 +4396,19 @@
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
+      <c r="N52" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
-      <c r="R52" s="1"/>
+      <c r="Q52" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="R52" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="S52" s="4"/>
       <c r="T52" s="1"/>
       <c r="U52" s="4"/>
@@ -4272,8 +4450,8 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-      <c r="O54" s="1"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
@@ -4318,8 +4496,8 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="1"/>
       <c r="R56" s="1"/>
@@ -4364,8 +4542,8 @@
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
@@ -4410,8 +4588,8 @@
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-      <c r="O60" s="1"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
@@ -4456,8 +4634,8 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
@@ -4502,8 +4680,8 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="N64" s="1"/>
-      <c r="O64" s="1"/>
+      <c r="N64" s="4"/>
+      <c r="O64" s="4"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
@@ -4548,8 +4726,8 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
+      <c r="N66" s="4"/>
+      <c r="O66" s="4"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
@@ -4594,8 +4772,8 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
+      <c r="N68" s="4"/>
+      <c r="O68" s="4"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="1"/>
       <c r="R68" s="1"/>
@@ -4640,8 +4818,8 @@
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
-      <c r="O70" s="1"/>
+      <c r="N70" s="4"/>
+      <c r="O70" s="4"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="1"/>
       <c r="R70" s="1"/>
@@ -4686,8 +4864,8 @@
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
-      <c r="N72" s="1"/>
-      <c r="O72" s="1"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
@@ -4732,8 +4910,8 @@
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="1"/>
       <c r="R74" s="1"/>
@@ -4776,22 +4954,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="3">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="10" priority="2">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6132,41 +6310,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B66">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="12">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="12">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="11" priority="13">
+    <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F66">
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",E2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C66 E2:F66">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D66">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6178,7 +6356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A2291D0-3C09-0C45-8CBB-DD5A881036D5}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added breaker acceleration notebook
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87B4738-E468-DD41-B191-312CED6A1A0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC0B429-3DED-9048-A1F0-CB7B0344F4EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="263">
   <si>
     <t>Mission Number</t>
   </si>
@@ -823,6 +823,18 @@
   </si>
   <si>
     <t>SOMEWHERE IN ARCTIC</t>
+  </si>
+  <si>
+    <t>40,57</t>
+  </si>
+  <si>
+    <t>2021-10-22T14:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T15:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-22T16:00:00</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1105,57 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <u val="none"/>
@@ -1618,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="M26" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView topLeftCell="G43" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4625,8 +4687,10 @@
       <c r="T52" s="1"/>
       <c r="U52" s="4"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
+    <row r="53" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -4639,17 +4703,27 @@
       <c r="K53" s="1"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
+      <c r="N53" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="P53" s="4"/>
-      <c r="Q53" s="1"/>
-      <c r="R53" s="1"/>
+      <c r="Q53" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="R53" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="S53" s="4"/>
       <c r="T53" s="1"/>
       <c r="U53" s="4"/>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
+    <row r="54" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -4662,11 +4736,19 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
+      <c r="N54" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>259</v>
+      </c>
       <c r="P54" s="1"/>
-      <c r="Q54" s="1"/>
-      <c r="R54" s="1"/>
+      <c r="Q54" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="R54" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="S54" s="4"/>
       <c r="T54" s="1"/>
       <c r="U54" s="4"/>
@@ -5156,32 +5238,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
-    <cfRule type="containsBlanks" dxfId="13" priority="12">
+    <cfRule type="containsBlanks" dxfId="15" priority="12">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="6">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="11" priority="4">
+    <cfRule type="containsBlanks" dxfId="13" priority="4">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="3">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="9" priority="2">
+    <cfRule type="containsBlanks" dxfId="11" priority="2">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="1">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5194,7 +5276,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5535,14 +5617,24 @@
       <c r="B11" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="L11" s="10" t="s">
@@ -5659,16 +5751,16 @@
       <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="C15" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
       <c r="L15" s="22" t="s">
         <v>75</v>
       </c>
@@ -5952,16 +6044,16 @@
       <c r="B25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="C25" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
       <c r="L25" s="22" t="s">
         <v>75</v>
       </c>
@@ -7011,9 +7103,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
     <mergeCell ref="C53:J53"/>
     <mergeCell ref="C55:J55"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C25:J25"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="B30:J30"/>
     <mergeCell ref="C47:J47"/>
@@ -7021,42 +7115,52 @@
     <mergeCell ref="C51:J51"/>
     <mergeCell ref="C52:J52"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:J5 B6:C6 K12 B7:J27 B30 B31:J46 B47 B29:J29 B28 B48:J50 B51:C51 B52:B53 B54:J54 B55 B56:J60">
-    <cfRule type="containsBlanks" dxfId="7" priority="10">
+  <conditionalFormatting sqref="B2:J5 B6:C6 K12 B30 B31:J46 B47 B29:J29 B28 B48:J50 B51:C51 B52:B53 B54:J54 B55 B56:J60 B16:J24 B15 B26:J27 B25 B7:J14">
+    <cfRule type="containsBlanks" dxfId="9" priority="12">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L60 B61:B66">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(C28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(C52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(C53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(C55))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(C15))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C55))=0</formula>
+      <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated notes to mission 56
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F13F36-0F5B-A640-BF38-F25618800241}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AC63FF-C994-7F47-B58D-9046AD9C7353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="301">
   <si>
     <t>Mission Number</t>
   </si>
@@ -901,6 +901,54 @@
   </si>
   <si>
     <t>2021-10-23T17:50:00</t>
+  </si>
+  <si>
+    <t>DUNEX-development</t>
+  </si>
+  <si>
+    <t>Jake Davis</t>
+  </si>
+  <si>
+    <t>2,3,4,5,7,10,12,13,14,16,17,18,19,20,21,23</t>
+  </si>
+  <si>
+    <t>1,2,3,4</t>
+  </si>
+  <si>
+    <t>2021-10-25T14:24:00</t>
+  </si>
+  <si>
+    <t>2021-10-25T14:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-25T15:13:00</t>
+  </si>
+  <si>
+    <t>2021-10-25T15:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-25T18:24:00</t>
+  </si>
+  <si>
+    <t>dead at the moment - need to check connectors</t>
+  </si>
+  <si>
+    <t>started picking up buoys at 10:38 ET - picked up at before the next burst</t>
+  </si>
+  <si>
+    <t>4 of the micros remained out from the previous mission 54 which are the ones that look like they started far on the north side of the pier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offshore buoys pickedup by paddlers then thehy paddled north and headed into the beach - many of the other micros were caught in a convergence zone in the surfzone </t>
+  </si>
+  <si>
+    <t>2021-10-25T17:10:00</t>
+  </si>
+  <si>
+    <t>missing IMU data starting at mission 54</t>
+  </si>
+  <si>
+    <t>No devices and printing out i2cdetect result weird</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1164,206 +1212,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <u val="none"/>
@@ -1597,31 +1453,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <fill>
@@ -1963,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="M38" workbookViewId="0">
-      <selection activeCell="R56" sqref="R56"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5431,72 +5262,186 @@
       <c r="T55" s="1"/>
       <c r="U55" s="4"/>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
-      <c r="N56" s="4"/>
-      <c r="O56" s="4"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
-      <c r="S56" s="4"/>
+    <row r="56" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C56" s="1">
+        <v>7</v>
+      </c>
+      <c r="D56" s="1">
+        <v>100</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L56" s="1">
+        <v>16</v>
+      </c>
+      <c r="M56" s="1">
+        <v>4</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P56" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="R56" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="S56" s="4" t="s">
+        <v>295</v>
+      </c>
       <c r="T56" s="1"/>
       <c r="U56" s="4"/>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="4"/>
-      <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
-      <c r="O57" s="4"/>
-      <c r="P57" s="4"/>
-      <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
-      <c r="S57" s="4"/>
+    <row r="57" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C57" s="1">
+        <v>7</v>
+      </c>
+      <c r="D57" s="1">
+        <v>100</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L57" s="1">
+        <v>16</v>
+      </c>
+      <c r="M57" s="1">
+        <v>4</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P57" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="R57" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="S57" s="4" t="s">
+        <v>296</v>
+      </c>
       <c r="T57" s="1"/>
       <c r="U57" s="4"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="4"/>
+    <row r="58" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C58" s="1">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1">
+        <v>100</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L58" s="1">
+        <v>16</v>
+      </c>
+      <c r="M58" s="1">
+        <v>4</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P58" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="R58" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="S58" s="4" t="s">
+        <v>297</v>
+      </c>
       <c r="T58" s="1"/>
       <c r="U58" s="4"/>
     </row>
@@ -5892,33 +5837,33 @@
       <c r="U75" s="4"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A59:U75 A58:Q58 S58:U58">
+    <cfRule type="containsBlanks" dxfId="2" priority="12">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U75">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="6">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A59:U75 A58:Q58 S58:U58">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="6">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="25" priority="4">
+    <cfRule type="containsBlanks" dxfId="15" priority="4">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="24" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="3">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="23" priority="2">
+    <cfRule type="containsBlanks" dxfId="13" priority="2">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="22" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5931,7 +5876,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5940,7 +5885,8 @@
     <col min="2" max="2" width="26.33203125" customWidth="1"/>
     <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="6" max="6" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
@@ -5998,7 +5944,7 @@
         <v>16</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>16</v>
@@ -6029,7 +5975,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>16</v>
@@ -6060,7 +6006,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>16</v>
@@ -6091,24 +6037,27 @@
         <v>16</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>16</v>
+      <c r="F5" s="16" t="s">
+        <v>300</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>16</v>
+      <c r="H5" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
+      <c r="K5" s="25" t="s">
+        <v>299</v>
+      </c>
       <c r="L5" s="10" t="s">
-        <v>244</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -6143,7 +6092,7 @@
         <v>16</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>16</v>
@@ -6174,7 +6123,7 @@
         <v>16</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>16</v>
@@ -6182,8 +6131,8 @@
       <c r="F8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>16</v>
+      <c r="G8" s="16" t="s">
+        <v>74</v>
       </c>
       <c r="H8" s="13" t="s">
         <v>16</v>
@@ -6191,7 +6140,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
       <c r="L8" s="10" t="s">
-        <v>244</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -6239,7 +6188,7 @@
         <v>16</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>16</v>
@@ -6270,7 +6219,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>16</v>
@@ -6302,7 +6251,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>16</v>
@@ -6336,7 +6285,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>16</v>
@@ -6369,7 +6318,7 @@
         <v>16</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>16</v>
@@ -6423,7 +6372,7 @@
         <v>16</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>16</v>
@@ -6454,7 +6403,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>16</v>
@@ -6485,7 +6434,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>16</v>
@@ -6518,7 +6467,7 @@
         <v>16</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>16</v>
@@ -6551,7 +6500,7 @@
         <v>16</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>16</v>
@@ -6584,7 +6533,7 @@
         <v>16</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>16</v>
@@ -6648,7 +6597,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>16</v>
@@ -6679,7 +6628,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>16</v>
@@ -6733,7 +6682,7 @@
         <v>16</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>16</v>
@@ -6766,7 +6715,7 @@
         <v>16</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>16</v>
@@ -6820,7 +6769,7 @@
         <v>16</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E29" s="13" t="s">
         <v>16</v>
@@ -6872,7 +6821,7 @@
         <v>16</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>16</v>
@@ -6939,7 +6888,7 @@
         <v>16</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>16</v>
@@ -6972,7 +6921,7 @@
         <v>16</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>16</v>
@@ -7005,7 +6954,7 @@
         <v>16</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>16</v>
@@ -7038,7 +6987,7 @@
         <v>16</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>16</v>
@@ -7071,7 +7020,7 @@
         <v>16</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>16</v>
@@ -7104,7 +7053,7 @@
         <v>16</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>16</v>
@@ -7137,7 +7086,7 @@
         <v>16</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>73</v>
+        <v>285</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>16</v>
@@ -7170,7 +7119,7 @@
         <v>16</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>16</v>
@@ -7203,7 +7152,7 @@
         <v>16</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>16</v>
@@ -7269,7 +7218,7 @@
         <v>16</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>16</v>
@@ -7335,7 +7284,7 @@
         <v>16</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>16</v>
@@ -7368,7 +7317,7 @@
         <v>16</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>16</v>
@@ -7386,8 +7335,11 @@
         <v>16</v>
       </c>
       <c r="J46" s="13"/>
+      <c r="K46" s="12" t="s">
+        <v>294</v>
+      </c>
       <c r="L46" s="18" t="s">
-        <v>244</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -7422,7 +7374,7 @@
         <v>16</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>16</v>
@@ -7453,7 +7405,7 @@
         <v>16</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>16</v>
@@ -7486,7 +7438,7 @@
         <v>16</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>16</v>
@@ -7574,7 +7526,7 @@
         <v>16</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>16</v>
@@ -7626,7 +7578,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E56" s="13" t="s">
         <v>16</v>
@@ -7659,7 +7611,7 @@
         <v>16</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>16</v>
@@ -7692,7 +7644,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E58" s="13" t="s">
         <v>16</v>
@@ -7723,7 +7675,7 @@
         <v>16</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E59" s="13" t="s">
         <v>16</v>
@@ -7756,7 +7708,7 @@
         <v>16</v>
       </c>
       <c r="D60" s="13" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="E60" s="13" t="s">
         <v>16</v>
@@ -7791,51 +7743,51 @@
     <mergeCell ref="B53:J53"/>
     <mergeCell ref="B55:J55"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:J5 B6:C6 B30 B47 B29:J29 B28 B51 B54:J54 B15 B26:J27 B25 B48:J50 B56:J60 B31:J46 B16:J24 B7:J14">
-    <cfRule type="containsBlanks" dxfId="21" priority="12">
+  <conditionalFormatting sqref="B6:C6 B30 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5">
+    <cfRule type="containsBlanks" dxfId="0" priority="12">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L60 B61:B66">
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="18" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsBlanks" dxfId="17" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(C28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsBlanks" dxfId="16" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(B52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsBlanks" dxfId="15" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(B53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsBlanks" dxfId="14" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(B55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsBlanks" dxfId="13" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(C15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsBlanks" dxfId="12" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated notes and accel exploration
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AC63FF-C994-7F47-B58D-9046AD9C7353}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227AE275-186E-634D-B4FF-E21B66670A70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -1794,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5875,8 +5875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added up to mission 64
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680F3933-5992-7A4A-81A4-359FB580E9F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF971EEF-4449-424B-B659-A24B558B2DA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" activeTab="1" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1347" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="330">
   <si>
     <t>Mission Number</t>
   </si>
@@ -991,6 +991,51 @@
   </si>
   <si>
     <t>one alongshore line and cluster offshore</t>
+  </si>
+  <si>
+    <t>56,57,60,36,30,45,71,58</t>
+  </si>
+  <si>
+    <t>2021-10-27T14:30:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T14:50:00</t>
+  </si>
+  <si>
+    <t>31,33,34,35,37,38,40,41</t>
+  </si>
+  <si>
+    <t>2021-10-27T15:16:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T15:20:00</t>
+  </si>
+  <si>
+    <t>3,12,13,16,17,18,19,20,21,23,24,26,27,29,31,33,34,35,37,38,40,41,42,43,48,49,50,59,72,73</t>
+  </si>
+  <si>
+    <t>2021-10-27T15:32:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T15:48:00</t>
+  </si>
+  <si>
+    <t>3,71,73,56,72,59,60,10,58,57,12,13,16,17,18,20,21,23,24,26,27,29,30,31,33,34,35,36,37,38,40,41,42,43,45,48,49,50</t>
+  </si>
+  <si>
+    <t>2021-10-27T16:10:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T16:35:00</t>
+  </si>
+  <si>
+    <t>3,56,57,58,59,60,71,72,73,10,12,13,16,17,18,20,21,23,24,26,27,29,30,31,33,34,35,36,37,38,40,41,42,43,45,48,49,50</t>
+  </si>
+  <si>
+    <t>2021-10-27T16:29:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T16:39:00</t>
   </si>
 </sst>
 </file>
@@ -2150,8 +2195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U75"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="L47" workbookViewId="0">
+      <selection activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5985,8 +6030,10 @@
       <c r="T61" s="1"/>
       <c r="U61" s="4"/>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
+    <row r="62" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -5999,17 +6046,27 @@
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="N62" s="4"/>
-      <c r="O62" s="4"/>
+      <c r="N62" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+      <c r="Q62" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="R62" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="S62" s="4"/>
       <c r="T62" s="1"/>
       <c r="U62" s="4"/>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
+    <row r="63" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
@@ -6022,17 +6079,27 @@
       <c r="K63" s="1"/>
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
-      <c r="N63" s="4"/>
-      <c r="O63" s="4"/>
+      <c r="N63" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>318</v>
+      </c>
       <c r="P63" s="4"/>
-      <c r="Q63" s="1"/>
-      <c r="R63" s="1"/>
+      <c r="Q63" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="R63" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="S63" s="4"/>
       <c r="T63" s="1"/>
       <c r="U63" s="4"/>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
+    <row r="64" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -6045,17 +6112,27 @@
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
-      <c r="N64" s="4"/>
-      <c r="O64" s="4"/>
+      <c r="N64" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>321</v>
+      </c>
       <c r="P64" s="1"/>
-      <c r="Q64" s="1"/>
-      <c r="R64" s="1"/>
+      <c r="Q64" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="S64" s="4"/>
       <c r="T64" s="1"/>
       <c r="U64" s="4"/>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
+    <row r="65" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -6068,17 +6145,27 @@
       <c r="K65" s="1"/>
       <c r="L65" s="4"/>
       <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
+      <c r="N65" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>324</v>
+      </c>
       <c r="P65" s="4"/>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="1"/>
+      <c r="Q65" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="R65" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="S65" s="4"/>
       <c r="T65" s="1"/>
       <c r="U65" s="4"/>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
+    <row r="66" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -6091,11 +6178,19 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
-      <c r="N66" s="4"/>
-      <c r="O66" s="4"/>
+      <c r="N66" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>327</v>
+      </c>
       <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
+      <c r="Q66" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="R66" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="S66" s="4"/>
       <c r="T66" s="1"/>
       <c r="U66" s="4"/>
@@ -6346,8 +6441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBC2C10-2C0F-BE4E-B55B-FB92E38AA170}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated notes to mission 73
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF971EEF-4449-424B-B659-A24B558B2DA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ACAC22-22D2-4445-A43F-14DE9BC68C6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="372">
   <si>
     <t>Mission Number</t>
   </si>
@@ -1032,10 +1032,136 @@
     <t>3,56,57,58,59,60,71,72,73,10,12,13,16,17,18,20,21,23,24,26,27,29,30,31,33,34,35,36,37,38,40,41,42,43,45,48,49,50</t>
   </si>
   <si>
-    <t>2021-10-27T16:29:00</t>
-  </si>
-  <si>
-    <t>2021-10-27T16:39:00</t>
+    <t>3,64,61,71,59,66,62,60,72,73,10,12,16,19,21,23,24,29,30,34,35,36,37,38,45,48,50</t>
+  </si>
+  <si>
+    <t>2021-10-28T14:02:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T14:13:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T14:27:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T14:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T15:30:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T16:20:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T17:05:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T17:30:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T17:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T17:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T18:04:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T18:20:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T18:28:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T18:50:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T19:10:00</t>
+  </si>
+  <si>
+    <t>2021-10-28T19:30:00</t>
+  </si>
+  <si>
+    <t>43,33,42,40,41,49,57,58,3,64,61,71,59,66,62,60,72,73,10,12,16,19,23,24,29,30,34,35,36,37,38,45,48,50</t>
+  </si>
+  <si>
+    <t>2021-10-27T18:00:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T18:14:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T18:29:00</t>
+  </si>
+  <si>
+    <t>2021-10-27T18:39:00</t>
+  </si>
+  <si>
+    <t>Helicopter</t>
+  </si>
+  <si>
+    <t>alongshore line on north side of pier</t>
+  </si>
+  <si>
+    <t>close clusters</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>pier drop</t>
+  </si>
+  <si>
+    <t>cluster</t>
+  </si>
+  <si>
+    <t>cross shore line</t>
+  </si>
+  <si>
+    <t>Helicopter and Pier Drop</t>
+  </si>
+  <si>
+    <t>alongshore line on north side and cross shore line from the pier</t>
+  </si>
+  <si>
+    <t>4,5,6,7,8</t>
+  </si>
+  <si>
+    <t>2,3,4,5,6,7,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Number of buoys deployed </t>
+  </si>
+  <si>
+    <t>shep 8 was the last to be dropped - good break on a bunch at 11:33 local</t>
+  </si>
+  <si>
+    <t>3 of them picked up and brought to shore</t>
+  </si>
+  <si>
+    <t>have location of gator for video rectification</t>
+  </si>
+  <si>
+    <t>43,33,42,40,41,49,57,58 were all dropped from helicopter with chutes rest were dropped from pier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took out 72 since the swing arm fell off - board is ok </t>
+  </si>
+  <si>
+    <t>Same batch as 70</t>
+  </si>
+  <si>
+    <t>same as 70 except for 36 and 71 since they had water damage</t>
+  </si>
+  <si>
+    <t>3,64,61,71,59,66,62,60,72,73,10,12,16,19,23,24,29,30,34,35,36,37,38,45,48,50,43,33,42,40,41,49,57,58</t>
+  </si>
+  <si>
+    <t>3,64,61,71,59,66,62,60,73,10,12,16,19,23,24,29,30,34,35,36,37,38,45,48,50,43,33,42,40,41,49,57,58</t>
+  </si>
+  <si>
+    <t>3,64,61,59,66,62,60,73,10,12,16,19,23,24,29,30,34,35,37,38,45,48,50,43,33,42,40,41,49,57,58</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1311,15 +1437,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="36">
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1327,39 +1456,39 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -2193,10 +2322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L47" workbookViewId="0">
-      <selection activeCell="S66" sqref="S66"/>
+    <sheetView tabSelected="1" topLeftCell="G66" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6034,32 +6163,60 @@
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
+      <c r="B62" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C62" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D62" s="1">
+        <v>34</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L62" s="1">
+        <v>8</v>
+      </c>
+      <c r="M62" s="1">
+        <v>2</v>
+      </c>
       <c r="N62" s="4" t="s">
         <v>315</v>
       </c>
       <c r="O62" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="P62" s="1"/>
+      <c r="P62" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="Q62" s="1" t="s">
         <v>316</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="S62" s="4"/>
+      <c r="S62" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T62" s="1"/>
       <c r="U62" s="4"/>
     </row>
@@ -6067,32 +6224,60 @@
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="L63" s="4"/>
-      <c r="M63" s="4"/>
+      <c r="B63" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C63" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D63" s="1">
+        <v>34</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L63" s="4">
+        <v>8</v>
+      </c>
+      <c r="M63" s="4">
+        <v>2</v>
+      </c>
       <c r="N63" s="4" t="s">
         <v>318</v>
       </c>
       <c r="O63" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="P63" s="4"/>
+      <c r="P63" s="4" t="s">
+        <v>353</v>
+      </c>
       <c r="Q63" s="1" t="s">
         <v>319</v>
       </c>
       <c r="R63" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="S63" s="4"/>
+      <c r="S63" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T63" s="1"/>
       <c r="U63" s="4"/>
     </row>
@@ -6100,32 +6285,60 @@
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="L64" s="1"/>
-      <c r="M64" s="1"/>
+      <c r="B64" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C64" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D64" s="1">
+        <v>34</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L64" s="1">
+        <v>30</v>
+      </c>
+      <c r="M64" s="1">
+        <v>5</v>
+      </c>
       <c r="N64" s="4" t="s">
         <v>321</v>
       </c>
       <c r="O64" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="P64" s="1"/>
+      <c r="P64" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="Q64" s="1" t="s">
         <v>322</v>
       </c>
       <c r="R64" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="S64" s="4"/>
+      <c r="S64" s="4" t="s">
+        <v>362</v>
+      </c>
       <c r="T64" s="1"/>
       <c r="U64" s="4"/>
     </row>
@@ -6133,32 +6346,60 @@
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
+      <c r="B65" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D65" s="1">
+        <v>34</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L65" s="4">
+        <v>38</v>
+      </c>
+      <c r="M65" s="4">
+        <v>7</v>
+      </c>
       <c r="N65" s="4" t="s">
         <v>324</v>
       </c>
       <c r="O65" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="P65" s="4"/>
+      <c r="P65" s="4" t="s">
+        <v>360</v>
+      </c>
       <c r="Q65" s="1" t="s">
         <v>325</v>
       </c>
       <c r="R65" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="S65" s="4"/>
+      <c r="S65" s="4" t="s">
+        <v>363</v>
+      </c>
       <c r="T65" s="1"/>
       <c r="U65" s="4"/>
     </row>
@@ -6166,271 +6407,973 @@
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
-      <c r="N66" s="4" t="s">
+      <c r="B66" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C66" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D66" s="1">
+        <v>34</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L66" s="1">
+        <v>38</v>
+      </c>
+      <c r="M66" s="1">
+        <v>7</v>
+      </c>
+      <c r="N66" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="O66" s="4" t="s">
+      <c r="O66" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="R66" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="S66" s="4"/>
+      <c r="P66" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q66" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="R66" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="S66" s="4" t="s">
+        <v>364</v>
+      </c>
       <c r="T66" s="1"/>
       <c r="U66" s="4"/>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="4"/>
-      <c r="M67" s="4"/>
-      <c r="N67" s="4"/>
-      <c r="O67" s="4"/>
-      <c r="P67" s="4"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="4"/>
+    <row r="67" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C67" s="1">
+        <v>6.25</v>
+      </c>
+      <c r="D67" s="1">
+        <v>34</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K67" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L67" s="4">
+        <v>38</v>
+      </c>
+      <c r="M67" s="4">
+        <v>7</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="O67" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="P67" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="S67" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T67" s="1"/>
       <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="L68" s="1"/>
-      <c r="M68" s="1"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
-      <c r="S68" s="4"/>
+    <row r="68" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C68" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D68" s="1">
+        <v>73</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K68" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L68" s="1">
+        <v>27</v>
+      </c>
+      <c r="M68" s="1">
+        <v>5</v>
+      </c>
+      <c r="N68" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="O68" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="P68" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="R68" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="S68" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T68" s="1"/>
       <c r="U68" s="4"/>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="L69" s="4"/>
-      <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
-      <c r="O69" s="4"/>
-      <c r="P69" s="4"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="4"/>
+    <row r="69" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C69" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D69" s="1">
+        <v>73</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L69" s="4">
+        <v>27</v>
+      </c>
+      <c r="M69" s="4">
+        <v>5</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="P69" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q69" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="R69" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="S69" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T69" s="1"/>
       <c r="U69" s="4"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="1"/>
-      <c r="Q70" s="1"/>
-      <c r="R70" s="1"/>
-      <c r="S70" s="4"/>
+    <row r="70" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C70" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D70" s="1">
+        <v>73</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K70" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L70" s="1">
+        <v>34</v>
+      </c>
+      <c r="M70" s="1">
+        <v>7</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="O70" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="P70" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="R70" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="S70" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="T70" s="1"/>
       <c r="U70" s="4"/>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="L71" s="4"/>
-      <c r="M71" s="4"/>
-      <c r="N71" s="4"/>
-      <c r="O71" s="4"/>
-      <c r="P71" s="4"/>
-      <c r="Q71" s="1"/>
-      <c r="R71" s="1"/>
-      <c r="S71" s="4"/>
+    <row r="71" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C71" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D71" s="1">
+        <v>73</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L71" s="4">
+        <v>34</v>
+      </c>
+      <c r="M71" s="4">
+        <v>7</v>
+      </c>
+      <c r="N71" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="O71" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="P71" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q71" s="29" t="s">
+        <v>335</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="S71" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T71" s="1"/>
       <c r="U71" s="4"/>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="L72" s="1"/>
-      <c r="M72" s="1"/>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1"/>
-      <c r="R72" s="1"/>
-      <c r="S72" s="4"/>
+    <row r="72" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C72" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D72" s="1">
+        <v>73</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K72" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L72" s="1">
+        <v>34</v>
+      </c>
+      <c r="M72" s="1">
+        <v>7</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="P72" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="S72" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="T72" s="1"/>
       <c r="U72" s="4"/>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="1"/>
-      <c r="S73" s="4"/>
+    <row r="73" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C73" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D73" s="1">
+        <v>73</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K73" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L73" s="4">
+        <v>33</v>
+      </c>
+      <c r="M73" s="4">
+        <v>7</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="O73" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="P73" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="S73" s="4" t="s">
+        <v>366</v>
+      </c>
       <c r="T73" s="1"/>
       <c r="U73" s="4"/>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
-      <c r="N74" s="4"/>
-      <c r="O74" s="4"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
-      <c r="S74" s="4"/>
+    <row r="74" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C74" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D74" s="1">
+        <v>73</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K74" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L74" s="1">
+        <v>33</v>
+      </c>
+      <c r="M74" s="1">
+        <v>7</v>
+      </c>
+      <c r="N74" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="O74" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="S74" s="4" t="s">
+        <v>367</v>
+      </c>
       <c r="T74" s="1"/>
       <c r="U74" s="4"/>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-      <c r="Q75" s="1"/>
-      <c r="R75" s="1"/>
-      <c r="S75" s="4"/>
+    <row r="75" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="C75" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="D75" s="1">
+        <v>73</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K75" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L75" s="4">
+        <v>31</v>
+      </c>
+      <c r="M75" s="4">
+        <v>7</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="P75" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="S75" s="4" t="s">
+        <v>368</v>
+      </c>
       <c r="T75" s="1"/>
       <c r="U75" s="4"/>
     </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="J76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="4"/>
+      <c r="M76" s="4"/>
+      <c r="N76" s="4"/>
+      <c r="O76" s="4"/>
+      <c r="P76" s="4"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="1"/>
+      <c r="S76" s="4"/>
+      <c r="T76" s="1"/>
+      <c r="U76" s="4"/>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="J77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="1"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="1"/>
+      <c r="U77" s="4"/>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="J78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="4"/>
+      <c r="M78" s="4"/>
+      <c r="N78" s="4"/>
+      <c r="O78" s="4"/>
+      <c r="P78" s="4"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+      <c r="S78" s="4"/>
+      <c r="T78" s="1"/>
+      <c r="U78" s="4"/>
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="4"/>
+      <c r="M79" s="4"/>
+      <c r="N79" s="4"/>
+      <c r="O79" s="4"/>
+      <c r="P79" s="4"/>
+      <c r="Q79" s="1"/>
+      <c r="R79" s="1"/>
+      <c r="S79" s="4"/>
+      <c r="T79" s="1"/>
+      <c r="U79" s="4"/>
+    </row>
+    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="J80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="4"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="4"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="4"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="1"/>
+      <c r="S80" s="4"/>
+      <c r="T80" s="1"/>
+      <c r="U80" s="4"/>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+      <c r="I81" s="1"/>
+      <c r="J81" s="1"/>
+      <c r="K81" s="1"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
+      <c r="O81" s="4"/>
+      <c r="P81" s="4"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="1"/>
+      <c r="S81" s="4"/>
+      <c r="T81" s="1"/>
+      <c r="U81" s="4"/>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="4"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="4"/>
+      <c r="Q82" s="1"/>
+      <c r="R82" s="1"/>
+      <c r="S82" s="4"/>
+      <c r="T82" s="1"/>
+      <c r="U82" s="4"/>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1"/>
+      <c r="H83" s="1"/>
+      <c r="I83" s="1"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+      <c r="N83" s="4"/>
+      <c r="O83" s="4"/>
+      <c r="P83" s="4"/>
+      <c r="Q83" s="1"/>
+      <c r="R83" s="1"/>
+      <c r="S83" s="4"/>
+      <c r="T83" s="1"/>
+      <c r="U83" s="4"/>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
+      <c r="H84" s="1"/>
+      <c r="I84" s="1"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="4"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="4"/>
+      <c r="Q84" s="1"/>
+      <c r="R84" s="1"/>
+      <c r="S84" s="4"/>
+      <c r="T84" s="1"/>
+      <c r="U84" s="4"/>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
+      <c r="H85" s="1"/>
+      <c r="I85" s="1"/>
+      <c r="J85" s="1"/>
+      <c r="K85" s="1"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="1"/>
+      <c r="R85" s="1"/>
+      <c r="S85" s="4"/>
+      <c r="T85" s="1"/>
+      <c r="U85" s="4"/>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
+      <c r="H86" s="1"/>
+      <c r="I86" s="1"/>
+      <c r="J86" s="1"/>
+      <c r="K86" s="1"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="1"/>
+      <c r="R86" s="1"/>
+      <c r="S86" s="4"/>
+      <c r="T86" s="1"/>
+      <c r="U86" s="4"/>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1"/>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="1"/>
+      <c r="R87" s="1"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="1"/>
+      <c r="U87" s="4"/>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>361</v>
+      </c>
+      <c r="B89">
+        <f>SUM(L2:M87)</f>
+        <v>1851</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A59:U75">
-    <cfRule type="containsBlanks" dxfId="32" priority="12">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A88 S66:U66 Q66 A59:U65 A66:N66 B76:U87 B67:J75 L67:U75">
+    <cfRule type="containsBlanks" dxfId="35" priority="42">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A59:U75">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="6">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A88 S66:U66 Q66 A59:U65 A66:N66 B76:U87 B67:J75 L67:U75">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="36">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="30" priority="4">
+    <cfRule type="containsBlanks" dxfId="33" priority="34">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="29" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="28" priority="2">
+    <cfRule type="containsBlanks" dxfId="31" priority="32">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
       <formula>LEN(TRIM(O36))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O66">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(O66))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O66">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(O66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R66">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(R66))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R66">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(R66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P66">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(P66))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P66">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(P66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8417,114 +9360,114 @@
     <mergeCell ref="B55:J55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C6 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5 K36 B30">
-    <cfRule type="containsBlanks" dxfId="26" priority="29">
+    <cfRule type="containsBlanks" dxfId="29" priority="29">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L60 B64:B65">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="23" priority="24">
+    <cfRule type="containsBlanks" dxfId="26" priority="24">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsBlanks" dxfId="22" priority="23">
+    <cfRule type="containsBlanks" dxfId="25" priority="23">
       <formula>LEN(TRIM(C28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsBlanks" dxfId="21" priority="22">
+    <cfRule type="containsBlanks" dxfId="24" priority="22">
       <formula>LEN(TRIM(B52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsBlanks" dxfId="20" priority="21">
+    <cfRule type="containsBlanks" dxfId="23" priority="21">
       <formula>LEN(TRIM(B53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsBlanks" dxfId="19" priority="20">
+    <cfRule type="containsBlanks" dxfId="22" priority="20">
       <formula>LEN(TRIM(B55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsBlanks" dxfId="18" priority="19">
+    <cfRule type="containsBlanks" dxfId="21" priority="19">
       <formula>LEN(TRIM(C15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsBlanks" dxfId="17" priority="18">
+    <cfRule type="containsBlanks" dxfId="20" priority="18">
       <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsBlanks" dxfId="16" priority="17">
+    <cfRule type="containsBlanks" dxfId="19" priority="17">
       <formula>LEN(TRIM(C30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="15" priority="16">
+    <cfRule type="containsBlanks" dxfId="18" priority="16">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="14" priority="15">
+    <cfRule type="containsBlanks" dxfId="17" priority="15">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="containsBlanks" dxfId="13" priority="14">
+    <cfRule type="containsBlanks" dxfId="16" priority="14">
       <formula>LEN(TRIM(G30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="12" priority="13">
+    <cfRule type="containsBlanks" dxfId="15" priority="13">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:J61">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="14" priority="12">
       <formula>LEN(TRIM(B61))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L61">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:J62">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(B62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:J63">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(B63))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
DUNEX Notes Sheet complete at Mission 81
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ACAC22-22D2-4445-A43F-14DE9BC68C6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B35D1D8-6D0F-6343-92FC-2D75613CA84A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="395">
   <si>
     <t>Mission Number</t>
   </si>
@@ -1162,6 +1162,75 @@
   </si>
   <si>
     <t>3,64,61,59,66,62,60,73,10,12,16,19,23,24,29,30,34,35,37,38,45,48,50,43,33,42,40,41,49,57,58</t>
+  </si>
+  <si>
+    <t>59,58,76,66,73,10,3,54,12,15,18,19,23,24,26,30,29,33,34,35,37,40,41,42,43,45,48,50,60,62,38</t>
+  </si>
+  <si>
+    <t>2,4,5,7,8</t>
+  </si>
+  <si>
+    <t>2021-10-29T12:12:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T12:40:00</t>
+  </si>
+  <si>
+    <t>dropped from north side of pier</t>
+  </si>
+  <si>
+    <t>7,2,8,4</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:02:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:20:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:28:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T13:44:00</t>
+  </si>
+  <si>
+    <t>Dropped from north side of pier</t>
+  </si>
+  <si>
+    <t>64,72,78,61,49,16,57,75,10,50,66,15,73,60,40,29,19,48,26,23,30,3,45,43,33,62,34,24,18,42,41,12,54,58,59,37,35,38,76</t>
+  </si>
+  <si>
+    <t>2021-10-29T14:02:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T14:18:00</t>
+  </si>
+  <si>
+    <t>Awesome last deployment - super rainy and so much fun!</t>
+  </si>
+  <si>
+    <t>2021-10-29T14:28:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T14:47:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T15:03:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T15:16:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T15:24:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T15:40:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T16:03:00</t>
+  </si>
+  <si>
+    <t>2021-10-29T16:25:00</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1516,91 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="52">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2012,6 +2165,34 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2322,10 +2503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:U84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G66" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView tabSelected="1" topLeftCell="P81" workbookViewId="0">
+      <selection activeCell="T83" sqref="T83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7013,367 +7194,642 @@
       <c r="T75" s="1"/>
       <c r="U75" s="4"/>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="L76" s="4"/>
-      <c r="M76" s="4"/>
-      <c r="N76" s="4"/>
-      <c r="O76" s="4"/>
-      <c r="P76" s="4"/>
-      <c r="Q76" s="1"/>
-      <c r="R76" s="1"/>
-      <c r="S76" s="4"/>
+      <c r="B76" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C76" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D76" s="1">
+        <v>102</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J76" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K76" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L76" s="4">
+        <v>31</v>
+      </c>
+      <c r="M76" s="4">
+        <v>5</v>
+      </c>
+      <c r="N76" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="P76" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="R76" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="S76" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="T76" s="1"/>
       <c r="U76" s="4"/>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="L77" s="4"/>
-      <c r="M77" s="4"/>
-      <c r="N77" s="4"/>
-      <c r="O77" s="4"/>
-      <c r="P77" s="4"/>
-      <c r="Q77" s="1"/>
-      <c r="R77" s="1"/>
-      <c r="S77" s="4"/>
+      <c r="B77" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C77" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D77" s="1">
+        <v>102</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K77" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L77" s="4">
+        <v>31</v>
+      </c>
+      <c r="M77" s="4">
+        <v>4</v>
+      </c>
+      <c r="N77" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="P77" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="R77" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="S77" s="4" t="s">
+        <v>376</v>
+      </c>
       <c r="T77" s="1"/>
       <c r="U77" s="4"/>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="L78" s="4"/>
-      <c r="M78" s="4"/>
-      <c r="N78" s="4"/>
-      <c r="O78" s="4"/>
-      <c r="P78" s="4"/>
-      <c r="Q78" s="1"/>
-      <c r="R78" s="1"/>
-      <c r="S78" s="4"/>
+      <c r="B78" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C78" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>102</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K78" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L78" s="4">
+        <v>31</v>
+      </c>
+      <c r="M78" s="4">
+        <v>4</v>
+      </c>
+      <c r="N78" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="P78" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="R78" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="S78" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="T78" s="1"/>
       <c r="U78" s="4"/>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="L79" s="4"/>
-      <c r="M79" s="4"/>
-      <c r="N79" s="4"/>
-      <c r="O79" s="4"/>
-      <c r="P79" s="4"/>
-      <c r="Q79" s="1"/>
-      <c r="R79" s="1"/>
-      <c r="S79" s="4"/>
+      <c r="B79" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C79" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D79" s="1">
+        <v>102</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J79" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K79" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L79" s="4">
+        <v>39</v>
+      </c>
+      <c r="M79" s="4">
+        <v>7</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="P79" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="S79" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="T79" s="1"/>
       <c r="U79" s="4"/>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4"/>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="1"/>
-      <c r="R80" s="1"/>
-      <c r="S80" s="4"/>
+      <c r="B80" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C80" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>102</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K80" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L80" s="4">
+        <v>39</v>
+      </c>
+      <c r="M80" s="4">
+        <v>7</v>
+      </c>
+      <c r="N80" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="P80" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="R80" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="S80" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="T80" s="1"/>
       <c r="U80" s="4"/>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4"/>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="1"/>
-      <c r="R81" s="1"/>
-      <c r="S81" s="4"/>
+      <c r="B81" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C81" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D81" s="1">
+        <v>102</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K81" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L81" s="4">
+        <v>39</v>
+      </c>
+      <c r="M81" s="4">
+        <v>7</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="P81" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="R81" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="S81" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="T81" s="1"/>
       <c r="U81" s="4"/>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:21" ht="68" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4"/>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
-      <c r="Q82" s="1"/>
-      <c r="R82" s="1"/>
-      <c r="S82" s="4"/>
+      <c r="B82" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C82" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D82" s="1">
+        <v>102</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K82" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L82" s="4">
+        <v>39</v>
+      </c>
+      <c r="M82" s="4">
+        <v>7</v>
+      </c>
+      <c r="N82" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="P82" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="S82" s="4" t="s">
+        <v>382</v>
+      </c>
       <c r="T82" s="1"/>
       <c r="U82" s="4"/>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4"/>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="1"/>
-      <c r="R83" s="1"/>
-      <c r="S83" s="4"/>
+    <row r="83" spans="1:21" ht="68" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="C83" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="D83" s="1">
+        <v>102</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J83" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="K83" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L83" s="4">
+        <v>39</v>
+      </c>
+      <c r="M83" s="4">
+        <v>7</v>
+      </c>
+      <c r="N83" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="P83" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="S83" s="4" t="s">
+        <v>386</v>
+      </c>
       <c r="T83" s="1"/>
       <c r="U83" s="4"/>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
-      <c r="N84" s="4"/>
-      <c r="O84" s="4"/>
-      <c r="P84" s="4"/>
-      <c r="Q84" s="1"/>
-      <c r="R84" s="1"/>
-      <c r="S84" s="4"/>
-      <c r="T84" s="1"/>
-      <c r="U84" s="4"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
-      <c r="N85" s="4"/>
-      <c r="O85" s="4"/>
-      <c r="P85" s="4"/>
-      <c r="Q85" s="1"/>
-      <c r="R85" s="1"/>
-      <c r="S85" s="4"/>
-      <c r="T85" s="1"/>
-      <c r="U85" s="4"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="1"/>
-      <c r="R86" s="1"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="1"/>
-      <c r="U86" s="4"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
-      <c r="O87" s="4"/>
-      <c r="P87" s="4"/>
-      <c r="Q87" s="1"/>
-      <c r="R87" s="1"/>
-      <c r="S87" s="4"/>
-      <c r="T87" s="1"/>
-      <c r="U87" s="4"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="A84" t="s">
         <v>361</v>
       </c>
-      <c r="B89">
-        <f>SUM(L2:M87)</f>
-        <v>1851</v>
+      <c r="B84">
+        <f>SUM(L2:M83)</f>
+        <v>2187</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A88 S66:U66 Q66 A59:U65 A66:N66 B76:U87 B67:J75 L67:U75">
-    <cfRule type="containsBlanks" dxfId="35" priority="42">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A83 S66:U66 Q66 A59:U65 A66:N66 B67:J75 L67:U83 B76:F83">
+    <cfRule type="containsBlanks" dxfId="17" priority="58">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A88 S66:U66 Q66 A59:U65 A66:N66 B76:U87 B67:J75 L67:U75">
-    <cfRule type="notContainsBlanks" dxfId="34" priority="36">
+  <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A83 S66:U66 Q66 A59:U65 A66:N66 B67:J75 L67:U83 B76:F83">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="52">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="33" priority="34">
+    <cfRule type="containsBlanks" dxfId="51" priority="50">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="32" priority="33">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="49">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="31" priority="32">
+    <cfRule type="containsBlanks" dxfId="49" priority="48">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="30" priority="31">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="47">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O66">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="47" priority="22">
       <formula>LEN(TRIM(O66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O66">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="21">
       <formula>LEN(TRIM(O66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R66">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="45" priority="20">
       <formula>LEN(TRIM(R66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R66">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="19">
       <formula>LEN(TRIM(R66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P66">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="43" priority="18">
       <formula>LEN(TRIM(P66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P66">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="17">
+      <formula>LEN(TRIM(P66))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G76:J76">
+    <cfRule type="containsBlanks" dxfId="15" priority="16">
+      <formula>LEN(TRIM(G76))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G76:J76">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(G76))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G77:J77">
+    <cfRule type="containsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(G77))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G77:J77">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(G77))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G78:J78">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
+      <formula>LEN(TRIM(G78))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G78:J78">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(G78))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G79:J79">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(G79))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G79:J79">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(G79))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G80:J80">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(G80))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G80:J80">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(G80))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G81:J81">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(G81))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G81:J81">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(G81))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G82:J82">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(G82))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G82:J82">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(G82))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G83:J83">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(G83))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G83:J83">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(P66))&gt;0</formula>
+      <formula>LEN(TRIM(G83))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9360,114 +9816,114 @@
     <mergeCell ref="B55:J55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C6 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5 K36 B30">
-    <cfRule type="containsBlanks" dxfId="29" priority="29">
+    <cfRule type="containsBlanks" dxfId="41" priority="29">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L60 B64:B65">
-    <cfRule type="cellIs" dxfId="28" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="25" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="26" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="26" priority="24">
+    <cfRule type="containsBlanks" dxfId="38" priority="24">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsBlanks" dxfId="25" priority="23">
+    <cfRule type="containsBlanks" dxfId="37" priority="23">
       <formula>LEN(TRIM(C28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsBlanks" dxfId="24" priority="22">
+    <cfRule type="containsBlanks" dxfId="36" priority="22">
       <formula>LEN(TRIM(B52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsBlanks" dxfId="23" priority="21">
+    <cfRule type="containsBlanks" dxfId="35" priority="21">
       <formula>LEN(TRIM(B53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsBlanks" dxfId="22" priority="20">
+    <cfRule type="containsBlanks" dxfId="34" priority="20">
       <formula>LEN(TRIM(B55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsBlanks" dxfId="21" priority="19">
+    <cfRule type="containsBlanks" dxfId="33" priority="19">
       <formula>LEN(TRIM(C15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsBlanks" dxfId="20" priority="18">
+    <cfRule type="containsBlanks" dxfId="32" priority="18">
       <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsBlanks" dxfId="19" priority="17">
+    <cfRule type="containsBlanks" dxfId="31" priority="17">
       <formula>LEN(TRIM(C30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="18" priority="16">
+    <cfRule type="containsBlanks" dxfId="30" priority="16">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="17" priority="15">
+    <cfRule type="containsBlanks" dxfId="29" priority="15">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="containsBlanks" dxfId="16" priority="14">
+    <cfRule type="containsBlanks" dxfId="28" priority="14">
       <formula>LEN(TRIM(G30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="15" priority="13">
+    <cfRule type="containsBlanks" dxfId="27" priority="13">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:J61">
-    <cfRule type="containsBlanks" dxfId="14" priority="12">
+    <cfRule type="containsBlanks" dxfId="26" priority="12">
       <formula>LEN(TRIM(B61))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L61">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:J62">
-    <cfRule type="containsBlanks" dxfId="11" priority="9">
+    <cfRule type="containsBlanks" dxfId="23" priority="9">
       <formula>LEN(TRIM(B62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:J63">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="20" priority="6">
       <formula>LEN(TRIM(B63))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
removed final throw number value since it was messing with the rest of the sheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,32 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEXdata/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B35D1D8-6D0F-6343-92FC-2D75613CA84A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC70F28D-8E7E-AC45-8B63-4834C3BAC72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="37480" windowHeight="18100" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="394">
   <si>
     <t>Mission Number</t>
   </si>
@@ -1129,9 +1138,6 @@
   </si>
   <si>
     <t>2,3,4,5,6,7,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total Number of buoys deployed </t>
   </si>
   <si>
     <t>shep 8 was the last to be dropped - good break on a bunch at 11:33 local</t>
@@ -1482,24 +1488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1512,137 +1500,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -2193,6 +2073,132 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2503,10 +2509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
-  <dimension ref="A1:U84"/>
+  <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P81" workbookViewId="0">
-      <selection activeCell="T83" sqref="T83"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6518,7 +6524,7 @@
         <v>323</v>
       </c>
       <c r="S64" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="T64" s="1"/>
       <c r="U64" s="4"/>
@@ -6579,7 +6585,7 @@
         <v>326</v>
       </c>
       <c r="S65" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="T65" s="1"/>
       <c r="U65" s="4"/>
@@ -6624,10 +6630,10 @@
       <c r="M66" s="1">
         <v>7</v>
       </c>
-      <c r="N66" s="30" t="s">
+      <c r="N66" s="24" t="s">
         <v>327</v>
       </c>
-      <c r="O66" s="30" t="s">
+      <c r="O66" s="24" t="s">
         <v>327</v>
       </c>
       <c r="P66" s="4" t="s">
@@ -6640,7 +6646,7 @@
         <v>347</v>
       </c>
       <c r="S66" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="T66" s="1"/>
       <c r="U66" s="4"/>
@@ -6884,7 +6890,7 @@
         <v>334</v>
       </c>
       <c r="S70" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="T70" s="1"/>
       <c r="U70" s="4"/>
@@ -6930,15 +6936,15 @@
         <v>7</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O71" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P71" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="Q71" s="29" t="s">
+      <c r="Q71" s="23" t="s">
         <v>335</v>
       </c>
       <c r="R71" s="1" t="s">
@@ -6991,10 +6997,10 @@
         <v>7</v>
       </c>
       <c r="N72" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="O72" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="P72" s="1" t="s">
         <v>360</v>
@@ -7052,10 +7058,10 @@
         <v>7</v>
       </c>
       <c r="N73" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P73" s="1" t="s">
         <v>360</v>
@@ -7067,7 +7073,7 @@
         <v>340</v>
       </c>
       <c r="S73" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="T73" s="1"/>
       <c r="U73" s="4"/>
@@ -7113,10 +7119,10 @@
         <v>7</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="O74" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="P74" s="1" t="s">
         <v>360</v>
@@ -7128,7 +7134,7 @@
         <v>342</v>
       </c>
       <c r="S74" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="T74" s="1"/>
       <c r="U74" s="4"/>
@@ -7174,10 +7180,10 @@
         <v>7</v>
       </c>
       <c r="N75" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="O75" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="P75" s="1" t="s">
         <v>360</v>
@@ -7189,7 +7195,7 @@
         <v>344</v>
       </c>
       <c r="S75" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="T75" s="1"/>
       <c r="U75" s="4"/>
@@ -7235,22 +7241,22 @@
         <v>5</v>
       </c>
       <c r="N76" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="P76" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="O76" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="P76" s="4" t="s">
+      <c r="Q76" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="Q76" s="1" t="s">
+      <c r="R76" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="R76" s="1" t="s">
+      <c r="S76" s="4" t="s">
         <v>375</v>
-      </c>
-      <c r="S76" s="4" t="s">
-        <v>376</v>
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="4"/>
@@ -7296,22 +7302,22 @@
         <v>4</v>
       </c>
       <c r="N77" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O77" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P77" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q77" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="Q77" s="1" t="s">
+      <c r="R77" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="R77" s="1" t="s">
-        <v>379</v>
-      </c>
       <c r="S77" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="T77" s="1"/>
       <c r="U77" s="4"/>
@@ -7357,22 +7363,22 @@
         <v>4</v>
       </c>
       <c r="N78" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P78" s="4" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="Q78" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="R78" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="R78" s="1" t="s">
+      <c r="S78" s="4" t="s">
         <v>381</v>
-      </c>
-      <c r="S78" s="4" t="s">
-        <v>382</v>
       </c>
       <c r="T78" s="1"/>
       <c r="U78" s="4"/>
@@ -7418,22 +7424,22 @@
         <v>7</v>
       </c>
       <c r="N79" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O79" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P79" s="4" t="s">
         <v>360</v>
       </c>
       <c r="Q79" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="R79" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="R79" s="1" t="s">
-        <v>385</v>
-      </c>
       <c r="S79" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T79" s="1"/>
       <c r="U79" s="4"/>
@@ -7479,22 +7485,22 @@
         <v>7</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P80" s="4" t="s">
         <v>360</v>
       </c>
       <c r="Q80" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="R80" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="R80" s="1" t="s">
-        <v>388</v>
-      </c>
       <c r="S80" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T80" s="1"/>
       <c r="U80" s="4"/>
@@ -7540,22 +7546,22 @@
         <v>7</v>
       </c>
       <c r="N81" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O81" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P81" s="4" t="s">
         <v>360</v>
       </c>
       <c r="Q81" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="R81" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="R81" s="1" t="s">
-        <v>390</v>
-      </c>
       <c r="S81" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T81" s="1"/>
       <c r="U81" s="4"/>
@@ -7601,22 +7607,22 @@
         <v>7</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P82" s="4" t="s">
         <v>360</v>
       </c>
       <c r="Q82" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="R82" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="R82" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="S82" s="4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T82" s="1"/>
       <c r="U82" s="4"/>
@@ -7662,173 +7668,164 @@
         <v>7</v>
       </c>
       <c r="N83" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="P83" s="4" t="s">
         <v>360</v>
       </c>
       <c r="Q83" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="R83" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="R83" s="1" t="s">
-        <v>394</v>
-      </c>
       <c r="S83" s="4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="T83" s="1"/>
       <c r="U83" s="4"/>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>361</v>
-      </c>
-      <c r="B84">
-        <f>SUM(L2:M83)</f>
-        <v>2187</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A83 S66:U66 Q66 A59:U65 A66:N66 B67:J75 L67:U83 B76:F83">
-    <cfRule type="containsBlanks" dxfId="17" priority="58">
+    <cfRule type="containsBlanks" dxfId="51" priority="58">
       <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:P21 A2:U18 S19:U21 A22:U28 S29:U30 A29:P30 A36:M36 A31:U35 P36:U36 A37:U57 A58:Q58 S58:U58 A67:A83 S66:U66 Q66 A59:U65 A66:N66 B67:J75 L67:U83 B76:F83">
-    <cfRule type="notContainsBlanks" dxfId="16" priority="52">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="52">
       <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="containsBlanks" dxfId="51" priority="50">
+    <cfRule type="containsBlanks" dxfId="49" priority="50">
       <formula>LEN(TRIM(N36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N36">
-    <cfRule type="notContainsBlanks" dxfId="50" priority="49">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="49">
       <formula>LEN(TRIM(N36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="containsBlanks" dxfId="49" priority="48">
+    <cfRule type="containsBlanks" dxfId="47" priority="48">
       <formula>LEN(TRIM(O36))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O36">
-    <cfRule type="notContainsBlanks" dxfId="48" priority="47">
+    <cfRule type="notContainsBlanks" dxfId="46" priority="47">
       <formula>LEN(TRIM(O36))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O66">
-    <cfRule type="containsBlanks" dxfId="47" priority="22">
+    <cfRule type="containsBlanks" dxfId="45" priority="22">
       <formula>LEN(TRIM(O66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O66">
-    <cfRule type="notContainsBlanks" dxfId="46" priority="21">
+    <cfRule type="notContainsBlanks" dxfId="44" priority="21">
       <formula>LEN(TRIM(O66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R66">
-    <cfRule type="containsBlanks" dxfId="45" priority="20">
+    <cfRule type="containsBlanks" dxfId="43" priority="20">
       <formula>LEN(TRIM(R66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R66">
-    <cfRule type="notContainsBlanks" dxfId="44" priority="19">
+    <cfRule type="notContainsBlanks" dxfId="42" priority="19">
       <formula>LEN(TRIM(R66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P66">
-    <cfRule type="containsBlanks" dxfId="43" priority="18">
+    <cfRule type="containsBlanks" dxfId="41" priority="18">
       <formula>LEN(TRIM(P66))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P66">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="17">
+    <cfRule type="notContainsBlanks" dxfId="40" priority="17">
       <formula>LEN(TRIM(P66))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76:J76">
-    <cfRule type="containsBlanks" dxfId="15" priority="16">
+    <cfRule type="containsBlanks" dxfId="39" priority="16">
       <formula>LEN(TRIM(G76))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G76:J76">
-    <cfRule type="notContainsBlanks" dxfId="14" priority="15">
+    <cfRule type="notContainsBlanks" dxfId="38" priority="15">
       <formula>LEN(TRIM(G76))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:J77">
-    <cfRule type="containsBlanks" dxfId="13" priority="14">
+    <cfRule type="containsBlanks" dxfId="37" priority="14">
       <formula>LEN(TRIM(G77))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G77:J77">
-    <cfRule type="notContainsBlanks" dxfId="12" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="36" priority="13">
       <formula>LEN(TRIM(G77))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78:J78">
-    <cfRule type="containsBlanks" dxfId="11" priority="12">
+    <cfRule type="containsBlanks" dxfId="35" priority="12">
       <formula>LEN(TRIM(G78))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G78:J78">
-    <cfRule type="notContainsBlanks" dxfId="10" priority="11">
+    <cfRule type="notContainsBlanks" dxfId="34" priority="11">
       <formula>LEN(TRIM(G78))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:J79">
-    <cfRule type="containsBlanks" dxfId="9" priority="10">
+    <cfRule type="containsBlanks" dxfId="33" priority="10">
       <formula>LEN(TRIM(G79))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G79:J79">
-    <cfRule type="notContainsBlanks" dxfId="8" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="32" priority="9">
       <formula>LEN(TRIM(G79))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:J80">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="31" priority="8">
       <formula>LEN(TRIM(G80))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G80:J80">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="7">
       <formula>LEN(TRIM(G80))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:J81">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="29" priority="6">
       <formula>LEN(TRIM(G81))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81:J81">
-    <cfRule type="notContainsBlanks" dxfId="4" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="5">
       <formula>LEN(TRIM(G81))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:J82">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="27" priority="4">
       <formula>LEN(TRIM(G82))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G82:J82">
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="3">
       <formula>LEN(TRIM(G82))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:J83">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="25" priority="2">
       <formula>LEN(TRIM(G83))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83:J83">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="1">
       <formula>LEN(TRIM(G83))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8018,7 +8015,7 @@
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="19" t="s">
         <v>298</v>
       </c>
       <c r="L5" s="10" t="s">
@@ -8032,16 +8029,16 @@
       <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
       <c r="L6" s="10" t="s">
         <v>73</v>
       </c>
@@ -8312,16 +8309,16 @@
       <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
       <c r="L15" s="18" t="s">
         <v>73</v>
       </c>
@@ -8622,16 +8619,16 @@
       <c r="B25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="24"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
       <c r="L25" s="18" t="s">
         <v>73</v>
       </c>
@@ -8709,16 +8706,16 @@
       <c r="B28" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
       <c r="L28" s="18" t="s">
         <v>73</v>
       </c>
@@ -8766,7 +8763,7 @@
       <c r="C30" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="20" t="s">
         <v>284</v>
       </c>
       <c r="E30" s="13" t="s">
@@ -8781,8 +8778,8 @@
       <c r="H30" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="27"/>
-      <c r="J30" s="28"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="22"/>
       <c r="L30" s="18" t="s">
         <v>243</v>
       </c>
@@ -8982,7 +8979,7 @@
         <v>16</v>
       </c>
       <c r="J36" s="13"/>
-      <c r="K36" s="25" t="s">
+      <c r="K36" s="19" t="s">
         <v>300</v>
       </c>
       <c r="L36" s="18" t="s">
@@ -9329,16 +9326,16 @@
       <c r="B47" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="22" t="s">
+      <c r="C47" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="23"/>
-      <c r="G47" s="23"/>
-      <c r="H47" s="23"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="24"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
       <c r="L47" s="18" t="s">
         <v>73</v>
       </c>
@@ -9442,17 +9439,17 @@
       <c r="A51" s="6">
         <v>51</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="20"/>
-      <c r="I51" s="20"/>
-      <c r="J51" s="21"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="30"/>
       <c r="L51" s="18" t="s">
         <v>73</v>
       </c>
@@ -9461,17 +9458,17 @@
       <c r="A52" s="6">
         <v>52</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="21"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="30"/>
       <c r="L52" s="18" t="s">
         <v>73</v>
       </c>
@@ -9480,17 +9477,17 @@
       <c r="A53" s="6">
         <v>53</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C53" s="20"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
-      <c r="J53" s="21"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="30"/>
       <c r="L53" s="18" t="s">
         <v>73</v>
       </c>
@@ -9532,17 +9529,17 @@
       <c r="A55" s="6">
         <v>55</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="21"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="30"/>
       <c r="L55" s="18" t="s">
         <v>73</v>
       </c>
@@ -9805,125 +9802,125 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B51:J51"/>
+    <mergeCell ref="B52:J52"/>
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B55:J55"/>
     <mergeCell ref="C15:J15"/>
     <mergeCell ref="C25:J25"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C47:J47"/>
     <mergeCell ref="C28:J28"/>
-    <mergeCell ref="B51:J51"/>
-    <mergeCell ref="B52:J52"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B55:J55"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C6 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5 K36 B30">
-    <cfRule type="containsBlanks" dxfId="41" priority="29">
+    <cfRule type="containsBlanks" dxfId="23" priority="29">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L60 B64:B65">
-    <cfRule type="cellIs" dxfId="40" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="26" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsBlanks" dxfId="38" priority="24">
+    <cfRule type="containsBlanks" dxfId="20" priority="24">
       <formula>LEN(TRIM(C47))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28">
-    <cfRule type="containsBlanks" dxfId="37" priority="23">
+    <cfRule type="containsBlanks" dxfId="19" priority="23">
       <formula>LEN(TRIM(C28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
-    <cfRule type="containsBlanks" dxfId="36" priority="22">
+    <cfRule type="containsBlanks" dxfId="18" priority="22">
       <formula>LEN(TRIM(B52))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="containsBlanks" dxfId="35" priority="21">
+    <cfRule type="containsBlanks" dxfId="17" priority="21">
       <formula>LEN(TRIM(B53))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="containsBlanks" dxfId="34" priority="20">
+    <cfRule type="containsBlanks" dxfId="16" priority="20">
       <formula>LEN(TRIM(B55))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="containsBlanks" dxfId="33" priority="19">
+    <cfRule type="containsBlanks" dxfId="15" priority="19">
       <formula>LEN(TRIM(C15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="containsBlanks" dxfId="32" priority="18">
+    <cfRule type="containsBlanks" dxfId="14" priority="18">
       <formula>LEN(TRIM(C25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsBlanks" dxfId="31" priority="17">
+    <cfRule type="containsBlanks" dxfId="13" priority="17">
       <formula>LEN(TRIM(C30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="containsBlanks" dxfId="30" priority="16">
+    <cfRule type="containsBlanks" dxfId="12" priority="16">
       <formula>LEN(TRIM(E30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30">
-    <cfRule type="containsBlanks" dxfId="29" priority="15">
+    <cfRule type="containsBlanks" dxfId="11" priority="15">
       <formula>LEN(TRIM(F30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G30">
-    <cfRule type="containsBlanks" dxfId="28" priority="14">
+    <cfRule type="containsBlanks" dxfId="10" priority="14">
       <formula>LEN(TRIM(G30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H30">
-    <cfRule type="containsBlanks" dxfId="27" priority="13">
+    <cfRule type="containsBlanks" dxfId="9" priority="13">
       <formula>LEN(TRIM(H30))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:J61">
-    <cfRule type="containsBlanks" dxfId="26" priority="12">
+    <cfRule type="containsBlanks" dxfId="8" priority="12">
       <formula>LEN(TRIM(B61))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L61">
-    <cfRule type="cellIs" dxfId="25" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:J62">
-    <cfRule type="containsBlanks" dxfId="23" priority="9">
+    <cfRule type="containsBlanks" dxfId="5" priority="9">
       <formula>LEN(TRIM(B62))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L62">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63:J63">
-    <cfRule type="containsBlanks" dxfId="20" priority="6">
+    <cfRule type="containsBlanks" dxfId="2" priority="6">
       <formula>LEN(TRIM(B63))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Adjusted end time in mission 57 to match the notesheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC70F28D-8E7E-AC45-8B63-4834C3BAC72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB16F8B1-9E5D-6747-9DF6-3B3CBFC2AF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="395">
   <si>
     <t>Mission Number</t>
   </si>
@@ -1237,6 +1237,9 @@
   </si>
   <si>
     <t>2021-10-29T16:25:00</t>
+  </si>
+  <si>
+    <t>2021-10-26T13:15:00</t>
   </si>
 </sst>
 </file>
@@ -1501,6 +1504,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1508,15 +1520,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2511,8 +2514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="N52" workbookViewId="0">
+      <selection activeCell="R59" sqref="R59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6216,7 +6219,7 @@
         <v>304</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="S59" s="4" t="s">
         <v>309</v>
@@ -8029,16 +8032,16 @@
       <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
       <c r="L6" s="10" t="s">
         <v>73</v>
       </c>
@@ -8309,16 +8312,16 @@
       <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="30"/>
       <c r="L15" s="18" t="s">
         <v>73</v>
       </c>
@@ -8619,16 +8622,16 @@
       <c r="B25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="30"/>
       <c r="L25" s="18" t="s">
         <v>73</v>
       </c>
@@ -8706,16 +8709,16 @@
       <c r="B28" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="30"/>
       <c r="L28" s="18" t="s">
         <v>73</v>
       </c>
@@ -9326,16 +9329,16 @@
       <c r="B47" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="30"/>
       <c r="L47" s="18" t="s">
         <v>73</v>
       </c>
@@ -9439,17 +9442,17 @@
       <c r="A51" s="6">
         <v>51</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-      <c r="I51" s="29"/>
-      <c r="J51" s="30"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="26"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="26"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
       <c r="L51" s="18" t="s">
         <v>73</v>
       </c>
@@ -9458,17 +9461,17 @@
       <c r="A52" s="6">
         <v>52</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="30"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="27"/>
       <c r="L52" s="18" t="s">
         <v>73</v>
       </c>
@@ -9477,17 +9480,17 @@
       <c r="A53" s="6">
         <v>53</v>
       </c>
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="30"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="26"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
       <c r="L53" s="18" t="s">
         <v>73</v>
       </c>
@@ -9529,17 +9532,17 @@
       <c r="A55" s="6">
         <v>55</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="25" t="s">
         <v>248</v>
       </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="30"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="26"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
       <c r="L55" s="18" t="s">
         <v>73</v>
       </c>
@@ -9802,15 +9805,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C6:J6"/>
+    <mergeCell ref="C47:J47"/>
+    <mergeCell ref="C28:J28"/>
     <mergeCell ref="B51:J51"/>
     <mergeCell ref="B52:J52"/>
     <mergeCell ref="B53:J53"/>
     <mergeCell ref="B55:J55"/>
     <mergeCell ref="C15:J15"/>
     <mergeCell ref="C25:J25"/>
-    <mergeCell ref="C6:J6"/>
-    <mergeCell ref="C47:J47"/>
-    <mergeCell ref="C28:J28"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C6 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5 K36 B30">
     <cfRule type="containsBlanks" dxfId="23" priority="29">

</xml_diff>

<commit_message>
Updated DUNEX notes spreadsheet with masks sheet
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUNEX/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB16F8B1-9E5D-6747-9DF6-3B3CBFC2AF1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D989EE-4439-1A45-A1F6-CDCC8D0F9B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="35200" yWindow="1380" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main Experiment" sheetId="1" r:id="rId1"/>
+    <sheet name="microSWIFT Status" sheetId="2" r:id="rId2"/>
+    <sheet name="microSWIFT Masks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1633" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="404">
   <si>
     <t>Mission Number</t>
   </si>
@@ -1240,6 +1241,33 @@
   </si>
   <si>
     <t>2021-10-26T13:15:00</t>
+  </si>
+  <si>
+    <t>microSWIFT ID</t>
+  </si>
+  <si>
+    <t>Additional Masking indices</t>
+  </si>
+  <si>
+    <t>microSWIFT_3</t>
+  </si>
+  <si>
+    <t>microSWIFT_4</t>
+  </si>
+  <si>
+    <t>Notes on why each point was masked</t>
+  </si>
+  <si>
+    <t>5,10,15</t>
+  </si>
+  <si>
+    <t>Start Mask End Index</t>
+  </si>
+  <si>
+    <t>End Mask Start Index</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -1435,7 +1463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1504,6 +1532,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1512,14 +1549,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2514,8 +2545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N52" workbookViewId="0">
-      <selection activeCell="R59" sqref="R59"/>
+    <sheetView topLeftCell="N27" workbookViewId="0">
+      <selection activeCell="O67" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8032,16 +8063,16 @@
       <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
       <c r="L6" s="10" t="s">
         <v>73</v>
       </c>
@@ -8312,16 +8343,16 @@
       <c r="B15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="30"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
       <c r="L15" s="18" t="s">
         <v>73</v>
       </c>
@@ -8622,16 +8653,16 @@
       <c r="B25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="30"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
       <c r="L25" s="18" t="s">
         <v>73</v>
       </c>
@@ -8709,16 +8740,16 @@
       <c r="B28" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="30"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
       <c r="L28" s="18" t="s">
         <v>73</v>
       </c>
@@ -9329,16 +9360,16 @@
       <c r="B47" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="25" t="s">
         <v>241</v>
       </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-      <c r="I47" s="29"/>
-      <c r="J47" s="30"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
       <c r="L47" s="18" t="s">
         <v>73</v>
       </c>
@@ -9442,17 +9473,17 @@
       <c r="A51" s="6">
         <v>51</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="30"/>
       <c r="L51" s="18" t="s">
         <v>73</v>
       </c>
@@ -9461,17 +9492,17 @@
       <c r="A52" s="6">
         <v>52</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="26"/>
-      <c r="J52" s="27"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="30"/>
       <c r="L52" s="18" t="s">
         <v>73</v>
       </c>
@@ -9480,17 +9511,17 @@
       <c r="A53" s="6">
         <v>53</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="27"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="30"/>
       <c r="L53" s="18" t="s">
         <v>73</v>
       </c>
@@ -9532,17 +9563,17 @@
       <c r="A55" s="6">
         <v>55</v>
       </c>
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="30"/>
       <c r="L55" s="18" t="s">
         <v>73</v>
       </c>
@@ -9805,15 +9836,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B53:J53"/>
+    <mergeCell ref="B55:J55"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="C25:J25"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C47:J47"/>
     <mergeCell ref="C28:J28"/>
     <mergeCell ref="B51:J51"/>
     <mergeCell ref="B52:J52"/>
-    <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B55:J55"/>
-    <mergeCell ref="C15:J15"/>
-    <mergeCell ref="C25:J25"/>
   </mergeCells>
   <conditionalFormatting sqref="B6:C6 B47 B28 B51 B15 B25 B7:J14 B16:J24 B26:J27 B29:J29 K46 B48:J50 B54:J54 B56:J60 B31:J46 K5 B2:J5 K36 B30">
     <cfRule type="containsBlanks" dxfId="23" priority="29">
@@ -9929,4 +9960,884 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FE30A9-F57B-EB49-8BDD-C157B71BFDBB}">
+  <dimension ref="A1:F83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C2" s="10">
+        <v>200</v>
+      </c>
+      <c r="D2" s="10">
+        <v>800</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="31"/>
+      <c r="B3" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C3" s="10">
+        <v>200</v>
+      </c>
+      <c r="D3" s="10">
+        <v>800</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="10">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="10">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="10">
+        <v>8</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="10">
+        <v>9</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="10">
+        <v>10</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="10">
+        <v>11</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="10">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="10">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="10">
+        <v>15</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="10">
+        <v>16</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>17</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="10">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="10">
+        <v>19</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="10">
+        <v>20</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="10">
+        <v>21</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="10">
+        <v>22</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="10">
+        <v>23</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="10">
+        <v>24</v>
+      </c>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="10">
+        <v>25</v>
+      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="10">
+        <v>26</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="10">
+        <v>27</v>
+      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="10">
+        <v>28</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="10">
+        <v>29</v>
+      </c>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="10">
+        <v>30</v>
+      </c>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="10">
+        <v>31</v>
+      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="10">
+        <v>32</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="10">
+        <v>33</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>34</v>
+      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="10">
+        <v>35</v>
+      </c>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="10">
+        <v>36</v>
+      </c>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="10">
+        <v>37</v>
+      </c>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="10">
+        <v>38</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="10">
+        <v>39</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="10">
+        <v>40</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="10">
+        <v>41</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="10">
+        <v>42</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="10">
+        <v>43</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="10">
+        <v>44</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="10">
+        <v>45</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="10">
+        <v>46</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="10">
+        <v>47</v>
+      </c>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="10">
+        <v>48</v>
+      </c>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="10">
+        <v>49</v>
+      </c>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="10">
+        <v>50</v>
+      </c>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="10">
+        <v>51</v>
+      </c>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="10">
+        <v>52</v>
+      </c>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="10">
+        <v>53</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="10">
+        <v>54</v>
+      </c>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="10">
+        <v>55</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="10">
+        <v>56</v>
+      </c>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="10">
+        <v>57</v>
+      </c>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="10">
+        <v>58</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="10">
+        <v>59</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="10">
+        <v>60</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="10">
+        <v>61</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="10">
+        <v>62</v>
+      </c>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="10">
+        <v>63</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="10">
+        <v>64</v>
+      </c>
+      <c r="B66" s="10"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="10">
+        <v>65</v>
+      </c>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="10">
+        <v>66</v>
+      </c>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="10">
+        <v>67</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="10">
+        <v>68</v>
+      </c>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="10">
+        <v>69</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="10">
+        <v>70</v>
+      </c>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="10">
+        <v>71</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="10">
+        <v>72</v>
+      </c>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="10">
+        <v>73</v>
+      </c>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="10">
+        <v>74</v>
+      </c>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="10">
+        <v>75</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="10">
+        <v>76</v>
+      </c>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="10">
+        <v>77</v>
+      </c>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="10">
+        <v>78</v>
+      </c>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="10">
+        <v>79</v>
+      </c>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="10">
+        <v>80</v>
+      </c>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="10">
+        <v>81</v>
+      </c>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated .gitignore and notes with old microSWIFT data
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejrainville/Documents/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394F49BC-73AF-8D4C-B983-989950D9D78F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFBD26B-F375-E445-8F4C-77F8EFC61177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="500" windowWidth="39940" windowHeight="26580" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -10678,7 +10678,7 @@
   <dimension ref="A1:F203"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated through mission 27 cleaning
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejrainville/Documents/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0C3FD3-C42E-CD4E-BED7-14DF62508B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1E418-56A5-924D-BDE1-771148AFCB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="71680" yWindow="500" windowWidth="25600" windowHeight="18740" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -3238,7 +3238,7 @@
   <dimension ref="A1:U83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O25" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
corrects the dataset and adds the final dataset
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejrainville/Documents/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C1E418-56A5-924D-BDE1-771148AFCB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7DE38D-9726-034B-8C2B-0313558E211C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="71680" yWindow="500" windowWidth="25600" windowHeight="18740" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="71680" yWindow="500" windowWidth="25600" windowHeight="18740" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Experiment" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="623">
   <si>
     <t>Mission Number</t>
   </si>
@@ -935,9 +935,6 @@
     <t>microSWIFT_4</t>
   </si>
   <si>
-    <t>Notes on why each point was masked</t>
-  </si>
-  <si>
     <t>Start Mask End Index</t>
   </si>
   <si>
@@ -1430,18 +1427,9 @@
     <t>2021-10-05T14:42:00</t>
   </si>
   <si>
-    <t>Masked microSWIFT 4 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in</t>
-  </si>
-  <si>
-    <t>Masked microSWIFT 3 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in</t>
-  </si>
-  <si>
     <t>microSWIFT_5</t>
   </si>
   <si>
-    <t>Masked microSWIFT 5 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in</t>
-  </si>
-  <si>
     <t>2021-10-05T17:17:00</t>
   </si>
   <si>
@@ -1926,6 +1914,15 @@
   </si>
   <si>
     <t>2021-10-11T17:50:00</t>
+  </si>
+  <si>
+    <t>Masked microSWIFT 4 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.</t>
+  </si>
+  <si>
+    <t>Masked microSWIFT 5 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.</t>
+  </si>
+  <si>
+    <t>Masked microSWIFT 3 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.</t>
   </si>
 </sst>
 </file>
@@ -3237,7 +3234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:U83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O25" workbookViewId="0">
+    <sheetView topLeftCell="O25" workbookViewId="0">
       <selection activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
@@ -3447,10 +3444,10 @@
         <v>38</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>454</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>455</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>52</v>
@@ -3512,10 +3509,10 @@
         <v>38</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="S4" s="9" t="s">
         <v>45</v>
@@ -3577,10 +3574,10 @@
         <v>38</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>47</v>
@@ -3642,10 +3639,10 @@
         <v>38</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>48</v>
@@ -3707,7 +3704,7 @@
         <v>38</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>56</v>
@@ -3837,10 +3834,10 @@
         <v>38</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>60</v>
@@ -3902,10 +3899,10 @@
         <v>69</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>81</v>
@@ -3970,7 +3967,7 @@
         <v>71</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>81</v>
@@ -4032,7 +4029,7 @@
         <v>69</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>73</v>
@@ -4097,10 +4094,10 @@
         <v>38</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>81</v>
@@ -4162,10 +4159,10 @@
         <v>76</v>
       </c>
       <c r="Q14" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>313</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>81</v>
@@ -4227,10 +4224,10 @@
         <v>76</v>
       </c>
       <c r="Q15" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="R15" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>78</v>
@@ -4292,10 +4289,10 @@
         <v>76</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>81</v>
@@ -4360,7 +4357,7 @@
         <v>84</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="S17" s="4" t="s">
         <v>88</v>
@@ -4422,10 +4419,10 @@
         <v>87</v>
       </c>
       <c r="Q18" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>321</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>322</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>81</v>
@@ -4487,10 +4484,10 @@
         <v>87</v>
       </c>
       <c r="Q19" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="R19" s="11" t="s">
         <v>323</v>
-      </c>
-      <c r="R19" s="11" t="s">
-        <v>324</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>81</v>
@@ -4552,10 +4549,10 @@
         <v>87</v>
       </c>
       <c r="Q20" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="S20" s="4" t="s">
         <v>81</v>
@@ -4620,7 +4617,7 @@
         <v>86</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>81</v>
@@ -4685,7 +4682,7 @@
         <v>162</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S22" s="4" t="s">
         <v>81</v>
@@ -4746,7 +4743,7 @@
         <v>161</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="S23" s="4" t="s">
         <v>97</v>
@@ -4807,7 +4804,7 @@
         <v>163</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>81</v>
@@ -4865,10 +4862,10 @@
         <v>87</v>
       </c>
       <c r="Q25" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="S25" s="4" t="s">
         <v>81</v>
@@ -4926,10 +4923,10 @@
         <v>87</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>81</v>
@@ -4987,10 +4984,10 @@
         <v>87</v>
       </c>
       <c r="Q27" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="S27" s="4" t="s">
         <v>103</v>
@@ -5048,10 +5045,10 @@
         <v>87</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S28" s="4" t="s">
         <v>104</v>
@@ -5109,10 +5106,10 @@
         <v>87</v>
       </c>
       <c r="Q29" s="11" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="S29" s="4" t="s">
         <v>104</v>
@@ -5170,10 +5167,10 @@
         <v>87</v>
       </c>
       <c r="Q30" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>81</v>
@@ -5231,10 +5228,10 @@
         <v>109</v>
       </c>
       <c r="Q31" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>356</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>81</v>
@@ -5292,10 +5289,10 @@
         <v>111</v>
       </c>
       <c r="Q32" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>358</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>81</v>
@@ -5353,10 +5350,10 @@
         <v>113</v>
       </c>
       <c r="Q33" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>361</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>81</v>
@@ -5417,7 +5414,7 @@
         <v>116</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>136</v>
@@ -5475,10 +5472,10 @@
         <v>131</v>
       </c>
       <c r="Q35" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="R35" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>81</v>
@@ -5536,7 +5533,7 @@
         <v>133</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R36" s="1" t="s">
         <v>119</v>
@@ -5597,10 +5594,10 @@
         <v>132</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>81</v>
@@ -5658,10 +5655,10 @@
         <v>132</v>
       </c>
       <c r="Q38" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="R38" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="S38" s="4" t="s">
         <v>81</v>
@@ -5719,10 +5716,10 @@
         <v>134</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>81</v>
@@ -5783,7 +5780,7 @@
         <v>123</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>81</v>
@@ -5841,10 +5838,10 @@
         <v>138</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>142</v>
@@ -5902,10 +5899,10 @@
         <v>138</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>141</v>
@@ -5963,10 +5960,10 @@
         <v>185</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>81</v>
@@ -6024,10 +6021,10 @@
         <v>186</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>189</v>
@@ -6146,10 +6143,10 @@
         <v>195</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="S46" s="4" t="s">
         <v>196</v>
@@ -6207,10 +6204,10 @@
         <v>198</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="S47" s="4" t="s">
         <v>199</v>
@@ -6268,7 +6265,7 @@
         <v>201</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>151</v>
@@ -6573,7 +6570,7 @@
         <v>207</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>182</v>
@@ -6878,10 +6875,10 @@
         <v>218</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="R58" s="11" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="S58" s="4" t="s">
         <v>226</v>
@@ -7000,10 +6997,10 @@
         <v>232</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="S60" s="4" t="s">
         <v>237</v>
@@ -7064,7 +7061,7 @@
         <v>234</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="S61" s="4" t="s">
         <v>236</v>
@@ -7122,7 +7119,7 @@
         <v>232</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>242</v>
@@ -7183,10 +7180,10 @@
         <v>262</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="S63" s="4" t="s">
         <v>81</v>
@@ -7247,7 +7244,7 @@
         <v>245</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="S64" s="4" t="s">
         <v>270</v>
@@ -7427,7 +7424,7 @@
         <v>269</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="R67" s="1" t="s">
         <v>258</v>
@@ -7549,10 +7546,10 @@
         <v>268</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="S69" s="4" t="s">
         <v>81</v>
@@ -7610,10 +7607,10 @@
         <v>268</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="S70" s="4" t="s">
         <v>273</v>
@@ -7671,10 +7668,10 @@
         <v>269</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="R71" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>81</v>
@@ -7732,10 +7729,10 @@
         <v>269</v>
       </c>
       <c r="Q72" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="R72" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="R72" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="S72" s="4" t="s">
         <v>81</v>
@@ -7793,10 +7790,10 @@
         <v>269</v>
       </c>
       <c r="Q73" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="R73" s="1" t="s">
         <v>376</v>
-      </c>
-      <c r="R73" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="S73" s="4" t="s">
         <v>274</v>
@@ -7915,10 +7912,10 @@
         <v>269</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S75" s="4" t="s">
         <v>276</v>
@@ -7976,10 +7973,10 @@
         <v>281</v>
       </c>
       <c r="Q76" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="R76" s="1" t="s">
         <v>382</v>
-      </c>
-      <c r="R76" s="1" t="s">
-        <v>383</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>282</v>
@@ -8037,10 +8034,10 @@
         <v>283</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="R77" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S77" s="4" t="s">
         <v>282</v>
@@ -8098,10 +8095,10 @@
         <v>283</v>
       </c>
       <c r="Q78" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="R78" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S78" s="4" t="s">
         <v>284</v>
@@ -8159,10 +8156,10 @@
         <v>269</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S79" s="4" t="s">
         <v>284</v>
@@ -8220,10 +8217,10 @@
         <v>269</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="S80" s="4" t="s">
         <v>284</v>
@@ -8281,10 +8278,10 @@
         <v>269</v>
       </c>
       <c r="Q81" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="R81" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="R81" s="1" t="s">
-        <v>408</v>
       </c>
       <c r="S81" s="4" t="s">
         <v>284</v>
@@ -8342,10 +8339,10 @@
         <v>269</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="R82" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="S82" s="4" t="s">
         <v>284</v>
@@ -8406,7 +8403,7 @@
         <v>287</v>
       </c>
       <c r="R83" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="S83" s="4" t="s">
         <v>286</v>
@@ -10659,8 +10656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FE30A9-F57B-EB49-8BDD-C157B71BFDBB}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10680,16 +10677,16 @@
         <v>289</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>294</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>295</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>290</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>293</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -10719,13 +10716,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>458</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="39"/>
       <c r="B4" s="10" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C4" s="10">
         <v>200</v>
@@ -10737,7 +10734,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>461</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10755,7 +10752,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>459</v>
+        <v>622</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10763,7 +10760,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
@@ -10775,7 +10772,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10793,13 +10790,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="39"/>
       <c r="B8" s="10" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -10811,13 +10808,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="10" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
@@ -10829,7 +10826,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10837,7 +10834,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -10849,13 +10846,13 @@
         <v>0</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="39"/>
       <c r="B11" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C11" s="10">
         <v>0</v>
@@ -10867,7 +10864,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10885,7 +10882,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -10905,13 +10902,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="39"/>
       <c r="B14" s="10" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C14" s="10">
         <v>1000</v>
@@ -10923,13 +10920,13 @@
         <v>0</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="39"/>
       <c r="B15" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C15" s="10">
         <v>500</v>
@@ -10941,13 +10938,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="39"/>
       <c r="B16" s="10" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C16" s="10">
         <v>500</v>
@@ -10959,13 +10956,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="39"/>
       <c r="B17" s="10" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C17" s="10">
         <v>1500</v>
@@ -10977,7 +10974,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -10995,7 +10992,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C19" s="10">
         <v>0</v>
@@ -11007,13 +11004,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="39"/>
       <c r="B20" s="10" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C20" s="10">
         <v>0</v>
@@ -11025,13 +11022,13 @@
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="39"/>
       <c r="B21" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C21" s="10">
         <v>0</v>
@@ -11043,13 +11040,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="39"/>
       <c r="B22" s="10" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
@@ -11097,7 +11094,7 @@
         <v>11</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C26" s="10">
         <v>2000</v>
@@ -11109,7 +11106,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11117,7 +11114,7 @@
         <v>12</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C27" s="10">
         <v>0</v>
@@ -11129,7 +11126,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="23" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -11147,7 +11144,7 @@
         <v>14</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C29" s="10">
         <v>0</v>
@@ -11159,7 +11156,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -11187,7 +11184,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C32" s="10">
         <v>0</v>
@@ -11199,13 +11196,13 @@
         <v>0</v>
       </c>
       <c r="F32" s="23" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="39"/>
       <c r="B33" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C33" s="10">
         <v>2000</v>
@@ -11217,13 +11214,13 @@
         <v>0</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="39"/>
       <c r="B34" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C34" s="10">
         <v>1000</v>
@@ -11235,7 +11232,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11243,7 +11240,7 @@
         <v>18</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C35" s="10">
         <v>0</v>
@@ -11255,13 +11252,13 @@
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="39"/>
       <c r="B36" s="10" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C36" s="10">
         <v>1000</v>
@@ -11273,7 +11270,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -11281,7 +11278,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C37" s="10">
         <v>0</v>
@@ -11293,13 +11290,13 @@
         <v>0</v>
       </c>
       <c r="F37" s="23" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="39"/>
       <c r="B38" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C38" s="10">
         <v>1000</v>
@@ -11311,7 +11308,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11319,7 +11316,7 @@
         <v>20</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C39" s="10">
         <v>0</v>
@@ -11331,7 +11328,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11339,7 +11336,7 @@
         <v>21</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C40" s="10">
         <v>0</v>
@@ -11351,13 +11348,13 @@
         <v>0</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="39"/>
       <c r="B41" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C41" s="10">
         <v>0</v>
@@ -11369,13 +11366,13 @@
         <v>0</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="39"/>
       <c r="B42" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C42" s="10">
         <v>0</v>
@@ -11387,7 +11384,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11395,7 +11392,7 @@
         <v>22</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C43" s="10">
         <v>0</v>
@@ -11407,7 +11404,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11415,7 +11412,7 @@
         <v>23</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C44" s="40">
         <v>500</v>
@@ -11427,13 +11424,13 @@
         <v>0</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="39"/>
       <c r="B45" s="40" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C45" s="40">
         <v>500</v>
@@ -11445,13 +11442,13 @@
         <v>0</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="39"/>
       <c r="B46" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C46" s="40">
         <v>500</v>
@@ -11463,7 +11460,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11471,7 +11468,7 @@
         <v>24</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C47" s="40">
         <v>500</v>
@@ -11483,13 +11480,13 @@
         <v>0</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="39"/>
       <c r="B48" s="40" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="C48" s="40">
         <v>500</v>
@@ -11501,7 +11498,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="41" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11509,7 +11506,7 @@
         <v>25</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C49" s="10">
         <v>0</v>
@@ -11521,7 +11518,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
@@ -11539,7 +11536,7 @@
         <v>27</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C51" s="10">
         <v>100</v>
@@ -11551,13 +11548,13 @@
         <v>0</v>
       </c>
       <c r="F51" s="23" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="39"/>
       <c r="B52" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C52" s="10">
         <v>0</v>
@@ -11569,13 +11566,13 @@
         <v>0</v>
       </c>
       <c r="F52" s="23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="39"/>
       <c r="B53" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C53" s="10">
         <v>0</v>
@@ -11587,7 +11584,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11605,13 +11602,13 @@
         <v>0</v>
       </c>
       <c r="F54" s="23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="39"/>
       <c r="B55" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C55" s="10">
         <v>0</v>
@@ -11623,13 +11620,13 @@
         <v>0</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="39"/>
       <c r="B56" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C56" s="10">
         <v>0</v>
@@ -11641,7 +11638,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -11669,7 +11666,7 @@
         <v>30</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C59" s="10">
         <v>0</v>
@@ -11681,7 +11678,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11689,7 +11686,7 @@
         <v>31</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C60" s="10">
         <v>1000</v>
@@ -11701,13 +11698,13 @@
         <v>0</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="39"/>
       <c r="B61" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C61" s="10">
         <v>1000</v>
@@ -11719,13 +11716,13 @@
         <v>0</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="39"/>
       <c r="B62" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C62" s="10">
         <v>2500</v>
@@ -11737,13 +11734,13 @@
         <v>0</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="39"/>
       <c r="B63" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C63" s="10">
         <v>1000</v>
@@ -11755,7 +11752,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11763,7 +11760,7 @@
         <v>32</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C64" s="10">
         <v>500</v>
@@ -11775,7 +11772,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11783,7 +11780,7 @@
         <v>33</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C65" s="10">
         <v>0</v>
@@ -11795,13 +11792,13 @@
         <v>0</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="39"/>
       <c r="B66" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C66" s="10">
         <v>0</v>
@@ -11813,7 +11810,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -11831,7 +11828,7 @@
         <v>35</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C68" s="10">
         <v>0</v>
@@ -11840,16 +11837,16 @@
         <v>-1</v>
       </c>
       <c r="E68" s="10" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" s="39"/>
       <c r="B69" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C69" s="10">
         <v>5500</v>
@@ -11858,10 +11855,10 @@
         <v>14000</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11869,7 +11866,7 @@
         <v>36</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C70" s="10">
         <v>0</v>
@@ -11881,13 +11878,13 @@
         <v>0</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="39"/>
       <c r="B71" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C71" s="10">
         <v>500</v>
@@ -11899,7 +11896,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11919,7 +11916,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -11937,13 +11934,13 @@
         <v>0</v>
       </c>
       <c r="F73" s="23" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="39"/>
       <c r="B74" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C74" s="10">
         <v>1000</v>
@@ -11955,13 +11952,13 @@
         <v>0</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="39"/>
       <c r="B75" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C75" s="10">
         <v>1200</v>
@@ -11973,13 +11970,13 @@
         <v>0</v>
       </c>
       <c r="F75" s="23" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="39"/>
       <c r="B76" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C76" s="10">
         <v>1300</v>
@@ -11991,13 +11988,13 @@
         <v>0</v>
       </c>
       <c r="F76" s="23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="39"/>
       <c r="B77" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C77" s="10">
         <v>500</v>
@@ -12009,13 +12006,13 @@
         <v>0</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="39"/>
       <c r="B78" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C78" s="10">
         <v>200</v>
@@ -12027,13 +12024,13 @@
         <v>0</v>
       </c>
       <c r="F78" s="23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="39"/>
       <c r="B79" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C79" s="10">
         <v>500</v>
@@ -12045,13 +12042,13 @@
         <v>0</v>
       </c>
       <c r="F79" s="23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="39"/>
       <c r="B80" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C80" s="10">
         <v>600</v>
@@ -12063,13 +12060,13 @@
         <v>0</v>
       </c>
       <c r="F80" s="23" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="39"/>
       <c r="B81" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C81" s="10">
         <v>1200</v>
@@ -12081,7 +12078,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="23" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12089,7 +12086,7 @@
         <v>38</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C82" s="10">
         <v>1000</v>
@@ -12101,13 +12098,13 @@
         <v>0</v>
       </c>
       <c r="F82" s="23" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="39"/>
       <c r="B83" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C83" s="10">
         <v>1000</v>
@@ -12119,13 +12116,13 @@
         <v>0</v>
       </c>
       <c r="F83" s="23" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" s="39"/>
       <c r="B84" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C84" s="10">
         <v>0</v>
@@ -12137,13 +12134,13 @@
         <v>0</v>
       </c>
       <c r="F84" s="23" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="39"/>
       <c r="B85" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C85" s="10">
         <v>1000</v>
@@ -12155,13 +12152,13 @@
         <v>0</v>
       </c>
       <c r="F85" s="23" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="39"/>
       <c r="B86" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C86" s="10">
         <v>1000</v>
@@ -12173,13 +12170,13 @@
         <v>0</v>
       </c>
       <c r="F86" s="23" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="39"/>
       <c r="B87" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C87" s="10">
         <v>1000</v>
@@ -12191,13 +12188,13 @@
         <v>0</v>
       </c>
       <c r="F87" s="23" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="39"/>
       <c r="B88" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C88" s="10">
         <v>2000</v>
@@ -12209,13 +12206,13 @@
         <v>0</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="39"/>
       <c r="B89" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C89" s="10">
         <v>1000</v>
@@ -12227,7 +12224,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12235,7 +12232,7 @@
         <v>39</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C90" s="10">
         <v>0</v>
@@ -12247,13 +12244,13 @@
         <v>0</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="39"/>
       <c r="B91" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C91" s="10">
         <v>0</v>
@@ -12262,16 +12259,16 @@
         <v>-1</v>
       </c>
       <c r="E91" s="10" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="39"/>
       <c r="B92" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C92" s="10">
         <v>0</v>
@@ -12280,16 +12277,16 @@
         <v>-1</v>
       </c>
       <c r="E92" s="10" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="39"/>
       <c r="B93" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C93" s="10">
         <v>0</v>
@@ -12298,16 +12295,16 @@
         <v>-1</v>
       </c>
       <c r="E93" s="10" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="39"/>
       <c r="B94" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C94" s="10">
         <v>0</v>
@@ -12319,7 +12316,7 @@
         <v>0</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12327,7 +12324,7 @@
         <v>40</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C95" s="10">
         <v>0</v>
@@ -12339,13 +12336,13 @@
         <v>0</v>
       </c>
       <c r="F95" s="23" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="39"/>
       <c r="B96" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C96" s="10">
         <v>0</v>
@@ -12357,13 +12354,13 @@
         <v>0</v>
       </c>
       <c r="F96" s="23" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="39"/>
       <c r="B97" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C97" s="10">
         <v>0</v>
@@ -12375,13 +12372,13 @@
         <v>0</v>
       </c>
       <c r="F97" s="23" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="39"/>
       <c r="B98" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C98" s="10">
         <v>0</v>
@@ -12393,13 +12390,13 @@
         <v>0</v>
       </c>
       <c r="F98" s="23" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="39"/>
       <c r="B99" s="10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C99" s="10">
         <v>0</v>
@@ -12411,13 +12408,13 @@
         <v>0</v>
       </c>
       <c r="F99" s="23" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="39"/>
       <c r="B100" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C100" s="10">
         <v>0</v>
@@ -12429,7 +12426,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="23" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12437,7 +12434,7 @@
         <v>41</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C101" s="10">
         <v>800</v>
@@ -12449,13 +12446,13 @@
         <v>0</v>
       </c>
       <c r="F101" s="23" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="39"/>
       <c r="B102" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C102" s="10">
         <v>800</v>
@@ -12467,13 +12464,13 @@
         <v>0</v>
       </c>
       <c r="F102" s="23" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="39"/>
       <c r="B103" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C103" s="10">
         <v>800</v>
@@ -12485,7 +12482,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="23" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12493,7 +12490,7 @@
         <v>42</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C104" s="10">
         <v>5000</v>
@@ -12505,7 +12502,7 @@
         <v>0</v>
       </c>
       <c r="F104" s="23" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12523,13 +12520,13 @@
         <v>0</v>
       </c>
       <c r="F105" s="23" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="39"/>
       <c r="B106" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C106" s="10">
         <v>5000</v>
@@ -12541,13 +12538,13 @@
         <v>0</v>
       </c>
       <c r="F106" s="23" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="39"/>
       <c r="B107" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C107" s="10">
         <v>5000</v>
@@ -12559,13 +12556,13 @@
         <v>0</v>
       </c>
       <c r="F107" s="23" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="39"/>
       <c r="B108" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C108" s="10">
         <v>5000</v>
@@ -12577,13 +12574,13 @@
         <v>0</v>
       </c>
       <c r="F108" s="23" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="39"/>
       <c r="B109" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C109" s="10">
         <v>5000</v>
@@ -12595,13 +12592,13 @@
         <v>0</v>
       </c>
       <c r="F109" s="23" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="39"/>
       <c r="B110" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C110" s="10">
         <v>5000</v>
@@ -12613,13 +12610,13 @@
         <v>0</v>
       </c>
       <c r="F110" s="23" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="39"/>
       <c r="B111" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C111" s="10">
         <v>5000</v>
@@ -12631,13 +12628,13 @@
         <v>0</v>
       </c>
       <c r="F111" s="23" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="39"/>
       <c r="B112" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C112" s="10">
         <v>5000</v>
@@ -12649,13 +12646,13 @@
         <v>0</v>
       </c>
       <c r="F112" s="23" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="39"/>
       <c r="B113" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C113" s="10">
         <v>5000</v>
@@ -12667,7 +12664,7 @@
         <v>0</v>
       </c>
       <c r="F113" s="23" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12685,7 +12682,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="23" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12693,7 +12690,7 @@
         <v>43</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C115" s="10">
         <v>28000</v>
@@ -12705,13 +12702,13 @@
         <v>0</v>
       </c>
       <c r="F115" s="23" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="39"/>
       <c r="B116" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C116" s="10">
         <v>3000</v>
@@ -12723,7 +12720,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="23" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12741,13 +12738,13 @@
         <v>0</v>
       </c>
       <c r="F117" s="23" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="39"/>
       <c r="B118" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C118" s="10">
         <v>500</v>
@@ -12759,13 +12756,13 @@
         <v>0</v>
       </c>
       <c r="F118" s="23" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="39"/>
       <c r="B119" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C119" s="10">
         <v>3000</v>
@@ -12777,7 +12774,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="23" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12785,7 +12782,7 @@
         <v>44</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C120" s="10">
         <v>2000</v>
@@ -12797,7 +12794,7 @@
         <v>0</v>
       </c>
       <c r="F120" s="23" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12805,7 +12802,7 @@
         <v>45</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C121" s="10">
         <v>0</v>
@@ -12817,7 +12814,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="23" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12835,13 +12832,13 @@
         <v>0</v>
       </c>
       <c r="F122" s="23" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="39"/>
       <c r="B123" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C123" s="10">
         <v>0</v>
@@ -12853,13 +12850,13 @@
         <v>0</v>
       </c>
       <c r="F123" s="23" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="39"/>
       <c r="B124" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C124" s="10">
         <v>1000</v>
@@ -12871,7 +12868,7 @@
         <v>0</v>
       </c>
       <c r="F124" s="23" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -12909,7 +12906,7 @@
         <v>49</v>
       </c>
       <c r="B128" s="10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C128" s="10">
         <v>2000</v>
@@ -12921,7 +12918,7 @@
         <v>0</v>
       </c>
       <c r="F128" s="23" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12929,7 +12926,7 @@
         <v>50</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C129" s="10">
         <v>7000</v>
@@ -12941,13 +12938,13 @@
         <v>0</v>
       </c>
       <c r="F129" s="23" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="39"/>
       <c r="B130" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C130" s="10">
         <v>0</v>
@@ -12959,13 +12956,13 @@
         <v>0</v>
       </c>
       <c r="F130" s="23" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="39"/>
       <c r="B131" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C131" s="29">
         <v>7000</v>
@@ -12977,13 +12974,13 @@
         <v>0</v>
       </c>
       <c r="F131" s="30" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="39"/>
       <c r="B132" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C132" s="29">
         <v>7000</v>
@@ -12995,13 +12992,13 @@
         <v>0</v>
       </c>
       <c r="F132" s="30" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="133" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="39"/>
       <c r="B133" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C133" s="29">
         <v>7000</v>
@@ -13013,13 +13010,13 @@
         <v>0</v>
       </c>
       <c r="F133" s="30" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="134" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="39"/>
       <c r="B134" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C134" s="29">
         <v>7000</v>
@@ -13031,13 +13028,13 @@
         <v>0</v>
       </c>
       <c r="F134" s="30" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="39"/>
       <c r="B135" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C135" s="29">
         <v>7000</v>
@@ -13049,13 +13046,13 @@
         <v>0</v>
       </c>
       <c r="F135" s="30" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="136" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="39"/>
       <c r="B136" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C136" s="29">
         <v>7000</v>
@@ -13067,7 +13064,7 @@
         <v>0</v>
       </c>
       <c r="F136" s="30" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13085,7 +13082,7 @@
         <v>0</v>
       </c>
       <c r="F137" s="23" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13093,7 +13090,7 @@
         <v>51</v>
       </c>
       <c r="B138" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C138" s="10">
         <v>156</v>
@@ -13102,16 +13099,16 @@
         <v>30504</v>
       </c>
       <c r="E138" s="10" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="F138" s="23" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="39"/>
       <c r="B139" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C139" s="10">
         <v>0</v>
@@ -13149,7 +13146,7 @@
         <v>54</v>
       </c>
       <c r="B142" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C142" s="10">
         <v>2000</v>
@@ -13161,13 +13158,13 @@
         <v>0</v>
       </c>
       <c r="F142" s="23" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="39"/>
       <c r="B143" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C143" s="10">
         <v>0</v>
@@ -13179,13 +13176,13 @@
         <v>0</v>
       </c>
       <c r="F143" s="23" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="39"/>
       <c r="B144" s="10" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="C144" s="10">
         <v>0</v>
@@ -13197,13 +13194,13 @@
         <v>0</v>
       </c>
       <c r="F144" s="23" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="39"/>
       <c r="B145" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C145" s="10">
         <v>0</v>
@@ -13215,13 +13212,13 @@
         <v>0</v>
       </c>
       <c r="F145" s="23" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="39"/>
       <c r="B146" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C146" s="10">
         <v>0</v>
@@ -13233,13 +13230,13 @@
         <v>0</v>
       </c>
       <c r="F146" s="23" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="147" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="39"/>
       <c r="B147" s="10" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C147" s="10">
         <v>0</v>
@@ -13251,13 +13248,13 @@
         <v>0</v>
       </c>
       <c r="F147" s="23" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="148" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A148" s="39"/>
       <c r="B148" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C148" s="10">
         <v>0</v>
@@ -13269,7 +13266,7 @@
         <v>0</v>
       </c>
       <c r="F148" s="23" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -13299,13 +13296,13 @@
         <v>0</v>
       </c>
       <c r="F150" s="23" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="39"/>
       <c r="B151" s="10" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C151" s="10">
         <v>0</v>
@@ -13317,7 +13314,7 @@
         <v>0</v>
       </c>
       <c r="F151" s="23" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -13365,7 +13362,7 @@
         <v>61</v>
       </c>
       <c r="B156" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C156" s="10">
         <v>0</v>
@@ -13377,7 +13374,7 @@
         <v>0</v>
       </c>
       <c r="F156" s="23" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13385,7 +13382,7 @@
         <v>62</v>
       </c>
       <c r="B157" s="10" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C157" s="10">
         <v>0</v>
@@ -13397,13 +13394,13 @@
         <v>0</v>
       </c>
       <c r="F157" s="23" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="39"/>
       <c r="B158" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C158" s="10">
         <v>400</v>
@@ -13415,13 +13412,13 @@
         <v>0</v>
       </c>
       <c r="F158" s="23" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="39"/>
       <c r="B159" s="10" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C159" s="10">
         <v>300</v>
@@ -13433,13 +13430,13 @@
         <v>0</v>
       </c>
       <c r="F159" s="23" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="39"/>
       <c r="B160" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C160" s="10">
         <v>0</v>
@@ -13451,13 +13448,13 @@
         <v>0</v>
       </c>
       <c r="F160" s="23" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="39"/>
       <c r="B161" s="10" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C161" s="10">
         <v>0</v>
@@ -13469,13 +13466,13 @@
         <v>0</v>
       </c>
       <c r="F161" s="23" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="162" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="39"/>
       <c r="B162" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C162" s="10">
         <v>100</v>
@@ -13487,13 +13484,13 @@
         <v>0</v>
       </c>
       <c r="F162" s="23" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="163" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="39"/>
       <c r="B163" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C163" s="10">
         <v>500</v>
@@ -13505,13 +13502,13 @@
         <v>0</v>
       </c>
       <c r="F163" s="23" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="164" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="39"/>
       <c r="B164" s="10" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C164" s="10">
         <v>200</v>
@@ -13523,7 +13520,7 @@
         <v>0</v>
       </c>
       <c r="F164" s="23" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
     </row>
     <row r="165" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13531,7 +13528,7 @@
         <v>63</v>
       </c>
       <c r="B165" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C165" s="10">
         <v>0</v>
@@ -13543,13 +13540,13 @@
         <v>0</v>
       </c>
       <c r="F165" s="23" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="166" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A166" s="39"/>
       <c r="B166" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C166" s="10">
         <v>0</v>
@@ -13561,13 +13558,13 @@
         <v>0</v>
       </c>
       <c r="F166" s="23" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="39"/>
       <c r="B167" s="10" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C167" s="10">
         <v>0</v>
@@ -13579,7 +13576,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="23" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13597,7 +13594,7 @@
         <v>0</v>
       </c>
       <c r="F168" s="23" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -13625,7 +13622,7 @@
         <v>66</v>
       </c>
       <c r="B171" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C171" s="10">
         <v>0</v>
@@ -13637,13 +13634,13 @@
         <v>0</v>
       </c>
       <c r="F171" s="10" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="39"/>
       <c r="B172" s="10" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C172" s="10">
         <v>1100</v>
@@ -13655,13 +13652,13 @@
         <v>0</v>
       </c>
       <c r="F172" s="10" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="39"/>
       <c r="B173" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C173" s="10">
         <v>500</v>
@@ -13673,13 +13670,13 @@
         <v>0</v>
       </c>
       <c r="F173" s="10" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="39"/>
       <c r="B174" s="10" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C174" s="10">
         <v>0</v>
@@ -13691,13 +13688,13 @@
         <v>0</v>
       </c>
       <c r="F174" s="10" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="39"/>
       <c r="B175" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C175" s="10">
         <v>500</v>
@@ -13709,13 +13706,13 @@
         <v>0</v>
       </c>
       <c r="F175" s="10" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="39"/>
       <c r="B176" s="10" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C176" s="10">
         <v>1200</v>
@@ -13727,13 +13724,13 @@
         <v>0</v>
       </c>
       <c r="F176" s="10" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177" s="39"/>
       <c r="B177" s="10" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C177" s="10">
         <v>500</v>
@@ -13745,7 +13742,7 @@
         <v>0</v>
       </c>
       <c r="F177" s="10" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
@@ -13763,13 +13760,13 @@
         <v>0</v>
       </c>
       <c r="F178" s="10" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179" s="39"/>
       <c r="B179" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C179" s="10">
         <v>0</v>
@@ -13781,7 +13778,7 @@
         <v>0</v>
       </c>
       <c r="F179" s="10" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -13789,7 +13786,7 @@
         <v>67</v>
       </c>
       <c r="B180" s="10" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C180" s="10">
         <v>0</v>
@@ -13801,13 +13798,13 @@
         <v>0</v>
       </c>
       <c r="F180" s="10" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181" s="39"/>
       <c r="B181" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C181" s="10">
         <v>0</v>
@@ -13819,13 +13816,13 @@
         <v>0</v>
       </c>
       <c r="F181" s="10" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="39"/>
       <c r="B182" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C182" s="10">
         <v>0</v>
@@ -13837,13 +13834,13 @@
         <v>0</v>
       </c>
       <c r="F182" s="10" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="39"/>
       <c r="B183" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C183" s="10">
         <v>0</v>
@@ -13855,7 +13852,7 @@
         <v>0</v>
       </c>
       <c r="F183" s="10" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
@@ -13863,7 +13860,7 @@
         <v>68</v>
       </c>
       <c r="B184" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C184" s="10">
         <v>0</v>
@@ -13875,13 +13872,13 @@
         <v>0</v>
       </c>
       <c r="F184" s="10" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="39"/>
       <c r="B185" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C185" s="10">
         <v>0</v>
@@ -13893,13 +13890,13 @@
         <v>0</v>
       </c>
       <c r="F185" s="10" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="39"/>
       <c r="B186" s="10" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C186" s="10">
         <v>0</v>
@@ -13911,7 +13908,7 @@
         <v>0</v>
       </c>
       <c r="F186" s="10" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -13919,7 +13916,7 @@
         <v>69</v>
       </c>
       <c r="B187" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C187" s="10">
         <v>1800</v>
@@ -13931,13 +13928,13 @@
         <v>0</v>
       </c>
       <c r="F187" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" s="39"/>
       <c r="B188" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C188" s="10">
         <v>0</v>
@@ -13949,7 +13946,7 @@
         <v>0</v>
       </c>
       <c r="F188" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -13977,7 +13974,7 @@
         <v>72</v>
       </c>
       <c r="B191" s="25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C191" s="25">
         <v>0</v>
@@ -13989,7 +13986,7 @@
         <v>0</v>
       </c>
       <c r="F191" s="25" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
@@ -14007,7 +14004,7 @@
         <v>74</v>
       </c>
       <c r="B193" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C193" s="25">
         <v>0</v>
@@ -14019,13 +14016,13 @@
         <v>0</v>
       </c>
       <c r="F193" s="25" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="39"/>
       <c r="B194" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C194" s="25">
         <v>0</v>
@@ -14037,7 +14034,7 @@
         <v>0</v>
       </c>
       <c r="F194" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -14055,7 +14052,7 @@
         <v>76</v>
       </c>
       <c r="B196" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C196" s="25">
         <v>2000</v>
@@ -14067,13 +14064,13 @@
         <v>0</v>
       </c>
       <c r="F196" s="25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="39"/>
       <c r="B197" s="25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C197" s="25">
         <v>0</v>
@@ -14085,13 +14082,13 @@
         <v>0</v>
       </c>
       <c r="F197" s="25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A198" s="39"/>
       <c r="B198" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C198" s="25">
         <v>0</v>
@@ -14103,7 +14100,7 @@
         <v>0</v>
       </c>
       <c r="F198" s="25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
@@ -14111,7 +14108,7 @@
         <v>77</v>
       </c>
       <c r="B199" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C199" s="25">
         <v>0</v>
@@ -14123,13 +14120,13 @@
         <v>0</v>
       </c>
       <c r="F199" s="25" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A200" s="39"/>
       <c r="B200" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C200" s="25">
         <v>0</v>
@@ -14141,13 +14138,13 @@
         <v>0</v>
       </c>
       <c r="F200" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A201" s="39"/>
       <c r="B201" s="25" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C201" s="25">
         <v>0</v>
@@ -14159,7 +14156,7 @@
         <v>0</v>
       </c>
       <c r="F201" s="25" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -14167,7 +14164,7 @@
         <v>78</v>
       </c>
       <c r="B202" s="25" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C202" s="25">
         <v>0</v>
@@ -14179,13 +14176,13 @@
         <v>0</v>
       </c>
       <c r="F202" s="25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A203" s="39"/>
       <c r="B203" s="25" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C203" s="25">
         <v>0</v>
@@ -14197,7 +14194,7 @@
         <v>0</v>
       </c>
       <c r="F203" s="25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
@@ -14205,7 +14202,7 @@
         <v>79</v>
       </c>
       <c r="B204" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C204" s="25">
         <v>0</v>
@@ -14217,13 +14214,13 @@
         <v>0</v>
       </c>
       <c r="F204" s="25" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A205" s="39"/>
       <c r="B205" s="25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C205" s="25">
         <v>0</v>
@@ -14235,7 +14232,7 @@
         <v>0</v>
       </c>
       <c r="F205" s="25" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
@@ -14243,7 +14240,7 @@
         <v>80</v>
       </c>
       <c r="B206" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C206" s="25">
         <v>0</v>
@@ -14255,13 +14252,13 @@
         <v>0</v>
       </c>
       <c r="F206" s="25" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="39"/>
       <c r="B207" s="25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C207" s="25">
         <v>0</v>
@@ -14273,13 +14270,13 @@
         <v>0</v>
       </c>
       <c r="F207" s="25" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="39"/>
       <c r="B208" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C208" s="25">
         <v>0</v>
@@ -14291,13 +14288,13 @@
         <v>0</v>
       </c>
       <c r="F208" s="25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="39"/>
       <c r="B209" s="25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C209" s="25">
         <v>0</v>
@@ -14309,7 +14306,7 @@
         <v>0</v>
       </c>
       <c r="F209" s="25" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adds data cleaning notes to the final netCDF build
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejrainville/Documents/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/projects/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D2D48F-3258-3A4F-B992-C84254995F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D1B34-DDBB-7144-9ADD-A9E91A63FC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="50160" windowHeight="26220" activeTab="2" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="50160" windowHeight="26220" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Experiment" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2034" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="650">
   <si>
     <t>Mission Number</t>
   </si>
@@ -2005,6 +2005,9 @@
   </si>
   <si>
     <t>microSWIFT_33 is masked from the start to index 500 due to a large spike in the data.</t>
+  </si>
+  <si>
+    <t>Mission 1(Cleaned on 02/24/22): Adjusted the end time from 2021-10-04T15:30:00 to 2021-10-04T15:17:00 since the microSWIFTs started being picked up at this point</t>
   </si>
 </sst>
 </file>
@@ -2206,7 +2209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2314,20 +2317,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3024,7 +3018,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3312,7 +3306,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3322,8 +3316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:V83"/>
   <sheetViews>
-    <sheetView topLeftCell="E60" workbookViewId="0">
-      <selection activeCell="R78" sqref="R78"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3544,7 +3538,9 @@
       <c r="S3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T3" s="4"/>
+      <c r="T3" s="4" t="s">
+        <v>649</v>
+      </c>
       <c r="U3" s="1" t="s">
         <v>8</v>
       </c>
@@ -10829,8 +10825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74FE30A9-F57B-EB49-8BDD-C157B71BFDBB}">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="N218" sqref="N218"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="I159" sqref="I159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10873,7 +10869,7 @@
       <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="40">
+      <c r="A3" s="39">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -10888,12 +10884,12 @@
       <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="40" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="10" t="s">
         <v>460</v>
       </c>
@@ -10906,10 +10902,10 @@
       <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="40"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="10" t="s">
         <v>294</v>
       </c>
@@ -10922,10 +10918,10 @@
       <c r="E5" s="10">
         <v>0</v>
       </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="40">
+      <c r="A6" s="39">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -10945,7 +10941,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="10" t="s">
         <v>294</v>
       </c>
@@ -10963,7 +10959,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="10" t="s">
         <v>466</v>
       </c>
@@ -10981,7 +10977,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="10" t="s">
         <v>464</v>
       </c>
@@ -10999,7 +10995,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="40">
+      <c r="A10" s="39">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -11019,7 +11015,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="10" t="s">
         <v>305</v>
       </c>
@@ -11037,7 +11033,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="10" t="s">
         <v>295</v>
       </c>
@@ -11055,7 +11051,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="40">
+      <c r="A13" s="39">
         <v>5</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -11075,7 +11071,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="10" t="s">
         <v>460</v>
       </c>
@@ -11093,7 +11089,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="10" t="s">
         <v>303</v>
       </c>
@@ -11111,7 +11107,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="10" t="s">
         <v>466</v>
       </c>
@@ -11129,7 +11125,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="40"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="10" t="s">
         <v>550</v>
       </c>
@@ -11157,7 +11153,7 @@
       <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="40">
+      <c r="A19" s="39">
         <v>7</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -11177,7 +11173,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="40"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="10" t="s">
         <v>460</v>
       </c>
@@ -11195,7 +11191,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="40"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="10" t="s">
         <v>305</v>
       </c>
@@ -11213,7 +11209,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="40"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="10" t="s">
         <v>464</v>
       </c>
@@ -11332,19 +11328,19 @@
       <c r="A30" s="10">
         <v>15</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="C30" s="41">
-        <v>0</v>
-      </c>
-      <c r="D30" s="41">
+      <c r="C30" s="10">
+        <v>0</v>
+      </c>
+      <c r="D30" s="10">
         <v>14000</v>
       </c>
-      <c r="E30" s="41">
-        <v>0</v>
-      </c>
-      <c r="F30" s="42" t="s">
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="23" t="s">
         <v>616</v>
       </c>
     </row>
@@ -11352,19 +11348,19 @@
       <c r="A31" s="10">
         <v>16</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="10" t="s">
         <v>550</v>
       </c>
-      <c r="C31" s="41">
-        <v>0</v>
-      </c>
-      <c r="D31" s="41">
+      <c r="C31" s="10">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10">
         <v>7000</v>
       </c>
-      <c r="E31" s="41">
-        <v>0</v>
-      </c>
-      <c r="F31" s="42" t="s">
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="23" t="s">
         <v>617</v>
       </c>
     </row>
@@ -11389,7 +11385,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40">
+      <c r="A33" s="39">
         <v>18</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -11409,7 +11405,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="40"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="10" t="s">
         <v>307</v>
       </c>
@@ -11427,7 +11423,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="40">
+      <c r="A35" s="39">
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -11447,7 +11443,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="10" t="s">
         <v>460</v>
       </c>
@@ -11465,7 +11461,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="40"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="10" t="s">
         <v>302</v>
       </c>
@@ -11503,7 +11499,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="40">
+      <c r="A39" s="39">
         <v>21</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -11523,7 +11519,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="40"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="10" t="s">
         <v>336</v>
       </c>
@@ -11564,57 +11560,57 @@
       <c r="A42" s="10">
         <v>23</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="C42" s="41">
+      <c r="C42" s="10">
         <v>500</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D42" s="10">
         <v>-1</v>
       </c>
-      <c r="E42" s="41">
-        <v>0</v>
-      </c>
-      <c r="F42" s="42" t="s">
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="23" t="s">
         <v>620</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="40">
+      <c r="A43" s="39">
         <v>24</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="41">
-        <v>0</v>
-      </c>
-      <c r="D43" s="41">
+      <c r="C43" s="10">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10">
         <v>4500</v>
       </c>
-      <c r="E43" s="41">
-        <v>0</v>
-      </c>
-      <c r="F43" s="42" t="s">
+      <c r="E43" s="10">
+        <v>0</v>
+      </c>
+      <c r="F43" s="23" t="s">
         <v>622</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="40"/>
-      <c r="B44" s="41" t="s">
+      <c r="A44" s="39"/>
+      <c r="B44" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C44" s="41">
+      <c r="C44" s="10">
         <v>1000</v>
       </c>
-      <c r="D44" s="41">
+      <c r="D44" s="10">
         <v>-1</v>
       </c>
-      <c r="E44" s="41">
-        <v>0</v>
-      </c>
-      <c r="F44" s="42" t="s">
+      <c r="E44" s="10">
+        <v>0</v>
+      </c>
+      <c r="F44" s="23" t="s">
         <v>621</v>
       </c>
     </row>
@@ -11639,99 +11635,99 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="40">
+      <c r="A46" s="39">
         <v>26</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C46" s="41">
+      <c r="C46" s="10">
         <v>500</v>
       </c>
-      <c r="D46" s="41">
+      <c r="D46" s="10">
         <v>-1</v>
       </c>
-      <c r="E46" s="41">
-        <v>0</v>
-      </c>
-      <c r="F46" s="42" t="s">
+      <c r="E46" s="10">
+        <v>0</v>
+      </c>
+      <c r="F46" s="23" t="s">
         <v>624</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="40"/>
-      <c r="B47" s="41" t="s">
+      <c r="A47" s="39"/>
+      <c r="B47" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="C47" s="41">
+      <c r="C47" s="10">
         <v>500</v>
       </c>
-      <c r="D47" s="41">
+      <c r="D47" s="10">
         <v>-1</v>
       </c>
-      <c r="E47" s="41">
-        <v>0</v>
-      </c>
-      <c r="F47" s="42" t="s">
+      <c r="E47" s="10">
+        <v>0</v>
+      </c>
+      <c r="F47" s="23" t="s">
         <v>627</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="40"/>
-      <c r="B48" s="41" t="s">
+      <c r="A48" s="39"/>
+      <c r="B48" s="10" t="s">
         <v>625</v>
       </c>
-      <c r="C48" s="41">
+      <c r="C48" s="10">
         <v>500</v>
       </c>
-      <c r="D48" s="41">
+      <c r="D48" s="10">
         <v>-1</v>
       </c>
-      <c r="E48" s="41">
-        <v>0</v>
-      </c>
-      <c r="F48" s="42" t="s">
+      <c r="E48" s="10">
+        <v>0</v>
+      </c>
+      <c r="F48" s="23" t="s">
         <v>626</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="40"/>
-      <c r="B49" s="41" t="s">
+      <c r="A49" s="39"/>
+      <c r="B49" s="10" t="s">
         <v>499</v>
       </c>
-      <c r="C49" s="41">
+      <c r="C49" s="10">
         <v>500</v>
       </c>
-      <c r="D49" s="41">
+      <c r="D49" s="10">
         <v>-1</v>
       </c>
-      <c r="E49" s="41">
-        <v>0</v>
-      </c>
-      <c r="F49" s="42" t="s">
+      <c r="E49" s="10">
+        <v>0</v>
+      </c>
+      <c r="F49" s="23" t="s">
         <v>628</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="40"/>
-      <c r="B50" s="41" t="s">
+      <c r="A50" s="39"/>
+      <c r="B50" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C50" s="41">
+      <c r="C50" s="10">
         <v>500</v>
       </c>
-      <c r="D50" s="41">
+      <c r="D50" s="10">
         <v>-1</v>
       </c>
-      <c r="E50" s="41">
-        <v>0</v>
-      </c>
-      <c r="F50" s="42" t="s">
+      <c r="E50" s="10">
+        <v>0</v>
+      </c>
+      <c r="F50" s="23" t="s">
         <v>623</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="40">
+      <c r="A51" s="39">
         <v>27</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -11751,7 +11747,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="40"/>
+      <c r="A52" s="39"/>
       <c r="B52" s="10" t="s">
         <v>309</v>
       </c>
@@ -11769,7 +11765,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="40"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="10" t="s">
         <v>353</v>
       </c>
@@ -11787,7 +11783,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="40"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="10" t="s">
         <v>295</v>
       </c>
@@ -11805,7 +11801,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="40"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="10" t="s">
         <v>299</v>
       </c>
@@ -11823,7 +11819,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="40"/>
+      <c r="A56" s="39"/>
       <c r="B56" s="10" t="s">
         <v>352</v>
       </c>
@@ -11844,19 +11840,19 @@
       <c r="A57" s="10">
         <v>28</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C57" s="10">
         <v>500</v>
       </c>
-      <c r="D57" s="41">
+      <c r="D57" s="10">
         <v>-1</v>
       </c>
-      <c r="E57" s="41">
-        <v>0</v>
-      </c>
-      <c r="F57" s="42" t="s">
+      <c r="E57" s="10">
+        <v>0</v>
+      </c>
+      <c r="F57" s="23" t="s">
         <v>632</v>
       </c>
     </row>
@@ -11899,7 +11895,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="40">
+      <c r="A61" s="39">
         <v>31</v>
       </c>
       <c r="B61" s="10" t="s">
@@ -11919,7 +11915,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="40"/>
+      <c r="A62" s="39"/>
       <c r="B62" s="10" t="s">
         <v>366</v>
       </c>
@@ -11937,7 +11933,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="40"/>
+      <c r="A63" s="39"/>
       <c r="B63" s="10" t="s">
         <v>300</v>
       </c>
@@ -11955,7 +11951,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="40"/>
+      <c r="A64" s="39"/>
       <c r="B64" s="10" t="s">
         <v>304</v>
       </c>
@@ -11993,7 +11989,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="40">
+      <c r="A66" s="39">
         <v>33</v>
       </c>
       <c r="B66" s="10" t="s">
@@ -12013,7 +12009,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="40"/>
+      <c r="A67" s="39"/>
       <c r="B67" s="10" t="s">
         <v>366</v>
       </c>
@@ -12041,7 +12037,7 @@
       <c r="F68" s="27"/>
     </row>
     <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="40">
+      <c r="A69" s="39">
         <v>35</v>
       </c>
       <c r="B69" s="10" t="s">
@@ -12061,7 +12057,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A70" s="40"/>
+      <c r="A70" s="39"/>
       <c r="B70" s="10" t="s">
         <v>412</v>
       </c>
@@ -12079,7 +12075,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="40">
+      <c r="A71" s="39">
         <v>36</v>
       </c>
       <c r="B71" s="10" t="s">
@@ -12099,7 +12095,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="40"/>
+      <c r="A72" s="39"/>
       <c r="B72" s="10" t="s">
         <v>366</v>
       </c>
@@ -12117,7 +12113,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="40"/>
+      <c r="A73" s="39"/>
       <c r="B73" s="10" t="s">
         <v>299</v>
       </c>
@@ -12135,7 +12131,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="40"/>
+      <c r="A74" s="39"/>
       <c r="B74" s="10" t="s">
         <v>304</v>
       </c>
@@ -12153,7 +12149,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="40">
+      <c r="A75" s="39">
         <v>37</v>
       </c>
       <c r="B75" s="10" t="s">
@@ -12173,7 +12169,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="40"/>
+      <c r="A76" s="39"/>
       <c r="B76" s="10" t="s">
         <v>295</v>
       </c>
@@ -12191,7 +12187,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="40"/>
+      <c r="A77" s="39"/>
       <c r="B77" s="10" t="s">
         <v>434</v>
       </c>
@@ -12209,7 +12205,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="40"/>
+      <c r="A78" s="39"/>
       <c r="B78" s="10" t="s">
         <v>433</v>
       </c>
@@ -12227,7 +12223,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="40"/>
+      <c r="A79" s="39"/>
       <c r="B79" s="10" t="s">
         <v>350</v>
       </c>
@@ -12245,7 +12241,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="40"/>
+      <c r="A80" s="39"/>
       <c r="B80" s="10" t="s">
         <v>309</v>
       </c>
@@ -12263,7 +12259,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="40"/>
+      <c r="A81" s="39"/>
       <c r="B81" s="10" t="s">
         <v>305</v>
       </c>
@@ -12281,7 +12277,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A82" s="40"/>
+      <c r="A82" s="39"/>
       <c r="B82" s="10" t="s">
         <v>395</v>
       </c>
@@ -12299,7 +12295,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A83" s="40"/>
+      <c r="A83" s="39"/>
       <c r="B83" s="10" t="s">
         <v>439</v>
       </c>
@@ -12317,7 +12313,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="40"/>
+      <c r="A84" s="39"/>
       <c r="B84" s="10" t="s">
         <v>432</v>
       </c>
@@ -12335,7 +12331,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="40">
+      <c r="A85" s="39">
         <v>38</v>
       </c>
       <c r="B85" s="10" t="s">
@@ -12355,7 +12351,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="40"/>
+      <c r="A86" s="39"/>
       <c r="B86" s="10" t="s">
         <v>301</v>
       </c>
@@ -12373,7 +12369,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A87" s="40"/>
+      <c r="A87" s="39"/>
       <c r="B87" s="10" t="s">
         <v>439</v>
       </c>
@@ -12391,7 +12387,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A88" s="40"/>
+      <c r="A88" s="39"/>
       <c r="B88" s="10" t="s">
         <v>302</v>
       </c>
@@ -12409,7 +12405,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="40"/>
+      <c r="A89" s="39"/>
       <c r="B89" s="10" t="s">
         <v>308</v>
       </c>
@@ -12427,7 +12423,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="40"/>
+      <c r="A90" s="39"/>
       <c r="B90" s="10" t="s">
         <v>299</v>
       </c>
@@ -12445,7 +12441,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="40"/>
+      <c r="A91" s="39"/>
       <c r="B91" s="10" t="s">
         <v>304</v>
       </c>
@@ -12463,7 +12459,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="40"/>
+      <c r="A92" s="39"/>
       <c r="B92" s="10" t="s">
         <v>366</v>
       </c>
@@ -12481,7 +12477,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="40"/>
+      <c r="A93" s="39"/>
       <c r="B93" s="10" t="s">
         <v>448</v>
       </c>
@@ -12499,7 +12495,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="40">
+      <c r="A94" s="39">
         <v>39</v>
       </c>
       <c r="B94" s="10" t="s">
@@ -12519,7 +12515,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="40"/>
+      <c r="A95" s="39"/>
       <c r="B95" s="10" t="s">
         <v>448</v>
       </c>
@@ -12537,7 +12533,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="40"/>
+      <c r="A96" s="39"/>
       <c r="B96" s="10" t="s">
         <v>303</v>
       </c>
@@ -12555,7 +12551,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="40"/>
+      <c r="A97" s="39"/>
       <c r="B97" s="10" t="s">
         <v>305</v>
       </c>
@@ -12573,7 +12569,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="40"/>
+      <c r="A98" s="39"/>
       <c r="B98" s="10" t="s">
         <v>300</v>
       </c>
@@ -12591,7 +12587,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="40">
+      <c r="A99" s="39">
         <v>40</v>
       </c>
       <c r="B99" s="10" t="s">
@@ -12611,7 +12607,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="40"/>
+      <c r="A100" s="39"/>
       <c r="B100" s="10" t="s">
         <v>448</v>
       </c>
@@ -12629,7 +12625,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="40"/>
+      <c r="A101" s="39"/>
       <c r="B101" s="10" t="s">
         <v>305</v>
       </c>
@@ -12647,7 +12643,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="40"/>
+      <c r="A102" s="39"/>
       <c r="B102" s="10" t="s">
         <v>439</v>
       </c>
@@ -12665,7 +12661,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="40"/>
+      <c r="A103" s="39"/>
       <c r="B103" s="10" t="s">
         <v>395</v>
       </c>
@@ -12683,7 +12679,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="40"/>
+      <c r="A104" s="39"/>
       <c r="B104" s="10" t="s">
         <v>301</v>
       </c>
@@ -12701,7 +12697,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="40"/>
+      <c r="A105" s="39"/>
       <c r="B105" s="10" t="s">
         <v>300</v>
       </c>
@@ -12719,7 +12715,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="40">
+      <c r="A106" s="39">
         <v>41</v>
       </c>
       <c r="B106" s="10" t="s">
@@ -12739,7 +12735,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="40"/>
+      <c r="A107" s="39"/>
       <c r="B107" s="10" t="s">
         <v>353</v>
       </c>
@@ -12757,7 +12753,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="40"/>
+      <c r="A108" s="39"/>
       <c r="B108" s="10" t="s">
         <v>299</v>
       </c>
@@ -12775,7 +12771,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A109" s="40">
+      <c r="A109" s="39">
         <v>42</v>
       </c>
       <c r="B109" s="10" t="s">
@@ -12795,7 +12791,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="40"/>
+      <c r="A110" s="39"/>
       <c r="B110" s="10" t="s">
         <v>295</v>
       </c>
@@ -12813,7 +12809,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="40"/>
+      <c r="A111" s="39"/>
       <c r="B111" s="10" t="s">
         <v>433</v>
       </c>
@@ -12831,7 +12827,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="40"/>
+      <c r="A112" s="39"/>
       <c r="B112" s="10" t="s">
         <v>414</v>
       </c>
@@ -12849,7 +12845,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="40"/>
+      <c r="A113" s="39"/>
       <c r="B113" s="10" t="s">
         <v>350</v>
       </c>
@@ -12867,7 +12863,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="40"/>
+      <c r="A114" s="39"/>
       <c r="B114" s="10" t="s">
         <v>497</v>
       </c>
@@ -12885,7 +12881,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A115" s="40"/>
+      <c r="A115" s="39"/>
       <c r="B115" s="10" t="s">
         <v>499</v>
       </c>
@@ -12903,7 +12899,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="40"/>
+      <c r="A116" s="39"/>
       <c r="B116" s="10" t="s">
         <v>309</v>
       </c>
@@ -12921,7 +12917,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="40"/>
+      <c r="A117" s="39"/>
       <c r="B117" s="10" t="s">
         <v>395</v>
       </c>
@@ -12939,7 +12935,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="40"/>
+      <c r="A118" s="39"/>
       <c r="B118" s="10" t="s">
         <v>374</v>
       </c>
@@ -12957,7 +12953,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A119" s="40"/>
+      <c r="A119" s="39"/>
       <c r="B119" s="10" t="s">
         <v>294</v>
       </c>
@@ -12975,7 +12971,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="40">
+      <c r="A120" s="39">
         <v>43</v>
       </c>
       <c r="B120" s="10" t="s">
@@ -12995,7 +12991,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="40"/>
+      <c r="A121" s="39"/>
       <c r="B121" s="10" t="s">
         <v>448</v>
       </c>
@@ -13013,7 +13009,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="40"/>
+      <c r="A122" s="39"/>
       <c r="B122" s="10" t="s">
         <v>294</v>
       </c>
@@ -13031,7 +13027,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="40"/>
+      <c r="A123" s="39"/>
       <c r="B123" s="10" t="s">
         <v>306</v>
       </c>
@@ -13049,7 +13045,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A124" s="40"/>
+      <c r="A124" s="39"/>
       <c r="B124" s="10" t="s">
         <v>499</v>
       </c>
@@ -13067,7 +13063,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="40"/>
+      <c r="A125" s="39"/>
       <c r="B125" s="10" t="s">
         <v>497</v>
       </c>
@@ -13085,7 +13081,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="40"/>
+      <c r="A126" s="39"/>
       <c r="B126" s="10" t="s">
         <v>432</v>
       </c>
@@ -13103,7 +13099,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="40"/>
+      <c r="A127" s="39"/>
       <c r="B127" s="10" t="s">
         <v>300</v>
       </c>
@@ -13131,7 +13127,7 @@
       <c r="F128" s="27"/>
     </row>
     <row r="129" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="40">
+      <c r="A129" s="39">
         <v>45</v>
       </c>
       <c r="B129" s="10" t="s">
@@ -13151,7 +13147,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="40"/>
+      <c r="A130" s="39"/>
       <c r="B130" s="10" t="s">
         <v>294</v>
       </c>
@@ -13169,7 +13165,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="40"/>
+      <c r="A131" s="39"/>
       <c r="B131" s="10" t="s">
         <v>510</v>
       </c>
@@ -13187,7 +13183,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="40"/>
+      <c r="A132" s="39"/>
       <c r="B132" s="10" t="s">
         <v>414</v>
       </c>
@@ -13255,7 +13251,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A137" s="40">
+      <c r="A137" s="39">
         <v>50</v>
       </c>
       <c r="B137" s="10" t="s">
@@ -13275,7 +13271,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A138" s="40"/>
+      <c r="A138" s="39"/>
       <c r="B138" s="10" t="s">
         <v>299</v>
       </c>
@@ -13293,7 +13289,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A139" s="40"/>
+      <c r="A139" s="39"/>
       <c r="B139" s="10" t="s">
         <v>309</v>
       </c>
@@ -13311,7 +13307,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A140" s="40"/>
+      <c r="A140" s="39"/>
       <c r="B140" s="10" t="s">
         <v>305</v>
       </c>
@@ -13329,7 +13325,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A141" s="40"/>
+      <c r="A141" s="39"/>
       <c r="B141" s="10" t="s">
         <v>433</v>
       </c>
@@ -13347,7 +13343,7 @@
       </c>
     </row>
     <row r="142" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A142" s="40"/>
+      <c r="A142" s="39"/>
       <c r="B142" s="10" t="s">
         <v>497</v>
       </c>
@@ -13365,7 +13361,7 @@
       </c>
     </row>
     <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A143" s="40"/>
+      <c r="A143" s="39"/>
       <c r="B143" s="10" t="s">
         <v>510</v>
       </c>
@@ -13383,7 +13379,7 @@
       </c>
     </row>
     <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A144" s="40"/>
+      <c r="A144" s="39"/>
       <c r="B144" s="10" t="s">
         <v>432</v>
       </c>
@@ -13401,7 +13397,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A145" s="40"/>
+      <c r="A145" s="39"/>
       <c r="B145" s="10" t="s">
         <v>295</v>
       </c>
@@ -13419,7 +13415,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A146" s="40">
+      <c r="A146" s="39">
         <v>51</v>
       </c>
       <c r="B146" s="10" t="s">
@@ -13439,7 +13435,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="40"/>
+      <c r="A147" s="39"/>
       <c r="B147" s="10" t="s">
         <v>305</v>
       </c>
@@ -13475,7 +13471,7 @@
       <c r="F149" s="27"/>
     </row>
     <row r="150" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A150" s="40">
+      <c r="A150" s="39">
         <v>54</v>
       </c>
       <c r="B150" s="10" t="s">
@@ -13495,7 +13491,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A151" s="40"/>
+      <c r="A151" s="39"/>
       <c r="B151" s="10" t="s">
         <v>439</v>
       </c>
@@ -13513,7 +13509,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A152" s="40"/>
+      <c r="A152" s="39"/>
       <c r="B152" s="10" t="s">
         <v>530</v>
       </c>
@@ -13531,7 +13527,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A153" s="40"/>
+      <c r="A153" s="39"/>
       <c r="B153" s="10" t="s">
         <v>510</v>
       </c>
@@ -13549,7 +13545,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A154" s="40"/>
+      <c r="A154" s="39"/>
       <c r="B154" s="10" t="s">
         <v>412</v>
       </c>
@@ -13567,7 +13563,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A155" s="40"/>
+      <c r="A155" s="39"/>
       <c r="B155" s="10" t="s">
         <v>497</v>
       </c>
@@ -13585,7 +13581,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="40"/>
+      <c r="A156" s="39"/>
       <c r="B156" s="10" t="s">
         <v>448</v>
       </c>
@@ -13613,7 +13609,7 @@
       <c r="F157" s="27"/>
     </row>
     <row r="158" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A158" s="40">
+      <c r="A158" s="39">
         <v>56</v>
       </c>
       <c r="B158" s="10" t="s">
@@ -13633,7 +13629,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="40"/>
+      <c r="A159" s="39"/>
       <c r="B159" s="10" t="s">
         <v>412</v>
       </c>
@@ -13651,7 +13647,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="40"/>
+      <c r="A160" s="39"/>
       <c r="B160" s="10" t="s">
         <v>432</v>
       </c>
@@ -13669,7 +13665,7 @@
       </c>
     </row>
     <row r="161" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="40"/>
+      <c r="A161" s="39"/>
       <c r="B161" s="10" t="s">
         <v>510</v>
       </c>
@@ -13747,7 +13743,7 @@
       </c>
     </row>
     <row r="167" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="40">
+      <c r="A167" s="39">
         <v>62</v>
       </c>
       <c r="B167" s="10" t="s">
@@ -13767,7 +13763,7 @@
       </c>
     </row>
     <row r="168" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="40"/>
+      <c r="A168" s="39"/>
       <c r="B168" s="10" t="s">
         <v>353</v>
       </c>
@@ -13785,7 +13781,7 @@
       </c>
     </row>
     <row r="169" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" s="40"/>
+      <c r="A169" s="39"/>
       <c r="B169" s="10" t="s">
         <v>601</v>
       </c>
@@ -13803,7 +13799,7 @@
       </c>
     </row>
     <row r="170" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" s="40"/>
+      <c r="A170" s="39"/>
       <c r="B170" s="10" t="s">
         <v>366</v>
       </c>
@@ -13821,7 +13817,7 @@
       </c>
     </row>
     <row r="171" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A171" s="40"/>
+      <c r="A171" s="39"/>
       <c r="B171" s="10" t="s">
         <v>299</v>
       </c>
@@ -13839,7 +13835,7 @@
       </c>
     </row>
     <row r="172" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A172" s="40"/>
+      <c r="A172" s="39"/>
       <c r="B172" s="10" t="s">
         <v>499</v>
       </c>
@@ -13857,7 +13853,7 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="40"/>
+      <c r="A173" s="39"/>
       <c r="B173" s="10" t="s">
         <v>433</v>
       </c>
@@ -13875,7 +13871,7 @@
       </c>
     </row>
     <row r="174" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A174" s="40"/>
+      <c r="A174" s="39"/>
       <c r="B174" s="10" t="s">
         <v>463</v>
       </c>
@@ -13893,7 +13889,7 @@
       </c>
     </row>
     <row r="175" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A175" s="40">
+      <c r="A175" s="39">
         <v>63</v>
       </c>
       <c r="B175" s="10" t="s">
@@ -13913,7 +13909,7 @@
       </c>
     </row>
     <row r="176" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="40"/>
+      <c r="A176" s="39"/>
       <c r="B176" s="10" t="s">
         <v>303</v>
       </c>
@@ -13931,7 +13927,7 @@
       </c>
     </row>
     <row r="177" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A177" s="40"/>
+      <c r="A177" s="39"/>
       <c r="B177" s="10" t="s">
         <v>587</v>
       </c>
@@ -13949,7 +13945,7 @@
       </c>
     </row>
     <row r="178" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" s="40"/>
+      <c r="A178" s="39"/>
       <c r="B178" s="10" t="s">
         <v>294</v>
       </c>
@@ -13987,7 +13983,7 @@
       <c r="F180" s="26"/>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A181" s="40">
+      <c r="A181" s="39">
         <v>66</v>
       </c>
       <c r="B181" s="10" t="s">
@@ -14007,7 +14003,7 @@
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A182" s="40"/>
+      <c r="A182" s="39"/>
       <c r="B182" s="10" t="s">
         <v>549</v>
       </c>
@@ -14025,7 +14021,7 @@
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A183" s="40"/>
+      <c r="A183" s="39"/>
       <c r="B183" s="10" t="s">
         <v>414</v>
       </c>
@@ -14043,7 +14039,7 @@
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A184" s="40"/>
+      <c r="A184" s="39"/>
       <c r="B184" s="10" t="s">
         <v>555</v>
       </c>
@@ -14061,7 +14057,7 @@
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A185" s="40"/>
+      <c r="A185" s="39"/>
       <c r="B185" s="10" t="s">
         <v>499</v>
       </c>
@@ -14079,7 +14075,7 @@
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A186" s="40"/>
+      <c r="A186" s="39"/>
       <c r="B186" s="10" t="s">
         <v>550</v>
       </c>
@@ -14097,7 +14093,7 @@
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A187" s="40"/>
+      <c r="A187" s="39"/>
       <c r="B187" s="10" t="s">
         <v>547</v>
       </c>
@@ -14115,7 +14111,7 @@
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A188" s="40"/>
+      <c r="A188" s="39"/>
       <c r="B188" s="10" t="s">
         <v>294</v>
       </c>
@@ -14133,7 +14129,7 @@
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A189" s="40"/>
+      <c r="A189" s="39"/>
       <c r="B189" s="10" t="s">
         <v>307</v>
       </c>
@@ -14151,7 +14147,7 @@
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A190" s="40">
+      <c r="A190" s="39">
         <v>67</v>
       </c>
       <c r="B190" s="10" t="s">
@@ -14171,7 +14167,7 @@
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A191" s="40"/>
+      <c r="A191" s="39"/>
       <c r="B191" s="10" t="s">
         <v>395</v>
       </c>
@@ -14189,7 +14185,7 @@
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A192" s="40"/>
+      <c r="A192" s="39"/>
       <c r="B192" s="10" t="s">
         <v>448</v>
       </c>
@@ -14207,7 +14203,7 @@
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A193" s="40"/>
+      <c r="A193" s="39"/>
       <c r="B193" s="10" t="s">
         <v>499</v>
       </c>
@@ -14225,7 +14221,7 @@
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A194" s="40"/>
+      <c r="A194" s="39"/>
       <c r="B194" s="10" t="s">
         <v>400</v>
       </c>
@@ -14243,7 +14239,7 @@
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A195" s="40">
+      <c r="A195" s="39">
         <v>68</v>
       </c>
       <c r="B195" s="10" t="s">
@@ -14263,7 +14259,7 @@
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A196" s="40"/>
+      <c r="A196" s="39"/>
       <c r="B196" s="10" t="s">
         <v>305</v>
       </c>
@@ -14281,7 +14277,7 @@
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A197" s="40"/>
+      <c r="A197" s="39"/>
       <c r="B197" s="10" t="s">
         <v>499</v>
       </c>
@@ -14299,7 +14295,7 @@
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A198" s="40">
+      <c r="A198" s="39">
         <v>69</v>
       </c>
       <c r="B198" s="10" t="s">
@@ -14319,7 +14315,7 @@
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A199" s="40"/>
+      <c r="A199" s="39"/>
       <c r="B199" s="10" t="s">
         <v>406</v>
       </c>
@@ -14337,7 +14333,7 @@
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A200" s="40"/>
+      <c r="A200" s="39"/>
       <c r="B200" s="10" t="s">
         <v>305</v>
       </c>
@@ -14375,27 +14371,27 @@
       <c r="F202" s="24"/>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A203" s="40">
+      <c r="A203" s="39">
         <v>72</v>
       </c>
-      <c r="B203" s="43" t="s">
+      <c r="B203" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="C203" s="43">
+      <c r="C203" s="25">
         <v>500</v>
       </c>
-      <c r="D203" s="43">
+      <c r="D203" s="25">
         <v>-1</v>
       </c>
-      <c r="E203" s="43">
-        <v>0</v>
-      </c>
-      <c r="F203" s="43" t="s">
+      <c r="E203" s="25">
+        <v>0</v>
+      </c>
+      <c r="F203" s="25" t="s">
         <v>648</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A204" s="40"/>
+      <c r="A204" s="39"/>
       <c r="B204" s="25" t="s">
         <v>381</v>
       </c>
@@ -14423,7 +14419,7 @@
       <c r="F205" s="24"/>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A206" s="40">
+      <c r="A206" s="39">
         <v>74</v>
       </c>
       <c r="B206" s="25" t="s">
@@ -14443,7 +14439,7 @@
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A207" s="40"/>
+      <c r="A207" s="39"/>
       <c r="B207" s="25" t="s">
         <v>388</v>
       </c>
@@ -14471,7 +14467,7 @@
       <c r="F208" s="24"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A209" s="40">
+      <c r="A209" s="39">
         <v>76</v>
       </c>
       <c r="B209" s="25" t="s">
@@ -14491,7 +14487,7 @@
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A210" s="40"/>
+      <c r="A210" s="39"/>
       <c r="B210" s="25" t="s">
         <v>366</v>
       </c>
@@ -14509,7 +14505,7 @@
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A211" s="40"/>
+      <c r="A211" s="39"/>
       <c r="B211" s="25" t="s">
         <v>550</v>
       </c>
@@ -14527,7 +14523,7 @@
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A212" s="40"/>
+      <c r="A212" s="39"/>
       <c r="B212" s="25" t="s">
         <v>395</v>
       </c>
@@ -14545,7 +14541,7 @@
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A213" s="40">
+      <c r="A213" s="39">
         <v>77</v>
       </c>
       <c r="B213" s="25" t="s">
@@ -14565,7 +14561,7 @@
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A214" s="40"/>
+      <c r="A214" s="39"/>
       <c r="B214" s="25" t="s">
         <v>395</v>
       </c>
@@ -14583,7 +14579,7 @@
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A215" s="40"/>
+      <c r="A215" s="39"/>
       <c r="B215" s="25" t="s">
         <v>388</v>
       </c>
@@ -14601,7 +14597,7 @@
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A216" s="40">
+      <c r="A216" s="39">
         <v>78</v>
       </c>
       <c r="B216" s="25" t="s">
@@ -14621,7 +14617,7 @@
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A217" s="40"/>
+      <c r="A217" s="39"/>
       <c r="B217" s="25" t="s">
         <v>406</v>
       </c>
@@ -14639,7 +14635,7 @@
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A218" s="40">
+      <c r="A218" s="39">
         <v>79</v>
       </c>
       <c r="B218" s="25" t="s">
@@ -14659,7 +14655,7 @@
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A219" s="40"/>
+      <c r="A219" s="39"/>
       <c r="B219" s="25" t="s">
         <v>412</v>
       </c>
@@ -14677,7 +14673,7 @@
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A220" s="40">
+      <c r="A220" s="39">
         <v>80</v>
       </c>
       <c r="B220" s="25" t="s">
@@ -14697,7 +14693,7 @@
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A221" s="40"/>
+      <c r="A221" s="39"/>
       <c r="B221" s="25" t="s">
         <v>395</v>
       </c>
@@ -14715,7 +14711,7 @@
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A222" s="40"/>
+      <c r="A222" s="39"/>
       <c r="B222" s="25" t="s">
         <v>305</v>
       </c>
@@ -14733,7 +14729,7 @@
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A223" s="40"/>
+      <c r="A223" s="39"/>
       <c r="B223" s="25" t="s">
         <v>414</v>
       </c>
@@ -14769,27 +14765,10 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A220:A223"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="A209:A212"/>
-    <mergeCell ref="A213:A215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A218:A219"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A51:A56"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A75:A84"/>
-    <mergeCell ref="A85:A93"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="A99:A105"/>
-    <mergeCell ref="A109:A119"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A120:A127"/>
     <mergeCell ref="A129:A132"/>
     <mergeCell ref="A137:A145"/>
@@ -14806,10 +14785,27 @@
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A51:A56"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A220:A223"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="A209:A212"/>
+    <mergeCell ref="A213:A215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A218:A219"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A75:A84"/>
+    <mergeCell ref="A85:A93"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A99:A105"/>
+    <mergeCell ref="A109:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added notes from mission 2 - testing
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/projects/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526D1B34-DDBB-7144-9ADD-A9E91A63FC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF6AE2-DAB0-4A4E-A473-296059955BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="50160" windowHeight="26220" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="651">
   <si>
     <t>Mission Number</t>
   </si>
@@ -2008,6 +2008,13 @@
   </si>
   <si>
     <t>Mission 1(Cleaned on 02/24/22): Adjusted the end time from 2021-10-04T15:30:00 to 2021-10-04T15:17:00 since the microSWIFTs started being picked up at this point</t>
+  </si>
+  <si>
+    <t>Mission 2(Cleaned on 02/24/22): Adjusted start time from 2021-10-05T14:30:00 to 2021-10-05T14:41:00 since the microSWIFTs were still on surfboards until this point.
+				Adjusted end time from 2021-10-05T16:00:00 to 2021-10-05T14:50:00 since all of the microSWIFTs have reached the beach at this point. 
+				Masked microSWIFT 4 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.
+				Masked microSWIFT 5 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.
+				Masked microSWIFT 3 from the start to index 200 since it was still on a surfboard as seen by smaller signals then a large spike in acceleration as it is thrown in.</t>
   </si>
 </sst>
 </file>
@@ -3317,7 +3324,7 @@
   <dimension ref="A1:V83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3606,7 +3613,9 @@
       <c r="S4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="T4" s="9"/>
+      <c r="T4" s="9" t="s">
+        <v>650</v>
+      </c>
       <c r="U4" s="1" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
final dataset complete and fully checked
</commit_message>
<xml_diff>
--- a/DUNEXMainExp_notes.xlsx
+++ b/DUNEXMainExp_notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edwinrainville/projects/DUNEXMainExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejrainville/Documents/DUNEXMainExp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490B1371-0275-1E43-AF3A-0E945D3E11BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64AB40F-16A5-194C-8BBB-F3872EF20A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="50160" windowHeight="26220" xr2:uid="{EB3AE160-BCBD-8143-A8BA-8E84C45D4E8F}"/>
   </bookViews>
@@ -1111,12 +1111,6 @@
     <t>2021-10-13T13:30:00</t>
   </si>
   <si>
-    <t>2021-10-13T14:18:00</t>
-  </si>
-  <si>
-    <t>2021-10-13T14:53:00</t>
-  </si>
-  <si>
     <t>Mask microSWIFT 42 from index 15000 to the end since it made it to the beach but then rolled back down briefly.</t>
   </si>
   <si>
@@ -2175,13 +2169,6 @@
   <si>
     <t>Mission 29(Cleaned on 01/28/22): Adjusted start time from 2021-10-13T13:00:00 to 2021-10-13T13:10:00 since all of the microSWIFTs were still on the jetski at this point which can be seen by the location and non-wave like IMU signals.
                                  Adjusted end time from 2021-10-13T13:35:00 to 2021-10-13T13:30:00 since all of the microSWIFTs made it to the beach by this point as seen by the signals being cut off by the spatial mask.</t>
-  </si>
-  <si>
-    <t>Mission 30(Cleaned on 01/28/22): Adjusted start time from 2021-10-13T14:04:00 to 2021-10-13T14:18:00 since all of the microSWIFTs were still on the jetski at this point which can be seen by the movement towards the north side from the pier and non-wave-like signals in the IMU.
-                                 Adjusted end time from 2021-10-13T15:15:00 to 2021-10-13T14:53:00 since all of the microSWIFTs made it to the beach in this time as seen by the signals being cut off by the spatial mask.
-                                 Removed microSWIFT 13 since it has bad gyroscope measurements(no fluctuations)
-                                 Note that microSWIFT 3 has a bad magnetometer(no fluctuations in measurements)
-                                 Mask microSWIFT 42 from index 15000 to the end since it made it to the beach but then rolled back down briefly.</t>
   </si>
   <si>
     <t>Mission 31(Cleaned on 01/28/22): Adjusted start time from 2021-10-13T16:15:00 to 2021-10-13T16:22:00since most of the microSWIFTs are still on the jetski as seen by the irregular/ choppy GPS locations and non-wave like IMU signals.
@@ -2528,14 +2515,6 @@
                                  Removed microSWIFT 66 since it doesn't have enough data and leads to spiky results. </t>
   </si>
   <si>
-    <t>Mission 68(Cleaned on 02/28/22): Adjusted the start time from 2021-10-28T15:30:00 to 2021-10-28T15:34:00 since most of the microSWIFTs were not in the water until this point
-                                 Adjusted the end time from 2021-10-28T16:20:00 to 2021-10-28T15:50:00 so that we do not have to have the 10-minute data gap and many of the microSWIFTs had already made it to the beach at this point
-                                 Removed microSWIFT 58 since it had a bad gyroscope
-                                 Masked microSWIFT 23 from index 10000 to the end since it was no longer recording as seen by completely flat signals
-                                 Masked microSWIFT 57 from index 2000 to the end since it was no longer recording as seen by completely flat signals
-                                 Masked microSWIFT 29 from index 4500 to the end since it was no longer recording as seen by completely flat signals</t>
-  </si>
-  <si>
     <t>Mission 69(Cleaned on 01/28/22): Adjusted the start time from 2021-10-28T17:05:00 to 2021-10-28T17:07:00 since that is when most of the microSWIFTs actually enter the water as seen by flat IMU signals.
                                  Adjusted end time from 2021-10-28T17:30:00 to 2021-10-28T17:20:00 since all microSWIFTs have reached the beach by this point.
                                  Note that microSWIFT 58 has bad gyroscope data - may need to be removed
@@ -2691,6 +2670,28 @@
   </si>
   <si>
     <t xml:space="preserve">offshore buoys picked up by paddlers then thehy paddled north and headed into the beach - many of the other micros were caught in a convergence zone in the surfzone </t>
+  </si>
+  <si>
+    <t>2021-10-13T14:38:00</t>
+  </si>
+  <si>
+    <t>Mission 30(Cleaned on 01/28/22): Adjusted start time from 2021-10-13T14:04:00 to 2021-10-13T14:20:00 and end time from 2021-10-13T14:53:00 to 2021-10-13T14:38:00 since all of the microSWIFTs were still on the jetski at this point which can be seen by the movement towards the north side from the pier and non-wave-like signals in the IMU.
+                                 Adjusted end time from 2021-10-13T15:15:00 to 2021-10-13T14:53:00 since all of the microSWIFTs made it to the beach in this time as seen by the signals being cut off by the spatial mask.
+                                 Removed microSWIFT 13 since it has bad gyroscope measurements(no fluctuations)
+                                 Note that microSWIFT 3 has a bad magnetometer(no fluctuations in measurements)
+                                 Mask microSWIFT 42 from index 15000 to the end since it made it to the beach but then rolled back down briefly.</t>
+  </si>
+  <si>
+    <t>2021-10-13T14:20:00</t>
+  </si>
+  <si>
+    <t>Mission 68(Cleaned on 02/28/22): Adjusted the start time from 2021-10-28T15:30:00 to 2021-10-28T15:34:00 since most of the microSWIFTs were not in the water until this point
+                                 Adjusted the end time from 2021-10-28T16:20:00 to 2021-10-28T15:50:00 so that we do not have to have the 10-minute data gap and many of the microSWIFTs had already made it to the beach at this point
+                                 Removed microSWIFT 58 since it had a bad gyroscope
+                                 Masked microSWIFT 23 from index 10000 to the end since it was no longer recording as seen by completely flat signals
+                                 Masked microSWIFT 57 from index 2000 to the end since it was no longer recording as seen by completely flat signals
+                                 Masked microSWIFT 29 from index 4500 to the end since it was no longer recording as seen by completely flat signals
+                                 Removed microSWIFTs 30, 62, 10, 73, and 60 since they all had two little data leading to spuriously large values</t>
   </si>
 </sst>
 </file>
@@ -3701,7 +3702,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3989,7 +3990,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3999,8 +4000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC5743F-24DA-014A-A99E-B60CA7AB8951}">
   <dimension ref="A1:V83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M81" workbookViewId="0">
-      <selection activeCell="S82" sqref="S82"/>
+    <sheetView tabSelected="1" topLeftCell="M67" workbookViewId="0">
+      <selection activeCell="T71" sqref="T71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4088,7 +4089,7 @@
         <v>6</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="U1" s="3" t="s">
         <v>18</v>
@@ -4156,7 +4157,7 @@
         <v>20</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="U2" s="2" t="s">
         <v>8</v>
@@ -4215,16 +4216,16 @@
         <v>38</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>8</v>
@@ -4283,16 +4284,16 @@
         <v>38</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>8</v>
@@ -4351,16 +4352,16 @@
         <v>38</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>46</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>8</v>
@@ -4419,16 +4420,16 @@
         <v>38</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="U6" s="1" t="s">
         <v>8</v>
@@ -4487,7 +4488,7 @@
         <v>38</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>54</v>
@@ -4496,7 +4497,7 @@
         <v>48</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>8</v>
@@ -4564,7 +4565,7 @@
         <v>53</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>8</v>
@@ -4623,16 +4624,16 @@
         <v>38</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>8</v>
@@ -4691,16 +4692,16 @@
         <v>66</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>8</v>
@@ -4762,13 +4763,13 @@
         <v>68</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>8</v>
@@ -4836,7 +4837,7 @@
         <v>78</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="U12" s="1" t="s">
         <v>8</v>
@@ -4904,7 +4905,7 @@
         <v>78</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="U13" s="1" t="s">
         <v>8</v>
@@ -4972,7 +4973,7 @@
         <v>78</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="U14" s="1" t="s">
         <v>8</v>
@@ -5040,7 +5041,7 @@
         <v>75</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="U15" s="1" t="s">
         <v>8</v>
@@ -5108,7 +5109,7 @@
         <v>78</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>8</v>
@@ -5176,7 +5177,7 @@
         <v>85</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="U17" s="1" t="s">
         <v>8</v>
@@ -5244,7 +5245,7 @@
         <v>78</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="U18" s="1" t="s">
         <v>8</v>
@@ -5312,7 +5313,7 @@
         <v>78</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="U19" s="1" t="s">
         <v>8</v>
@@ -5380,7 +5381,7 @@
         <v>78</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="U20" s="1" t="s">
         <v>8</v>
@@ -5448,7 +5449,7 @@
         <v>78</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="U21" s="1" t="s">
         <v>8</v>
@@ -5516,7 +5517,7 @@
         <v>78</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="U22" s="1" t="s">
         <v>8</v>
@@ -5584,7 +5585,7 @@
         <v>94</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>8</v>
@@ -5652,7 +5653,7 @@
         <v>78</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>8</v>
@@ -5720,7 +5721,7 @@
         <v>78</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>8</v>
@@ -5788,7 +5789,7 @@
         <v>78</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>8</v>
@@ -5856,7 +5857,7 @@
         <v>103</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="U27" s="1" t="s">
         <v>8</v>
@@ -5924,7 +5925,7 @@
         <v>104</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="U28" s="1" t="s">
         <v>8</v>
@@ -5992,7 +5993,7 @@
         <v>104</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="U29" s="1" t="s">
         <v>8</v>
@@ -6060,7 +6061,7 @@
         <v>78</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="U30" s="1" t="s">
         <v>8</v>
@@ -6128,7 +6129,7 @@
         <v>78</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="U31" s="1" t="s">
         <v>8</v>
@@ -6187,16 +6188,16 @@
         <v>111</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>356</v>
+        <v>729</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>357</v>
+        <v>727</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>674</v>
+        <v>728</v>
       </c>
       <c r="U32" s="1" t="s">
         <v>8</v>
@@ -6255,16 +6256,16 @@
         <v>113</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="U33" s="1" t="s">
         <v>8</v>
@@ -6326,13 +6327,13 @@
         <v>116</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>136</v>
       </c>
       <c r="T34" s="4" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="U34" s="1" t="s">
         <v>8</v>
@@ -6391,16 +6392,16 @@
         <v>131</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="R35" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T35" s="4" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="U35" s="1" t="s">
         <v>8</v>
@@ -6459,7 +6460,7 @@
         <v>133</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="R36" s="1" t="s">
         <v>119</v>
@@ -6468,7 +6469,7 @@
         <v>78</v>
       </c>
       <c r="T36" s="4" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="U36" s="1" t="s">
         <v>8</v>
@@ -6527,16 +6528,16 @@
         <v>132</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T37" s="4" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="U37" s="1" t="s">
         <v>8</v>
@@ -6595,16 +6596,16 @@
         <v>132</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="S38" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T38" s="4" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="U38" s="1" t="s">
         <v>8</v>
@@ -6613,7 +6614,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -6663,16 +6664,16 @@
         <v>134</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="R39" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T39" s="4" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="U39" s="1" t="s">
         <v>8</v>
@@ -6681,7 +6682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -6734,13 +6735,13 @@
         <v>123</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T40" s="4" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="U40" s="1" t="s">
         <v>8</v>
@@ -6799,16 +6800,16 @@
         <v>138</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="R41" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>142</v>
       </c>
       <c r="T41" s="4" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="U41" s="1" t="s">
         <v>8</v>
@@ -6867,16 +6868,16 @@
         <v>138</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>141</v>
       </c>
       <c r="T42" s="4" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="U42" s="1" t="s">
         <v>8</v>
@@ -6935,16 +6936,16 @@
         <v>185</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="R43" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T43" s="4" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="U43" s="1" t="s">
         <v>8</v>
@@ -6953,7 +6954,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -7003,16 +7004,16 @@
         <v>186</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="R44" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>189</v>
       </c>
       <c r="T44" s="4" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="U44" s="1" t="s">
         <v>8</v>
@@ -7080,7 +7081,7 @@
         <v>190</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="U45" s="1" t="s">
         <v>8</v>
@@ -7139,16 +7140,16 @@
         <v>195</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="S46" s="4" t="s">
         <v>196</v>
       </c>
       <c r="T46" s="4" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="U46" s="1" t="s">
         <v>8</v>
@@ -7207,16 +7208,16 @@
         <v>198</v>
       </c>
       <c r="Q47" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="R47" s="1" t="s">
         <v>507</v>
-      </c>
-      <c r="R47" s="1" t="s">
-        <v>509</v>
       </c>
       <c r="S47" s="4" t="s">
         <v>199</v>
       </c>
       <c r="T47" s="4" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="U47" s="1" t="s">
         <v>8</v>
@@ -7275,7 +7276,7 @@
         <v>201</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="R48" s="1" t="s">
         <v>151</v>
@@ -7284,7 +7285,7 @@
         <v>78</v>
       </c>
       <c r="T48" s="4" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="U48" s="1" t="s">
         <v>8</v>
@@ -7352,7 +7353,7 @@
         <v>78</v>
       </c>
       <c r="T49" s="4" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="U49" s="1" t="s">
         <v>8</v>
@@ -7420,7 +7421,7 @@
         <v>78</v>
       </c>
       <c r="T50" s="4" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="U50" s="1" t="s">
         <v>8</v>
@@ -7488,7 +7489,7 @@
         <v>78</v>
       </c>
       <c r="T51" s="4" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="U51" s="1" t="s">
         <v>8</v>
@@ -7556,7 +7557,7 @@
         <v>78</v>
       </c>
       <c r="T52" s="4" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
       <c r="U52" s="1" t="s">
         <v>8</v>
@@ -7565,7 +7566,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -7615,7 +7616,7 @@
         <v>207</v>
       </c>
       <c r="Q53" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="R53" s="1" t="s">
         <v>182</v>
@@ -7624,7 +7625,7 @@
         <v>208</v>
       </c>
       <c r="T53" s="4" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
       <c r="U53" s="1" t="s">
         <v>8</v>
@@ -7692,7 +7693,7 @@
         <v>208</v>
       </c>
       <c r="T54" s="4" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="U54" s="1" t="s">
         <v>8</v>
@@ -7760,7 +7761,7 @@
         <v>212</v>
       </c>
       <c r="T55" s="4" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="U55" s="1" t="s">
         <v>8</v>
@@ -7828,7 +7829,7 @@
         <v>224</v>
       </c>
       <c r="T56" s="4" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="U56" s="1" t="s">
         <v>8</v>
@@ -7896,7 +7897,7 @@
         <v>225</v>
       </c>
       <c r="T57" s="4" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="U57" s="1" t="s">
         <v>8</v>
@@ -7955,16 +7956,16 @@
         <v>218</v>
       </c>
       <c r="Q58" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="R58" s="11" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="S58" s="4" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="T58" s="4" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="U58" s="1" t="s">
         <v>8</v>
@@ -8032,7 +8033,7 @@
         <v>234</v>
       </c>
       <c r="T59" s="4" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="U59" s="1" t="s">
         <v>8</v>
@@ -8091,16 +8092,16 @@
         <v>231</v>
       </c>
       <c r="Q60" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="S60" s="4" t="s">
         <v>236</v>
       </c>
       <c r="T60" s="4" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
       <c r="U60" s="1" t="s">
         <v>8</v>
@@ -8162,13 +8163,13 @@
         <v>233</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="S61" s="4" t="s">
         <v>235</v>
       </c>
       <c r="T61" s="4" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
       <c r="U61" s="1" t="s">
         <v>8</v>
@@ -8227,7 +8228,7 @@
         <v>231</v>
       </c>
       <c r="Q62" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="R62" s="1" t="s">
         <v>241</v>
@@ -8236,7 +8237,7 @@
         <v>78</v>
       </c>
       <c r="T62" s="4" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="U62" s="1" t="s">
         <v>8</v>
@@ -8295,16 +8296,16 @@
         <v>261</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="S63" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T63" s="4" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="U63" s="1" t="s">
         <v>8</v>
@@ -8313,7 +8314,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -8366,13 +8367,13 @@
         <v>244</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="S64" s="4" t="s">
         <v>269</v>
       </c>
       <c r="T64" s="4" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="U64" s="1" t="s">
         <v>8</v>
@@ -8440,7 +8441,7 @@
         <v>270</v>
       </c>
       <c r="T65" s="4" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="U65" s="1" t="s">
         <v>8</v>
@@ -8508,7 +8509,7 @@
         <v>271</v>
       </c>
       <c r="T66" s="4" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="U66" s="1" t="s">
         <v>8</v>
@@ -8567,7 +8568,7 @@
         <v>268</v>
       </c>
       <c r="Q67" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="R67" s="1" t="s">
         <v>257</v>
@@ -8576,7 +8577,7 @@
         <v>78</v>
       </c>
       <c r="T67" s="4" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="U67" s="1" t="s">
         <v>8</v>
@@ -8644,7 +8645,7 @@
         <v>78</v>
       </c>
       <c r="T68" s="4" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="U68" s="1" t="s">
         <v>8</v>
@@ -8703,16 +8704,16 @@
         <v>267</v>
       </c>
       <c r="Q69" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="S69" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T69" s="4" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="U69" s="1" t="s">
         <v>8</v>
@@ -8721,7 +8722,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="187" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" ht="221" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -8771,16 +8772,16 @@
         <v>267</v>
       </c>
       <c r="Q70" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="R70" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="S70" s="4" t="s">
         <v>272</v>
       </c>
       <c r="T70" s="4" t="s">
-        <v>712</v>
+        <v>730</v>
       </c>
       <c r="U70" s="1" t="s">
         <v>8</v>
@@ -8839,16 +8840,16 @@
         <v>268</v>
       </c>
       <c r="Q71" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="R71" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="S71" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T71" s="4" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="U71" s="1" t="s">
         <v>8</v>
@@ -8907,16 +8908,16 @@
         <v>268</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="S72" s="4" t="s">
         <v>78</v>
       </c>
       <c r="T72" s="4" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="U72" s="1" t="s">
         <v>8</v>
@@ -8975,16 +8976,16 @@
         <v>268</v>
       </c>
       <c r="Q73" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="R73" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="S73" s="4" t="s">
         <v>273</v>
       </c>
       <c r="T73" s="4" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="U73" s="1" t="s">
         <v>8</v>
@@ -9052,7 +9053,7 @@
         <v>274</v>
       </c>
       <c r="T74" s="4" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="U74" s="1" t="s">
         <v>8</v>
@@ -9111,16 +9112,16 @@
         <v>268</v>
       </c>
       <c r="Q75" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S75" s="4" t="s">
         <v>275</v>
       </c>
       <c r="T75" s="4" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="U75" s="1" t="s">
         <v>8</v>
@@ -9179,16 +9180,16 @@
         <v>280</v>
       </c>
       <c r="Q76" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="R76" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="S76" s="4" t="s">
         <v>281</v>
       </c>
       <c r="T76" s="4" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="U76" s="1" t="s">
         <v>8</v>
@@ -9247,16 +9248,16 @@
         <v>282</v>
       </c>
       <c r="Q77" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="R77" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="S77" s="4" t="s">
         <v>281</v>
       </c>
       <c r="T77" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="U77" s="1" t="s">
         <v>8</v>
@@ -9315,16 +9316,16 @@
         <v>282</v>
       </c>
       <c r="Q78" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="R78" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="S78" s="4" t="s">
         <v>283</v>
       </c>
       <c r="T78" s="4" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="U78" s="1" t="s">
         <v>8</v>
@@ -9383,16 +9384,16 @@
         <v>268</v>
       </c>
       <c r="Q79" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="S79" s="4" t="s">
         <v>283</v>
       </c>
       <c r="T79" s="4" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="U79" s="1" t="s">
         <v>8</v>
@@ -9451,16 +9452,16 @@
         <v>268</v>
       </c>
       <c r="Q80" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="S80" s="4" t="s">
         <v>283</v>
       </c>
       <c r="T80" s="4" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="U80" s="1" t="s">
         <v>8</v>
@@ -9519,16 +9520,16 @@
         <v>268</v>
       </c>
       <c r="Q81" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="R81" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="S81" s="4" t="s">
         <v>283</v>
       </c>
       <c r="T81" s="4" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="U81" s="1" t="s">
         <v>8</v>
@@ -9587,16 +9588,16 @@
         <v>268</v>
       </c>
       <c r="Q82" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="R82" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="S82" s="4" t="s">
         <v>283</v>
       </c>
       <c r="T82" s="4" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="U82" s="1" t="s">
         <v>8</v>
@@ -9658,13 +9659,13 @@
         <v>286</v>
       </c>
       <c r="R83" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="S83" s="4" t="s">
         <v>285</v>
       </c>
       <c r="T83" s="4" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="U83" s="1" t="s">
         <v>8</v>
@@ -11978,13 +11979,13 @@
         <v>0</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="39"/>
       <c r="B4" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C4" s="10">
         <v>200</v>
@@ -12018,7 +12019,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C6" s="10">
         <v>0</v>
@@ -12030,7 +12031,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12048,13 +12049,13 @@
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="39"/>
       <c r="B8" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -12066,13 +12067,13 @@
         <v>0</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
       <c r="B9" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
@@ -12084,7 +12085,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12092,7 +12093,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C10" s="10">
         <v>0</v>
@@ -12104,7 +12105,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12122,7 +12123,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12140,7 +12141,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12160,13 +12161,13 @@
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="39"/>
       <c r="B14" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C14" s="10">
         <v>1000</v>
@@ -12178,7 +12179,7 @@
         <v>0</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12196,13 +12197,13 @@
         <v>0</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="39"/>
       <c r="B16" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C16" s="10">
         <v>500</v>
@@ -12214,13 +12215,13 @@
         <v>0</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="39"/>
       <c r="B17" s="10" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C17" s="10">
         <v>1500</v>
@@ -12232,7 +12233,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -12250,7 +12251,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C19" s="10">
         <v>0</v>
@@ -12262,13 +12263,13 @@
         <v>0</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="39"/>
       <c r="B20" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C20" s="10">
         <v>0</v>
@@ -12280,7 +12281,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12298,13 +12299,13 @@
         <v>0</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="39"/>
       <c r="B22" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C22" s="10">
         <v>0</v>
@@ -12422,7 +12423,7 @@
         <v>15</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C30" s="10">
         <v>0</v>
@@ -12434,7 +12435,7 @@
         <v>0</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12442,7 +12443,7 @@
         <v>16</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C31" s="10">
         <v>0</v>
@@ -12454,7 +12455,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="23" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -12482,7 +12483,7 @@
         <v>18</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C33" s="10">
         <v>1000</v>
@@ -12494,7 +12495,7 @@
         <v>0</v>
       </c>
       <c r="F33" s="23" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12520,7 +12521,7 @@
         <v>19</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C35" s="10">
         <v>1000</v>
@@ -12532,13 +12533,13 @@
         <v>0</v>
       </c>
       <c r="F35" s="23" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="39"/>
       <c r="B36" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C36" s="10">
         <v>0</v>
@@ -12550,7 +12551,7 @@
         <v>0</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -12666,7 +12667,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12674,7 +12675,7 @@
         <v>24</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C43" s="10">
         <v>0</v>
@@ -12686,13 +12687,13 @@
         <v>0</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="39"/>
       <c r="B44" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C44" s="10">
         <v>1000</v>
@@ -12704,7 +12705,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12744,7 +12745,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12762,13 +12763,13 @@
         <v>0</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="39"/>
       <c r="B48" s="10" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="C48" s="10">
         <v>500</v>
@@ -12780,13 +12781,13 @@
         <v>0</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="39"/>
       <c r="B49" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C49" s="10">
         <v>500</v>
@@ -12798,13 +12799,13 @@
         <v>0</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="39"/>
       <c r="B50" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C50" s="10">
         <v>500</v>
@@ -12816,7 +12817,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -12946,7 +12947,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="23" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -12984,7 +12985,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13004,13 +13005,13 @@
         <v>0</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="39"/>
       <c r="B62" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C62" s="10">
         <v>1000</v>
@@ -13022,7 +13023,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13040,7 +13041,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="23" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13058,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="23" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13066,7 +13067,7 @@
         <v>32</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C65" s="10">
         <v>500</v>
@@ -13078,7 +13079,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13098,13 +13099,13 @@
         <v>0</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="39"/>
       <c r="B67" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C67" s="10">
         <v>0</v>
@@ -13116,7 +13117,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="23" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
@@ -13134,7 +13135,7 @@
         <v>35</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C69" s="10">
         <v>0</v>
@@ -13143,16 +13144,16 @@
         <v>-1</v>
       </c>
       <c r="E69" s="10" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="39"/>
       <c r="B70" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C70" s="10">
         <v>5500</v>
@@ -13161,10 +13162,10 @@
         <v>14000</v>
       </c>
       <c r="E70" s="10" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13184,13 +13185,13 @@
         <v>0</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="39"/>
       <c r="B72" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C72" s="10">
         <v>0</v>
@@ -13202,7 +13203,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13220,7 +13221,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="23" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13238,7 +13239,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13258,7 +13259,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="23" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13276,13 +13277,13 @@
         <v>0</v>
       </c>
       <c r="F76" s="23" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="39"/>
       <c r="B77" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C77" s="10">
         <v>1000</v>
@@ -13294,13 +13295,13 @@
         <v>0</v>
       </c>
       <c r="F77" s="23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="39"/>
       <c r="B78" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C78" s="10">
         <v>1200</v>
@@ -13312,7 +13313,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="23" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13330,7 +13331,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="23" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13348,7 +13349,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="23" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13366,13 +13367,13 @@
         <v>0</v>
       </c>
       <c r="F81" s="23" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="39"/>
       <c r="B82" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C82" s="10">
         <v>500</v>
@@ -13384,13 +13385,13 @@
         <v>0</v>
       </c>
       <c r="F82" s="23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="39"/>
       <c r="B83" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C83" s="10">
         <v>600</v>
@@ -13402,13 +13403,13 @@
         <v>0</v>
       </c>
       <c r="F83" s="23" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="39"/>
       <c r="B84" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C84" s="10">
         <v>1200</v>
@@ -13420,7 +13421,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="23" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13440,7 +13441,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -13458,13 +13459,13 @@
         <v>0</v>
       </c>
       <c r="F86" s="23" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="39"/>
       <c r="B87" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C87" s="10">
         <v>0</v>
@@ -13476,7 +13477,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="23" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13494,7 +13495,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="23" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13512,7 +13513,7 @@
         <v>0</v>
       </c>
       <c r="F89" s="23" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13530,7 +13531,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="23" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13548,13 +13549,13 @@
         <v>0</v>
       </c>
       <c r="F91" s="23" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="39"/>
       <c r="B92" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C92" s="10">
         <v>1000</v>
@@ -13566,13 +13567,13 @@
         <v>0</v>
       </c>
       <c r="F92" s="23" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="39"/>
       <c r="B93" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C93" s="10">
         <v>1000</v>
@@ -13584,7 +13585,7 @@
         <v>0</v>
       </c>
       <c r="F93" s="23" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13592,7 +13593,7 @@
         <v>39</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C94" s="10">
         <v>0</v>
@@ -13604,13 +13605,13 @@
         <v>0</v>
       </c>
       <c r="F94" s="23" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="39"/>
       <c r="B95" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C95" s="10">
         <v>0</v>
@@ -13619,10 +13620,10 @@
         <v>-1</v>
       </c>
       <c r="E95" s="10" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F95" s="23" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13637,10 +13638,10 @@
         <v>-1</v>
       </c>
       <c r="E96" s="10" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F96" s="23" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13655,10 +13656,10 @@
         <v>-1</v>
       </c>
       <c r="E97" s="10" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F97" s="23" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13676,7 +13677,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="23" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13684,7 +13685,7 @@
         <v>40</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C99" s="10">
         <v>0</v>
@@ -13696,13 +13697,13 @@
         <v>0</v>
       </c>
       <c r="F99" s="23" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="39"/>
       <c r="B100" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C100" s="10">
         <v>0</v>
@@ -13714,7 +13715,7 @@
         <v>0</v>
       </c>
       <c r="F100" s="23" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13732,13 +13733,13 @@
         <v>0</v>
       </c>
       <c r="F101" s="23" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="39"/>
       <c r="B102" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C102" s="10">
         <v>0</v>
@@ -13750,13 +13751,13 @@
         <v>0</v>
       </c>
       <c r="F102" s="23" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="103" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="39"/>
       <c r="B103" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C103" s="10">
         <v>1000</v>
@@ -13768,7 +13769,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="23" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="104" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13786,7 +13787,7 @@
         <v>0</v>
       </c>
       <c r="F104" s="23" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13804,7 +13805,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13824,7 +13825,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="23" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13842,7 +13843,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="108" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13860,7 +13861,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="23" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13868,7 +13869,7 @@
         <v>42</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C109" s="10">
         <v>5000</v>
@@ -13880,7 +13881,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="23" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13898,13 +13899,13 @@
         <v>0</v>
       </c>
       <c r="F110" s="23" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="111" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="39"/>
       <c r="B111" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C111" s="10">
         <v>5000</v>
@@ -13916,13 +13917,13 @@
         <v>0</v>
       </c>
       <c r="F111" s="23" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="39"/>
       <c r="B112" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C112" s="10">
         <v>5000</v>
@@ -13934,7 +13935,7 @@
         <v>0</v>
       </c>
       <c r="F112" s="23" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -13952,13 +13953,13 @@
         <v>0</v>
       </c>
       <c r="F113" s="23" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="114" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="39"/>
       <c r="B114" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C114" s="10">
         <v>5000</v>
@@ -13970,13 +13971,13 @@
         <v>0</v>
       </c>
       <c r="F114" s="23" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="115" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="39"/>
       <c r="B115" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C115" s="10">
         <v>5000</v>
@@ -13988,7 +13989,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="23" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14006,13 +14007,13 @@
         <v>0</v>
       </c>
       <c r="F116" s="23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="39"/>
       <c r="B117" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C117" s="10">
         <v>5000</v>
@@ -14024,13 +14025,13 @@
         <v>0</v>
       </c>
       <c r="F117" s="23" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="118" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="39"/>
       <c r="B118" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C118" s="10">
         <v>5000</v>
@@ -14042,7 +14043,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="23" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14060,7 +14061,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="23" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="120" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14068,7 +14069,7 @@
         <v>43</v>
       </c>
       <c r="B120" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C120" s="10">
         <v>28000</v>
@@ -14080,13 +14081,13 @@
         <v>0</v>
       </c>
       <c r="F120" s="23" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="121" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="39"/>
       <c r="B121" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C121" s="10">
         <v>3000</v>
@@ -14098,7 +14099,7 @@
         <v>0</v>
       </c>
       <c r="F121" s="23" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="122" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14116,7 +14117,7 @@
         <v>0</v>
       </c>
       <c r="F122" s="23" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14134,13 +14135,13 @@
         <v>0</v>
       </c>
       <c r="F123" s="23" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="39"/>
       <c r="B124" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C124" s="10">
         <v>1000</v>
@@ -14152,13 +14153,13 @@
         <v>0</v>
       </c>
       <c r="F124" s="23" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="125" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="39"/>
       <c r="B125" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C125" s="10">
         <v>0</v>
@@ -14170,13 +14171,13 @@
         <v>0</v>
       </c>
       <c r="F125" s="23" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="126" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="39"/>
       <c r="B126" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C126" s="10">
         <v>1000</v>
@@ -14188,7 +14189,7 @@
         <v>0</v>
       </c>
       <c r="F126" s="23" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="127" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14206,7 +14207,7 @@
         <v>0</v>
       </c>
       <c r="F127" s="23" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
@@ -14224,7 +14225,7 @@
         <v>45</v>
       </c>
       <c r="B129" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C129" s="10">
         <v>0</v>
@@ -14236,7 +14237,7 @@
         <v>0</v>
       </c>
       <c r="F129" s="23" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="130" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14254,13 +14255,13 @@
         <v>0</v>
       </c>
       <c r="F130" s="23" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="39"/>
       <c r="B131" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C131" s="10">
         <v>0</v>
@@ -14272,13 +14273,13 @@
         <v>0</v>
       </c>
       <c r="F131" s="23" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="39"/>
       <c r="B132" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C132" s="10">
         <v>1000</v>
@@ -14290,7 +14291,7 @@
         <v>0</v>
       </c>
       <c r="F132" s="23" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -14340,7 +14341,7 @@
         <v>0</v>
       </c>
       <c r="F136" s="23" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="137" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14348,7 +14349,7 @@
         <v>50</v>
       </c>
       <c r="B137" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C137" s="10">
         <v>7000</v>
@@ -14360,7 +14361,7 @@
         <v>0</v>
       </c>
       <c r="F137" s="23" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="138" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14378,7 +14379,7 @@
         <v>0</v>
       </c>
       <c r="F138" s="23" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="139" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14396,7 +14397,7 @@
         <v>0</v>
       </c>
       <c r="F139" s="30" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="140" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14414,13 +14415,13 @@
         <v>0</v>
       </c>
       <c r="F140" s="30" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="141" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="39"/>
       <c r="B141" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C141" s="29">
         <v>7000</v>
@@ -14432,13 +14433,13 @@
         <v>0</v>
       </c>
       <c r="F141" s="30" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="142" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="39"/>
       <c r="B142" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C142" s="29">
         <v>7000</v>
@@ -14450,13 +14451,13 @@
         <v>0</v>
       </c>
       <c r="F142" s="30" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="143" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="39"/>
       <c r="B143" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C143" s="29">
         <v>7000</v>
@@ -14468,13 +14469,13 @@
         <v>0</v>
       </c>
       <c r="F143" s="30" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="144" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="39"/>
       <c r="B144" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C144" s="29">
         <v>7000</v>
@@ -14486,7 +14487,7 @@
         <v>0</v>
       </c>
       <c r="F144" s="30" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="145" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14504,7 +14505,7 @@
         <v>0</v>
       </c>
       <c r="F145" s="23" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="146" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14512,7 +14513,7 @@
         <v>51</v>
       </c>
       <c r="B146" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C146" s="10">
         <v>156</v>
@@ -14521,10 +14522,10 @@
         <v>30504</v>
       </c>
       <c r="E146" s="10" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F146" s="23" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
@@ -14568,7 +14569,7 @@
         <v>54</v>
       </c>
       <c r="B150" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C150" s="10">
         <v>2000</v>
@@ -14580,13 +14581,13 @@
         <v>0</v>
       </c>
       <c r="F150" s="23" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="151" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A151" s="39"/>
       <c r="B151" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C151" s="10">
         <v>0</v>
@@ -14598,13 +14599,13 @@
         <v>0</v>
       </c>
       <c r="F151" s="23" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="152" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A152" s="39"/>
       <c r="B152" s="10" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C152" s="10">
         <v>0</v>
@@ -14616,13 +14617,13 @@
         <v>0</v>
       </c>
       <c r="F152" s="23" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="153" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A153" s="39"/>
       <c r="B153" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C153" s="10">
         <v>0</v>
@@ -14634,13 +14635,13 @@
         <v>0</v>
       </c>
       <c r="F153" s="23" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="154" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="39"/>
       <c r="B154" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C154" s="10">
         <v>0</v>
@@ -14652,13 +14653,13 @@
         <v>0</v>
       </c>
       <c r="F154" s="23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="155" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="39"/>
       <c r="B155" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C155" s="10">
         <v>0</v>
@@ -14670,13 +14671,13 @@
         <v>0</v>
       </c>
       <c r="F155" s="23" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="156" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A156" s="39"/>
       <c r="B156" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C156" s="10">
         <v>0</v>
@@ -14688,7 +14689,7 @@
         <v>0</v>
       </c>
       <c r="F156" s="23" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
@@ -14718,13 +14719,13 @@
         <v>0</v>
       </c>
       <c r="F158" s="23" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="159" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="39"/>
       <c r="B159" s="10" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C159" s="10">
         <v>0</v>
@@ -14736,13 +14737,13 @@
         <v>0</v>
       </c>
       <c r="F159" s="23" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="160" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="39"/>
       <c r="B160" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C160" s="10">
         <v>1000</v>
@@ -14754,13 +14755,13 @@
         <v>0</v>
       </c>
       <c r="F160" s="23" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="161" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="39"/>
       <c r="B161" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C161" s="10">
         <v>0</v>
@@ -14772,7 +14773,7 @@
         <v>0</v>
       </c>
       <c r="F161" s="23" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -14820,7 +14821,7 @@
         <v>61</v>
       </c>
       <c r="B166" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C166" s="10">
         <v>0</v>
@@ -14832,7 +14833,7 @@
         <v>0</v>
       </c>
       <c r="F166" s="23" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="167" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14840,7 +14841,7 @@
         <v>62</v>
       </c>
       <c r="B167" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C167" s="10">
         <v>0</v>
@@ -14852,7 +14853,7 @@
         <v>0</v>
       </c>
       <c r="F167" s="23" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="168" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14870,13 +14871,13 @@
         <v>0</v>
       </c>
       <c r="F168" s="23" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="169" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="39"/>
       <c r="B169" s="10" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C169" s="10">
         <v>300</v>
@@ -14888,13 +14889,13 @@
         <v>0</v>
       </c>
       <c r="F169" s="23" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="170" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="39"/>
       <c r="B170" s="10" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C170" s="10">
         <v>0</v>
@@ -14906,7 +14907,7 @@
         <v>0</v>
       </c>
       <c r="F170" s="23" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="171" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14924,13 +14925,13 @@
         <v>0</v>
       </c>
       <c r="F171" s="23" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="172" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="39"/>
       <c r="B172" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C172" s="10">
         <v>100</v>
@@ -14942,13 +14943,13 @@
         <v>0</v>
       </c>
       <c r="F172" s="23" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="173" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="39"/>
       <c r="B173" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C173" s="10">
         <v>500</v>
@@ -14960,13 +14961,13 @@
         <v>0</v>
       </c>
       <c r="F173" s="23" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="174" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="39"/>
       <c r="B174" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C174" s="10">
         <v>200</v>
@@ -14978,7 +14979,7 @@
         <v>0</v>
       </c>
       <c r="F174" s="23" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="175" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -14986,7 +14987,7 @@
         <v>63</v>
       </c>
       <c r="B175" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C175" s="10">
         <v>0</v>
@@ -14998,7 +14999,7 @@
         <v>0</v>
       </c>
       <c r="F175" s="23" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="176" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -15016,13 +15017,13 @@
         <v>0</v>
       </c>
       <c r="F176" s="23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="177" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="39"/>
       <c r="B177" s="10" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C177" s="10">
         <v>0</v>
@@ -15034,7 +15035,7 @@
         <v>0</v>
       </c>
       <c r="F177" s="23" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="178" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -15052,7 +15053,7 @@
         <v>0</v>
       </c>
       <c r="F178" s="23" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -15080,7 +15081,7 @@
         <v>66</v>
       </c>
       <c r="B181" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C181" s="10">
         <v>500</v>
@@ -15092,13 +15093,13 @@
         <v>0</v>
       </c>
       <c r="F181" s="10" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182" s="39"/>
       <c r="B182" s="10" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C182" s="10">
         <v>1100</v>
@@ -15110,13 +15111,13 @@
         <v>0</v>
       </c>
       <c r="F182" s="10" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183" s="39"/>
       <c r="B183" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C183" s="10">
         <v>500</v>
@@ -15128,13 +15129,13 @@
         <v>0</v>
       </c>
       <c r="F183" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184" s="39"/>
       <c r="B184" s="10" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C184" s="10">
         <v>1000</v>
@@ -15146,13 +15147,13 @@
         <v>0</v>
       </c>
       <c r="F184" s="10" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185" s="39"/>
       <c r="B185" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C185" s="10">
         <v>500</v>
@@ -15164,13 +15165,13 @@
         <v>0</v>
       </c>
       <c r="F185" s="10" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" s="39"/>
       <c r="B186" s="10" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C186" s="10">
         <v>1200</v>
@@ -15182,13 +15183,13 @@
         <v>0</v>
       </c>
       <c r="F186" s="10" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187" s="39"/>
       <c r="B187" s="10" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C187" s="10">
         <v>500</v>
@@ -15200,7 +15201,7 @@
         <v>0</v>
       </c>
       <c r="F187" s="10" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
@@ -15218,7 +15219,7 @@
         <v>0</v>
       </c>
       <c r="F188" s="10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.2">
@@ -15236,7 +15237,7 @@
         <v>0</v>
       </c>
       <c r="F189" s="10" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.2">
@@ -15244,7 +15245,7 @@
         <v>67</v>
       </c>
       <c r="B190" s="10" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C190" s="10">
         <v>0</v>
@@ -15256,13 +15257,13 @@
         <v>0</v>
       </c>
       <c r="F190" s="10" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191" s="39"/>
       <c r="B191" s="10" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C191" s="10">
         <v>0</v>
@@ -15274,13 +15275,13 @@
         <v>0</v>
       </c>
       <c r="F191" s="10" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192" s="39"/>
       <c r="B192" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C192" s="10">
         <v>1000</v>
@@ -15292,13 +15293,13 @@
         <v>0</v>
       </c>
       <c r="F192" s="10" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" s="39"/>
       <c r="B193" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C193" s="10">
         <v>0</v>
@@ -15310,13 +15311,13 @@
         <v>0</v>
       </c>
       <c r="F193" s="10" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194" s="39"/>
       <c r="B194" s="10" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C194" s="10">
         <v>0</v>
@@ -15328,7 +15329,7 @@
         <v>0</v>
       </c>
       <c r="F194" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -15336,7 +15337,7 @@
         <v>68</v>
       </c>
       <c r="B195" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C195" s="10">
         <v>0</v>
@@ -15348,7 +15349,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="10" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
@@ -15366,13 +15367,13 @@
         <v>0</v>
       </c>
       <c r="F196" s="10" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" s="39"/>
       <c r="B197" s="10" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C197" s="10">
         <v>0</v>
@@ -15384,7 +15385,7 @@
         <v>0</v>
       </c>
       <c r="F197" s="10" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
@@ -15392,7 +15393,7 @@
         <v>69</v>
       </c>
       <c r="B198" s="10" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C198" s="10">
         <v>1800</v>
@@ -15404,13 +15405,13 @@
         <v>0</v>
       </c>
       <c r="F198" s="10" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A199" s="39"/>
       <c r="B199" s="10" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C199" s="10">
         <v>0</v>
@@ -15422,7 +15423,7 @@
         <v>0</v>
       </c>
       <c r="F199" s="10" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -15440,7 +15441,7 @@
         <v>0</v>
       </c>
       <c r="F200" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.2">
@@ -15480,13 +15481,13 @@
         <v>0</v>
       </c>
       <c r="F203" s="25" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A204" s="39"/>
       <c r="B204" s="25" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C204" s="25">
         <v>0</v>
@@ -15498,7 +15499,7 @@
         <v>0</v>
       </c>
       <c r="F204" s="25" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.2">
@@ -15528,13 +15529,13 @@
         <v>0</v>
       </c>
       <c r="F206" s="25" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A207" s="39"/>
       <c r="B207" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C207" s="25">
         <v>0</v>
@@ -15546,7 +15547,7 @@
         <v>0</v>
       </c>
       <c r="F207" s="25" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
@@ -15564,7 +15565,7 @@
         <v>76</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C209" s="25">
         <v>2000</v>
@@ -15576,13 +15577,13 @@
         <v>0</v>
       </c>
       <c r="F209" s="25" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="39"/>
       <c r="B210" s="25" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C210" s="25">
         <v>0</v>
@@ -15594,13 +15595,13 @@
         <v>0</v>
       </c>
       <c r="F210" s="25" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="39"/>
       <c r="B211" s="25" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C211" s="25">
         <v>0</v>
@@ -15612,13 +15613,13 @@
         <v>0</v>
       </c>
       <c r="F211" s="25" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="39"/>
       <c r="B212" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C212" s="25">
         <v>0</v>
@@ -15630,7 +15631,7 @@
         <v>0</v>
       </c>
       <c r="F212" s="25" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
@@ -15638,7 +15639,7 @@
         <v>77</v>
       </c>
       <c r="B213" s="25" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C213" s="25">
         <v>0</v>
@@ -15650,13 +15651,13 @@
         <v>0</v>
       </c>
       <c r="F213" s="25" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="39"/>
       <c r="B214" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C214" s="25">
         <v>0</v>
@@ -15668,13 +15669,13 @@
         <v>0</v>
       </c>
       <c r="F214" s="25" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="39"/>
       <c r="B215" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C215" s="25">
         <v>0</v>
@@ -15686,7 +15687,7 @@
         <v>0</v>
       </c>
       <c r="F215" s="25" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -15706,13 +15707,13 @@
         <v>0</v>
       </c>
       <c r="F216" s="25" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="39"/>
       <c r="B217" s="25" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C217" s="25">
         <v>0</v>
@@ -15724,7 +15725,7 @@
         <v>0</v>
       </c>
       <c r="F217" s="25" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
@@ -15732,7 +15733,7 @@
         <v>79</v>
       </c>
       <c r="B218" s="25" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C218" s="25">
         <v>0</v>
@@ -15744,13 +15745,13 @@
         <v>0</v>
       </c>
       <c r="F218" s="25" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="39"/>
       <c r="B219" s="25" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C219" s="25">
         <v>0</v>
@@ -15762,7 +15763,7 @@
         <v>0</v>
       </c>
       <c r="F219" s="25" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
@@ -15782,13 +15783,13 @@
         <v>0</v>
       </c>
       <c r="F220" s="25" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="39"/>
       <c r="B221" s="25" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C221" s="25">
         <v>0</v>
@@ -15800,7 +15801,7 @@
         <v>0</v>
       </c>
       <c r="F221" s="25" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
@@ -15818,13 +15819,13 @@
         <v>0</v>
       </c>
       <c r="F222" s="25" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="39"/>
       <c r="B223" s="25" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C223" s="25">
         <v>0</v>
@@ -15836,7 +15837,7 @@
         <v>0</v>
       </c>
       <c r="F223" s="25" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -15858,11 +15859,20 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A120:A127"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A75:A84"/>
+    <mergeCell ref="A85:A93"/>
+    <mergeCell ref="A94:A98"/>
+    <mergeCell ref="A106:A108"/>
+    <mergeCell ref="A99:A105"/>
+    <mergeCell ref="A109:A119"/>
+    <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A220:A223"/>
+    <mergeCell ref="A206:A207"/>
+    <mergeCell ref="A209:A212"/>
+    <mergeCell ref="A213:A215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A218:A219"/>
     <mergeCell ref="A129:A132"/>
     <mergeCell ref="A137:A145"/>
     <mergeCell ref="A195:A197"/>
@@ -15879,26 +15889,17 @@
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A120:A127"/>
     <mergeCell ref="A51:A56"/>
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A220:A223"/>
-    <mergeCell ref="A206:A207"/>
-    <mergeCell ref="A209:A212"/>
-    <mergeCell ref="A213:A215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A218:A219"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A75:A84"/>
-    <mergeCell ref="A85:A93"/>
-    <mergeCell ref="A94:A98"/>
-    <mergeCell ref="A106:A108"/>
-    <mergeCell ref="A99:A105"/>
-    <mergeCell ref="A109:A119"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>